<commit_message>
Termina de revisar los muros eje x
</commit_message>
<xml_diff>
--- a/Tarea 07/muros-fundaciones.xlsx
+++ b/Tarea 07/muros-fundaciones.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{B450D873-2D97-45D9-B113-59398A0D397A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{5AD96F4A-A710-4949-96FA-EEE9CBEA2794}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MUROS" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
   <si>
     <t>Ejes</t>
   </si>
@@ -68,6 +68,63 @@
   </si>
   <si>
     <t>EJE X</t>
+  </si>
+  <si>
+    <t>Espesor (m)</t>
+  </si>
+  <si>
+    <t>12 entre A y C</t>
+  </si>
+  <si>
+    <t>12 entre C y E</t>
+  </si>
+  <si>
+    <t>10 entre G y L</t>
+  </si>
+  <si>
+    <t>10 entre N y O</t>
+  </si>
+  <si>
+    <t>9 entre G y L</t>
+  </si>
+  <si>
+    <t>8 entre A y C</t>
+  </si>
+  <si>
+    <t>8 entre C y F</t>
+  </si>
+  <si>
+    <t>7 entre G y L</t>
+  </si>
+  <si>
+    <t>6 entre C y E</t>
+  </si>
+  <si>
+    <t>11' entre C y E</t>
+  </si>
+  <si>
+    <t>5 entre A y C</t>
+  </si>
+  <si>
+    <t>5 entre C y E</t>
+  </si>
+  <si>
+    <t>4 entre G y L</t>
+  </si>
+  <si>
+    <t>3 entre C y G</t>
+  </si>
+  <si>
+    <t>2' entre F y N</t>
+  </si>
+  <si>
+    <t>2 entre A y E</t>
+  </si>
+  <si>
+    <t>2 entre J y K</t>
+  </si>
+  <si>
+    <t>1 entre C y M</t>
   </si>
 </sst>
 </file>
@@ -122,7 +179,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -131,6 +188,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -413,87 +473,466 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:O3"/>
+  <dimension ref="B2:Q22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.5546875" style="1" customWidth="1"/>
-    <col min="2" max="3" width="8.88671875" style="1"/>
-    <col min="4" max="4" width="8.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="10.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="23.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="22.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="22" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7.77734375" style="1" customWidth="1"/>
-    <col min="14" max="14" width="7.33203125" style="1" customWidth="1"/>
-    <col min="15" max="15" width="8.88671875" style="1" customWidth="1"/>
-    <col min="16" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="2" width="3.5546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.88671875" style="1"/>
+    <col min="5" max="5" width="9.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="23.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="22.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="22" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.77734375" style="1" customWidth="1"/>
+    <col min="16" max="16" width="7.33203125" style="1" customWidth="1"/>
+    <col min="17" max="17" width="8.88671875" style="1" customWidth="1"/>
+    <col min="18" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B2" s="1" t="s">
+    <row r="2" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="C2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="O2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="N2" s="3"/>
-      <c r="O2" s="3"/>
-    </row>
-    <row r="3" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B3" s="2" t="s">
+      <c r="P2" s="3"/>
+      <c r="Q2" s="3"/>
+    </row>
+    <row r="3" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="C3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="I3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="J3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="K3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="L3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="M3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="L3" s="2" t="s">
+      <c r="N3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="M3" s="2" t="s">
+      <c r="O3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N3" s="2" t="s">
+      <c r="P3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O3" s="2" t="s">
+      <c r="Q3" s="2" t="s">
         <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B4" s="1">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="1" t="str">
+        <f>"F"&amp;B4&amp;"X"</f>
+        <v>F1X</v>
+      </c>
+      <c r="E4" s="4">
+        <v>1.92</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="5" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B5" s="1">
+        <f>B4+1</f>
+        <v>2</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="1" t="str">
+        <f t="shared" ref="D5:D22" si="0">"F"&amp;B5&amp;"X"</f>
+        <v>F2X</v>
+      </c>
+      <c r="E5" s="4">
+        <v>1.92</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="6" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B6" s="1">
+        <f t="shared" ref="B6:B26" si="1">B5+1</f>
+        <v>3</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>F3X</v>
+      </c>
+      <c r="E6" s="4">
+        <f>4.45+2*0.3</f>
+        <v>5.05</v>
+      </c>
+      <c r="F6" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="7" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B7" s="1">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>F4X</v>
+      </c>
+      <c r="E7" s="4">
+        <f>6.15+2*0.3</f>
+        <v>6.75</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="8" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B8" s="1">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>F5X</v>
+      </c>
+      <c r="E8" s="4">
+        <f>0.85+0.3</f>
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="F8" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="9" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B9" s="1">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>F6X</v>
+      </c>
+      <c r="E9" s="4">
+        <v>5.41</v>
+      </c>
+      <c r="F9" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="10" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B10" s="1">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>F7X</v>
+      </c>
+      <c r="E10" s="4">
+        <v>1.92</v>
+      </c>
+      <c r="F10" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="11" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B11" s="1">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>F8X</v>
+      </c>
+      <c r="E11" s="4">
+        <f>5+0.3</f>
+        <v>5.3</v>
+      </c>
+      <c r="F11" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="12" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B12" s="1">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>F9X</v>
+      </c>
+      <c r="E12" s="4">
+        <f>6.15+2*0.3</f>
+        <v>6.75</v>
+      </c>
+      <c r="F12" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="13" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B13" s="1">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>F10X</v>
+      </c>
+      <c r="E13" s="4">
+        <f>1.58+0.3</f>
+        <v>1.8800000000000001</v>
+      </c>
+      <c r="F13" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="14" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B14" s="1">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>F11X</v>
+      </c>
+      <c r="E14" s="4">
+        <f>2.07+0.3</f>
+        <v>2.3699999999999997</v>
+      </c>
+      <c r="F14" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="15" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B15" s="1">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D15" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>F12X</v>
+      </c>
+      <c r="E15" s="4">
+        <v>1.92</v>
+      </c>
+      <c r="F15" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="16" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B16" s="1">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>F13X</v>
+      </c>
+      <c r="E16" s="4">
+        <v>1.92</v>
+      </c>
+      <c r="F16" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B17" s="1">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D17" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>F14X</v>
+      </c>
+      <c r="E17" s="4">
+        <f>4.38+0.3</f>
+        <v>4.68</v>
+      </c>
+      <c r="F17" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B18" s="1">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D18" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>F15X</v>
+      </c>
+      <c r="E18" s="4">
+        <f>5.85+2*0.3</f>
+        <v>6.4499999999999993</v>
+      </c>
+      <c r="F18" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B19" s="1">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D19" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>F16X</v>
+      </c>
+      <c r="E19" s="4">
+        <f>11.82+2*0.3</f>
+        <v>12.42</v>
+      </c>
+      <c r="F19" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B20" s="1">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D20" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>F17X</v>
+      </c>
+      <c r="E20" s="4">
+        <f>12.08+0.3</f>
+        <v>12.38</v>
+      </c>
+      <c r="F20" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B21" s="1">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D21" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>F18X</v>
+      </c>
+      <c r="E21" s="4">
+        <f>0.41+0.3</f>
+        <v>0.71</v>
+      </c>
+      <c r="F21" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B22" s="1">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D22" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>F19X</v>
+      </c>
+      <c r="E22" s="4">
+        <f>13.4+2*0.3</f>
+        <v>14</v>
+      </c>
+      <c r="F22" s="1">
+        <v>0.25</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="M2:O2"/>
+    <mergeCell ref="O2:Q2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Diseñadas todas las fundaciones
</commit_message>
<xml_diff>
--- a/Tarea 07/muros-fundaciones.xlsx
+++ b/Tarea 07/muros-fundaciones.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{259A6D00-3777-4F18-9D89-B6E8AA276F34}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E93ADFBB-1A05-4CA4-AC11-347BC853E6AD}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="697" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1119,7 +1119,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="94">
+  <cellXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1389,6 +1389,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -72081,7 +72084,7 @@
   <dimension ref="B2:R22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -72377,8 +72380,8 @@
         <v>F4X</v>
       </c>
       <c r="E7" s="10">
-        <f>6.15+2*0.3</f>
-        <v>6.75</v>
+        <f>6.16+2*0.3</f>
+        <v>6.76</v>
       </c>
       <c r="F7" s="9">
         <v>0.25</v>
@@ -73318,7 +73321,7 @@
   <dimension ref="B2:R23"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -74614,10 +74617,10 @@
   <dimension ref="A1:BM51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="17" ySplit="6" topLeftCell="V19" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="17" ySplit="6" topLeftCell="BD7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="R1" sqref="R1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="O30" sqref="O30"/>
+      <selection pane="bottomRight" activeCell="O45" sqref="O45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -74906,7 +74909,7 @@
       <c r="Q6" s="22" t="s">
         <v>160</v>
       </c>
-      <c r="R6" s="93" t="s">
+      <c r="R6" s="94" t="s">
         <v>161</v>
       </c>
       <c r="S6" s="51" t="s">
@@ -74940,10 +74943,10 @@
       <c r="AC6" s="39"/>
       <c r="AD6" s="39"/>
       <c r="AE6" s="19"/>
-      <c r="AF6" s="91" t="s">
+      <c r="AF6" s="92" t="s">
         <v>166</v>
       </c>
-      <c r="AG6" s="92" t="s">
+      <c r="AG6" s="93" t="s">
         <v>167</v>
       </c>
       <c r="AH6" s="27" t="s">
@@ -74952,10 +74955,10 @@
       <c r="AI6" s="28" t="s">
         <v>169</v>
       </c>
-      <c r="AJ6" s="91" t="s">
+      <c r="AJ6" s="92" t="s">
         <v>170</v>
       </c>
-      <c r="AK6" s="92" t="s">
+      <c r="AK6" s="93" t="s">
         <v>171</v>
       </c>
       <c r="AL6" s="27" t="s">
@@ -74964,10 +74967,10 @@
       <c r="AM6" s="28" t="s">
         <v>173</v>
       </c>
-      <c r="AN6" s="91" t="s">
+      <c r="AN6" s="92" t="s">
         <v>174</v>
       </c>
-      <c r="AO6" s="92" t="s">
+      <c r="AO6" s="93" t="s">
         <v>175</v>
       </c>
       <c r="AP6" s="27" t="s">
@@ -74976,10 +74979,10 @@
       <c r="AQ6" s="28" t="s">
         <v>177</v>
       </c>
-      <c r="AR6" s="91" t="s">
+      <c r="AR6" s="92" t="s">
         <v>178</v>
       </c>
-      <c r="AS6" s="92" t="s">
+      <c r="AS6" s="93" t="s">
         <v>179</v>
       </c>
       <c r="AT6" s="27" t="s">
@@ -74988,10 +74991,10 @@
       <c r="AU6" s="28" t="s">
         <v>181</v>
       </c>
-      <c r="AV6" s="91" t="s">
+      <c r="AV6" s="92" t="s">
         <v>182</v>
       </c>
-      <c r="AW6" s="92" t="s">
+      <c r="AW6" s="93" t="s">
         <v>183</v>
       </c>
       <c r="AX6" s="27" t="s">
@@ -75000,10 +75003,10 @@
       <c r="AY6" s="28" t="s">
         <v>185</v>
       </c>
-      <c r="AZ6" s="91" t="s">
+      <c r="AZ6" s="92" t="s">
         <v>186</v>
       </c>
-      <c r="BA6" s="92" t="s">
+      <c r="BA6" s="93" t="s">
         <v>187</v>
       </c>
       <c r="BB6" s="27" t="s">
@@ -75013,7 +75016,7 @@
         <v>189</v>
       </c>
       <c r="BD6" s="67"/>
-      <c r="BF6" s="91" t="s">
+      <c r="BF6" s="92" t="s">
         <v>190</v>
       </c>
       <c r="BG6" s="27" t="s">
@@ -75796,7 +75799,7 @@
       </c>
       <c r="E10" s="30">
         <f>'MUROS EJE X'!E7</f>
-        <v>6.75</v>
+        <v>6.76</v>
       </c>
       <c r="F10" s="14">
         <f>'MUROS EJE X'!F7</f>
@@ -75835,26 +75838,26 @@
         <v>0.44340000000000002</v>
       </c>
       <c r="O10" s="29">
-        <f t="shared" ref="O10:O45" si="45">0.3+E10+0.3</f>
-        <v>7.35</v>
+        <f>0.55+E10+0.55</f>
+        <v>7.8599999999999994</v>
       </c>
       <c r="P10" s="30">
-        <v>1.2</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="Q10" s="30">
-        <v>1.2</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="R10" s="34">
         <f t="shared" si="18"/>
-        <v>26.46</v>
+        <v>23.776499999999999</v>
       </c>
       <c r="S10" s="32">
         <f t="shared" si="19"/>
-        <v>1.2249999999999999</v>
+        <v>1.3099999999999998</v>
       </c>
       <c r="U10" s="33">
         <f t="shared" si="0"/>
-        <v>442.44309999999996</v>
+        <v>439.75959999999998</v>
       </c>
       <c r="V10" s="34">
         <f t="shared" si="20"/>
@@ -75862,15 +75865,15 @@
       </c>
       <c r="W10" s="35">
         <f t="shared" si="21"/>
-        <v>1.5925211626082542E-2</v>
+        <v>1.6022390415126812E-2</v>
       </c>
       <c r="X10" s="32">
-        <f t="shared" ref="X10:X45" si="46">MAX(IF(W10&lt;$S10,(U10/($P10*$O10))-(6*V10/($P10*$O10^2)),IF(W10=$S10,(2*U10)/($P10*$O10),(2*U10)/($P10*(3*($O10/2-W10))))),IF(W10&lt;$S10,(U10/($P10*$O10))+(6*V10/($P10*$O10^2)),IF(W10=$S10,(2*U10)/($P10*$O10),(2*U10)/($P10*(3*($O10/2-W10))))))/10</f>
-        <v>5.0815752464251007</v>
+        <f t="shared" ref="X10:X45" si="45">MAX(IF(W10&lt;$S10,(U10/($P10*$O10))-(6*V10/($P10*$O10^2)),IF(W10=$S10,(2*U10)/($P10*$O10),(2*U10)/($P10*(3*($O10/2-W10))))),IF(W10&lt;$S10,(U10/($P10*$O10))+(6*V10/($P10*$O10^2)),IF(W10=$S10,(2*U10)/($P10*$O10),(2*U10)/($P10*(3*($O10/2-W10))))))/10</f>
+        <v>5.1484874618806193</v>
       </c>
       <c r="Y10" s="33">
         <f t="shared" si="1"/>
-        <v>560.53929999999991</v>
+        <v>557.85579999999993</v>
       </c>
       <c r="Z10" s="34">
         <f t="shared" si="2"/>
@@ -75878,24 +75881,24 @@
       </c>
       <c r="AA10" s="35">
         <f t="shared" si="22"/>
-        <v>1.2742549897928659E-2</v>
+        <v>1.2803846442037532E-2</v>
       </c>
       <c r="AB10" s="32">
-        <f t="shared" si="23"/>
-        <v>6.4214294275533348</v>
+        <f>MAX(IF(AA10&lt;$S10,(Y10/($P10*$O10))-(6*Z10/($P10*$O10^2)),IF(AA10=$S10,(2*Y10)/($P10*$O10),(2*Y10)/($P10*(3*($O10/2-AA10))))),IF(AA10&lt;$S10,(Y10/($P10*$O10))+(6*Z10/($P10*$O10^2)),IF(AA10=$S10,(2*Y10)/($P10*$O10),(2*Y10)/($P10*(3*($O10/2-AA10))))))/10-0.016</f>
+        <v>6.4992468511229644</v>
       </c>
       <c r="AC10" s="53">
         <f t="shared" si="3"/>
-        <v>0.78178080714232323</v>
+        <v>0.79207499413547988</v>
       </c>
       <c r="AD10" s="53">
         <f t="shared" si="4"/>
-        <v>0.98791221962358999</v>
+        <v>0.99988413094199458</v>
       </c>
       <c r="AE10" s="36"/>
       <c r="AF10" s="38">
         <f t="shared" si="5"/>
-        <v>659.16269999999997</v>
+        <v>656.47919999999999</v>
       </c>
       <c r="AG10" s="34">
         <f t="shared" si="6"/>
@@ -75903,15 +75906,15 @@
       </c>
       <c r="AH10" s="34">
         <f t="shared" si="24"/>
-        <v>1.0359506082489195E-2</v>
+        <v>1.0401852792898847E-2</v>
       </c>
       <c r="AI10" s="32">
         <f t="shared" si="25"/>
-        <v>7.5367014438428441</v>
+        <v>7.6531560462147254</v>
       </c>
       <c r="AJ10" s="38">
         <f t="shared" si="7"/>
-        <v>225.72349999999994</v>
+        <v>223.03999999999996</v>
       </c>
       <c r="AK10" s="34">
         <f t="shared" si="8"/>
@@ -75919,15 +75922,15 @@
       </c>
       <c r="AL10" s="34">
         <f t="shared" si="26"/>
-        <v>3.2178306645076836E-2</v>
+        <v>3.2565459110473462E-2</v>
       </c>
       <c r="AM10" s="32">
         <f t="shared" si="27"/>
-        <v>2.6264490490073582</v>
+        <v>2.643818877546515</v>
       </c>
       <c r="AN10" s="38">
         <f t="shared" si="9"/>
-        <v>693.55494999999996</v>
+        <v>690.87144999999998</v>
       </c>
       <c r="AO10" s="34">
         <f t="shared" si="10"/>
@@ -75935,15 +75938,15 @@
       </c>
       <c r="AP10" s="34">
         <f t="shared" si="28"/>
-        <v>1.0028729518836252E-2</v>
+        <v>1.0067683358459811E-2</v>
       </c>
       <c r="AQ10" s="32">
         <f t="shared" si="29"/>
-        <v>7.9278105303345825</v>
+        <v>8.0520584420629575</v>
       </c>
       <c r="AR10" s="38">
         <f t="shared" si="11"/>
-        <v>368.47554999999988</v>
+        <v>365.7920499999999</v>
       </c>
       <c r="AS10" s="34">
         <f t="shared" si="12"/>
@@ -75951,15 +75954,15 @@
       </c>
       <c r="AT10" s="34">
         <f t="shared" si="30"/>
-        <v>1.9761351872600509E-2</v>
+        <v>1.9906323825244432E-2</v>
       </c>
       <c r="AU10" s="32">
         <f t="shared" si="31"/>
-        <v>4.2451212342079687</v>
+        <v>4.2950555655617988</v>
       </c>
       <c r="AV10" s="38">
         <f t="shared" si="13"/>
-        <v>482.18545999999998</v>
+        <v>480.57535999999999</v>
       </c>
       <c r="AW10" s="34">
         <f t="shared" si="14"/>
@@ -75967,15 +75970,15 @@
       </c>
       <c r="AX10" s="34">
         <f t="shared" si="32"/>
-        <v>8.316716974418931E-3</v>
+        <v>8.3445809622865394E-3</v>
       </c>
       <c r="AY10" s="32">
         <f t="shared" si="33"/>
-        <v>5.5040713452728038</v>
+        <v>5.5937610614624775</v>
       </c>
       <c r="AZ10" s="38">
         <f t="shared" si="15"/>
-        <v>48.74625999999995</v>
+        <v>47.136159999999961</v>
       </c>
       <c r="BA10" s="34">
         <f t="shared" si="16"/>
@@ -75983,31 +75986,31 @@
       </c>
       <c r="BB10" s="34">
         <f t="shared" si="34"/>
-        <v>9.1186482819399964E-2</v>
+        <v>9.4301275284198016E-2</v>
       </c>
       <c r="BC10" s="32">
         <f t="shared" si="35"/>
-        <v>0.59381895043731725</v>
+        <v>0.58442389279426687</v>
       </c>
       <c r="BD10" s="37">
         <f t="shared" si="36"/>
-        <v>7.9278105303345825</v>
+        <v>8.0520584420629575</v>
       </c>
       <c r="BE10" s="53">
         <f t="shared" si="17"/>
-        <v>0.93268359180406857</v>
+        <v>0.94730099318387739</v>
       </c>
       <c r="BF10" s="38">
         <f t="shared" si="37"/>
-        <v>14.270058954602248</v>
+        <v>12.178738393620225</v>
       </c>
       <c r="BG10" s="34">
         <f t="shared" si="38"/>
-        <v>0.24</v>
+        <v>0.20166666666666669</v>
       </c>
       <c r="BH10" s="34">
         <f t="shared" si="39"/>
-        <v>5.9458578977509369</v>
+        <v>6.039043831547219</v>
       </c>
       <c r="BI10" s="32" t="str">
         <f t="shared" si="40"/>
@@ -76015,15 +76018,15 @@
       </c>
       <c r="BJ10" s="38">
         <f t="shared" si="41"/>
-        <v>3.5675147386505581</v>
+        <v>12.178738393620216</v>
       </c>
       <c r="BK10" s="34">
         <f t="shared" si="42"/>
-        <v>0.24</v>
+        <v>0.20166666666666669</v>
       </c>
       <c r="BL10" s="34">
         <f t="shared" si="43"/>
-        <v>1.4864644744377327</v>
+        <v>6.0390438315472137</v>
       </c>
       <c r="BM10" s="32" t="str">
         <f t="shared" si="44"/>
@@ -76113,7 +76116,7 @@
         <v>1.0952952772411786E-2</v>
       </c>
       <c r="X11" s="32">
-        <f t="shared" si="46"/>
+        <f t="shared" si="45"/>
         <v>3.7035864215263814</v>
       </c>
       <c r="Y11" s="33">
@@ -76341,156 +76344,156 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="R12" s="34">
-        <f t="shared" ref="R12" si="47">2.5*O12*P12*Q12</f>
+        <f t="shared" ref="R12" si="46">2.5*O12*P12*Q12</f>
         <v>18.180250000000001</v>
       </c>
       <c r="S12" s="32">
-        <f t="shared" ref="S12" si="48">O12/6</f>
+        <f t="shared" ref="S12" si="47">O12/6</f>
         <v>1.0016666666666667</v>
       </c>
       <c r="U12" s="33">
-        <f t="shared" ref="U12" si="49">ABS(R12+ABS(G12))</f>
+        <f t="shared" ref="U12" si="48">ABS(R12+ABS(G12))</f>
         <v>303.83114999999998</v>
       </c>
       <c r="V12" s="34">
-        <f t="shared" ref="V12" si="50">ABS(K12)</f>
+        <f t="shared" ref="V12" si="49">ABS(K12)</f>
         <v>5.8072999999999997</v>
       </c>
       <c r="W12" s="35">
-        <f t="shared" ref="W12" si="51">ABS(V12/U12)</f>
+        <f t="shared" ref="W12" si="50">ABS(V12/U12)</f>
         <v>1.9113576734972697E-2</v>
       </c>
       <c r="X12" s="32">
-        <f t="shared" ref="X12" si="52">MAX(IF(W12&lt;$S12,(U12/($P12*$O12))-(6*V12/($P12*$O12^2)),IF(W12=$S12,(2*U12)/($P12*$O12),(2*U12)/($P12*(3*($O12/2-W12))))),IF(W12&lt;$S12,(U12/($P12*$O12))+(6*V12/($P12*$O12^2)),IF(W12=$S12,(2*U12)/($P12*$O12),(2*U12)/($P12*(3*($O12/2-W12))))))/10</f>
+        <f t="shared" ref="X12" si="51">MAX(IF(W12&lt;$S12,(U12/($P12*$O12))-(6*V12/($P12*$O12^2)),IF(W12=$S12,(2*U12)/($P12*$O12),(2*U12)/($P12*(3*($O12/2-W12))))),IF(W12&lt;$S12,(U12/($P12*$O12))+(6*V12/($P12*$O12^2)),IF(W12=$S12,(2*U12)/($P12*$O12),(2*U12)/($P12*(3*($O12/2-W12))))))/10</f>
         <v>4.6835393627471582</v>
       </c>
       <c r="Y12" s="33">
-        <f t="shared" ref="Y12" si="53">ABS(R12+ABS(G12)+ABS(H12))</f>
+        <f t="shared" ref="Y12" si="52">ABS(R12+ABS(G12)+ABS(H12))</f>
         <v>391.48204999999996</v>
       </c>
       <c r="Z12" s="34">
-        <f t="shared" ref="Z12" si="54">ABS(K12+L12)</f>
+        <f t="shared" ref="Z12" si="53">ABS(K12+L12)</f>
         <v>5.8033999999999999</v>
       </c>
       <c r="AA12" s="35">
-        <f t="shared" ref="AA12" si="55">ABS(Z12/Y12)</f>
+        <f t="shared" ref="AA12" si="54">ABS(Z12/Y12)</f>
         <v>1.4824179039626467E-2</v>
       </c>
       <c r="AB12" s="32">
-        <f t="shared" ref="AB12" si="56">MAX(IF(AA12&lt;$S12,(Y12/($P12*$O12))-(6*Z12/($P12*$O12^2)),IF(AA12=$S12,(2*Y12)/($P12*$O12),(2*Y12)/($P12*(3*($O12/2-AA12))))),IF(AA12&lt;$S12,(Y12/($P12*$O12))+(6*Z12/($P12*$O12^2)),IF(AA12=$S12,(2*Y12)/($P12*$O12),(2*Y12)/($P12*(3*($O12/2-AA12))))))/10</f>
+        <f t="shared" ref="AB12" si="55">MAX(IF(AA12&lt;$S12,(Y12/($P12*$O12))-(6*Z12/($P12*$O12^2)),IF(AA12=$S12,(2*Y12)/($P12*$O12),(2*Y12)/($P12*(3*($O12/2-AA12))))),IF(AA12&lt;$S12,(Y12/($P12*$O12))+(6*Z12/($P12*$O12^2)),IF(AA12=$S12,(2*Y12)/($P12*$O12),(2*Y12)/($P12*(3*($O12/2-AA12))))))/10</f>
         <v>6.0093146840175349</v>
       </c>
       <c r="AC12" s="53">
-        <f t="shared" ref="AC12" si="57">X12/$E$2</f>
+        <f t="shared" ref="AC12" si="56">X12/$E$2</f>
         <v>0.72054451734571667</v>
       </c>
       <c r="AD12" s="53">
-        <f t="shared" ref="AD12" si="58">AB12/$E$2</f>
+        <f t="shared" ref="AD12" si="57">AB12/$E$2</f>
         <v>0.92450995138731307</v>
       </c>
       <c r="AE12" s="36"/>
       <c r="AF12" s="38">
-        <f t="shared" ref="AF12" si="59">ABS(IF(B12="x",$R12+ABS($G12)+$I12,$R12+ABS($G12)+$J12))</f>
+        <f t="shared" ref="AF12" si="58">ABS(IF(B12="x",$R12+ABS($G12)+$I12,$R12+ABS($G12)+$J12))</f>
         <v>500.48725000000002</v>
       </c>
       <c r="AG12" s="34">
-        <f t="shared" ref="AG12" si="60">ABS(IF(B12="x",$K12+$M12,$K12+$N12))</f>
+        <f t="shared" ref="AG12" si="59">ABS(IF(B12="x",$K12+$M12,$K12+$N12))</f>
         <v>5.6784999999999997</v>
       </c>
       <c r="AH12" s="34">
-        <f t="shared" ref="AH12" si="61">ABS(AG12/AF12)</f>
+        <f t="shared" ref="AH12" si="60">ABS(AG12/AF12)</f>
         <v>1.1345943378177965E-2</v>
       </c>
       <c r="AI12" s="32">
-        <f t="shared" ref="AI12" si="62">MAX(IF(AH12&lt;$S12,(AF12/($P12*$O12))-(6*AG12/($P12*$O12^2)),IF(AH12=$S12,(2*AF12)/($P12*$O12),(2*AF12)/($P12*(3*($O12/2-AH12))))),IF(AH12&lt;$S12,(AF12/($P12*$O12))+(6*AG12/($P12*$O12^2)),IF(AH12=$S12,(2*AF12)/($P12*$O12),(2*AF12)/($P12*(3*($O12/2-AH12))))))/10</f>
+        <f t="shared" ref="AI12" si="61">MAX(IF(AH12&lt;$S12,(AF12/($P12*$O12))-(6*AG12/($P12*$O12^2)),IF(AH12=$S12,(2*AF12)/($P12*$O12),(2*AF12)/($P12*(3*($O12/2-AH12))))),IF(AH12&lt;$S12,(AF12/($P12*$O12))+(6*AG12/($P12*$O12^2)),IF(AH12=$S12,(2*AF12)/($P12*$O12),(2*AF12)/($P12*(3*($O12/2-AH12))))))/10</f>
         <v>7.6562744150763695</v>
       </c>
       <c r="AJ12" s="38">
-        <f t="shared" ref="AJ12" si="63">ABS(IF(B12="x",$R12+ABS($G12)-$I12,$R12+ABS($G12)-$J12))</f>
+        <f t="shared" ref="AJ12" si="62">ABS(IF(B12="x",$R12+ABS($G12)-$I12,$R12+ABS($G12)-$J12))</f>
         <v>107.17504999999997</v>
       </c>
       <c r="AK12" s="34">
-        <f t="shared" ref="AK12" si="64">ABS(IF(B12="x",$K12-$M12,$K12-$N12))</f>
+        <f t="shared" ref="AK12" si="63">ABS(IF(B12="x",$K12-$M12,$K12-$N12))</f>
         <v>5.9360999999999997</v>
       </c>
       <c r="AL12" s="34">
-        <f t="shared" ref="AL12" si="65">ABS(AK12/AJ12)</f>
+        <f t="shared" ref="AL12" si="64">ABS(AK12/AJ12)</f>
         <v>5.5386958065333315E-2</v>
       </c>
       <c r="AM12" s="32">
-        <f t="shared" ref="AM12" si="66">MAX(IF(AL12&lt;$S12,(AJ12/($P12*$O12))-(6*AK12/($P12*$O12^2)),IF(AL12=$S12,(2*AJ12)/($P12*$O12),(2*AJ12)/($P12*(3*($O12/2-AL12))))),IF(AL12&lt;$S12,(AJ12/($P12*$O12))+(6*AK12/($P12*$O12^2)),IF(AL12=$S12,(2*AJ12)/($P12*$O12),(2*AJ12)/($P12*(3*($O12/2-AL12))))))/10</f>
+        <f t="shared" ref="AM12" si="65">MAX(IF(AL12&lt;$S12,(AJ12/($P12*$O12))-(6*AK12/($P12*$O12^2)),IF(AL12=$S12,(2*AJ12)/($P12*$O12),(2*AJ12)/($P12*(3*($O12/2-AL12))))),IF(AL12&lt;$S12,(AJ12/($P12*$O12))+(6*AK12/($P12*$O12^2)),IF(AL12=$S12,(2*AJ12)/($P12*$O12),(2*AJ12)/($P12*(3*($O12/2-AL12))))))/10</f>
         <v>1.7108043104179462</v>
       </c>
       <c r="AN12" s="38">
-        <f t="shared" ref="AN12" si="67">ABS(IF(B12="x",$R12+ABS($G12)+0.75*ABS($H12)+0.75*$I12,$R12+ABS($G12)+0.75*ABS($H12)+0.75*$J12))</f>
+        <f t="shared" ref="AN12" si="66">ABS(IF(B12="x",$R12+ABS($G12)+0.75*ABS($H12)+0.75*$I12,$R12+ABS($G12)+0.75*ABS($H12)+0.75*$J12))</f>
         <v>517.06140000000005</v>
       </c>
       <c r="AO12" s="34">
-        <f t="shared" ref="AO12" si="68">ABS(IF(B12="x",$K12+0.75*$L12+0.75*$M12,$K12+0.75*$L12+0.75*$N12))</f>
+        <f t="shared" ref="AO12" si="67">ABS(IF(B12="x",$K12+0.75*$L12+0.75*$M12,$K12+0.75*$L12+0.75*$N12))</f>
         <v>5.7077749999999998</v>
       </c>
       <c r="AP12" s="34">
-        <f t="shared" ref="AP12" si="69">ABS(AO12/AN12)</f>
+        <f t="shared" ref="AP12" si="68">ABS(AO12/AN12)</f>
         <v>1.1038872752829739E-2</v>
       </c>
       <c r="AQ12" s="32">
-        <f t="shared" ref="AQ12" si="70">MAX(IF(AP12&lt;$S12,(AN12/($P12*$O12))-(6*AO12/($P12*$O12^2)),IF(AP12=$S12,(2*AN12)/($P12*$O12),(2*AN12)/($P12*(3*($O12/2-AP12))))),IF(AP12&lt;$S12,(AN12/($P12*$O12))+(6*AO12/($P12*$O12^2)),IF(AP12=$S12,(2*AN12)/($P12*$O12),(2*AN12)/($P12*(3*($O12/2-AP12))))))/10</f>
+        <f t="shared" ref="AQ12" si="69">MAX(IF(AP12&lt;$S12,(AN12/($P12*$O12))-(6*AO12/($P12*$O12^2)),IF(AP12=$S12,(2*AN12)/($P12*$O12),(2*AN12)/($P12*(3*($O12/2-AP12))))),IF(AP12&lt;$S12,(AN12/($P12*$O12))+(6*AO12/($P12*$O12^2)),IF(AP12=$S12,(2*AN12)/($P12*$O12),(2*AN12)/($P12*(3*($O12/2-AP12))))))/10</f>
         <v>7.9074221429468512</v>
       </c>
       <c r="AR12" s="38">
-        <f t="shared" ref="AR12" si="71">ABS(IF(B12="x",$R12+ABS($G12)+0.75*ABS($H12)-0.75*$I12,$R12+ABS($G12)+0.75*ABS($H12)-0.75*$J12))</f>
+        <f t="shared" ref="AR12" si="70">ABS(IF(B12="x",$R12+ABS($G12)+0.75*ABS($H12)-0.75*$I12,$R12+ABS($G12)+0.75*ABS($H12)-0.75*$J12))</f>
         <v>222.07724999999999</v>
       </c>
       <c r="AS12" s="34">
-        <f t="shared" ref="AS12" si="72">ABS(IF(B12="x",$K12+0.75*$L12-0.75*$M12,$K12+0.75*$L12-0.75*$N12))</f>
+        <f t="shared" ref="AS12" si="71">ABS(IF(B12="x",$K12+0.75*$L12-0.75*$M12,$K12+0.75*$L12-0.75*$N12))</f>
         <v>5.900974999999999</v>
       </c>
       <c r="AT12" s="34">
-        <f t="shared" ref="AT12" si="73">ABS(AS12/AR12)</f>
+        <f t="shared" ref="AT12" si="72">ABS(AS12/AR12)</f>
         <v>2.6571722227288024E-2</v>
       </c>
       <c r="AU12" s="32">
-        <f t="shared" ref="AU12" si="74">MAX(IF(AT12&lt;$S12,(AR12/($P12*$O12))-(6*AS12/($P12*$O12^2)),IF(AT12=$S12,(2*AR12)/($P12*$O12),(2*AR12)/($P12*(3*($O12/2-AT12))))),IF(AT12&lt;$S12,(AR12/($P12*$O12))+(6*AS12/($P12*$O12^2)),IF(AT12=$S12,(2*AR12)/($P12*$O12),(2*AR12)/($P12*(3*($O12/2-AT12))))))/10</f>
+        <f t="shared" ref="AU12" si="73">MAX(IF(AT12&lt;$S12,(AR12/($P12*$O12))-(6*AS12/($P12*$O12^2)),IF(AT12=$S12,(2*AR12)/($P12*$O12),(2*AR12)/($P12*(3*($O12/2-AT12))))),IF(AT12&lt;$S12,(AR12/($P12*$O12))+(6*AS12/($P12*$O12^2)),IF(AT12=$S12,(2*AR12)/($P12*$O12),(2*AR12)/($P12*(3*($O12/2-AT12))))))/10</f>
         <v>3.4483195644530324</v>
       </c>
       <c r="AV12" s="38">
-        <f t="shared" ref="AV12" si="75">ABS(IF(B12="x",0.6*$R12+0.6*ABS($G12)+$I12,0.6*$R12+0.6*ABS($G12)+$J12))</f>
+        <f t="shared" ref="AV12" si="74">ABS(IF(B12="x",0.6*$R12+0.6*ABS($G12)+$I12,0.6*$R12+0.6*ABS($G12)+$J12))</f>
         <v>378.95479</v>
       </c>
       <c r="AW12" s="34">
-        <f t="shared" ref="AW12" si="76">ABS(IF(B12="x",0.6*$K12+$M12,0.6*$K12+$N12))</f>
+        <f t="shared" ref="AW12" si="75">ABS(IF(B12="x",0.6*$K12+$M12,0.6*$K12+$N12))</f>
         <v>3.3555799999999998</v>
       </c>
       <c r="AX12" s="34">
-        <f t="shared" ref="AX12" si="77">ABS(AW12/AV12)</f>
+        <f t="shared" ref="AX12" si="76">ABS(AW12/AV12)</f>
         <v>8.8548293584044674E-3</v>
       </c>
       <c r="AY12" s="32">
-        <f t="shared" ref="AY12" si="78">MAX(IF(AX12&lt;$S12,(AV12/($P12*$O12))-(6*AW12/($P12*$O12^2)),IF(AX12=$S12,(2*AV12)/($P12*$O12),(2*AV12)/($P12*(3*($O12/2-AX12))))),IF(AX12&lt;$S12,(AV12/($P12*$O12))+(6*AW12/($P12*$O12^2)),IF(AX12=$S12,(2*AV12)/($P12*$O12),(2*AV12)/($P12*(3*($O12/2-AX12))))))/10</f>
+        <f t="shared" ref="AY12" si="77">MAX(IF(AX12&lt;$S12,(AV12/($P12*$O12))-(6*AW12/($P12*$O12^2)),IF(AX12=$S12,(2*AV12)/($P12*$O12),(2*AV12)/($P12*(3*($O12/2-AX12))))),IF(AX12&lt;$S12,(AV12/($P12*$O12))+(6*AW12/($P12*$O12^2)),IF(AX12=$S12,(2*AV12)/($P12*$O12),(2*AV12)/($P12*(3*($O12/2-AX12))))))/10</f>
         <v>5.7828586699775064</v>
       </c>
       <c r="AZ12" s="38">
-        <f t="shared" ref="AZ12" si="79">ABS(IF(B12="x",0.6*$R12+0.6*ABS($G12)-$I12,0.6*$R12+0.6*ABS($G12)-$J12))</f>
+        <f t="shared" ref="AZ12" si="78">ABS(IF(B12="x",0.6*$R12+0.6*ABS($G12)-$I12,0.6*$R12+0.6*ABS($G12)-$J12))</f>
         <v>14.357410000000016</v>
       </c>
       <c r="BA12" s="34">
-        <f t="shared" ref="BA12" si="80">ABS(IF(B12="x",0.6*$K12-$M12,0.6*$K12-$N12))</f>
+        <f t="shared" ref="BA12" si="79">ABS(IF(B12="x",0.6*$K12-$M12,0.6*$K12-$N12))</f>
         <v>3.6131799999999998</v>
       </c>
       <c r="BB12" s="34">
-        <f t="shared" ref="BB12" si="81">ABS(BA12/AZ12)</f>
+        <f t="shared" ref="BB12" si="80">ABS(BA12/AZ12)</f>
         <v>0.25165959598562665</v>
       </c>
       <c r="BC12" s="32">
-        <f t="shared" ref="BC12" si="82">MAX(IF(BB12&lt;$S12,(AZ12/($P12*$O12))-(6*BA12/($P12*$O12^2)),IF(BB12=$S12,(2*AZ12)/($P12*$O12),(2*AZ12)/($P12*(3*($O12/2-BB12))))),IF(BB12&lt;$S12,(AZ12/($P12*$O12))+(6*BA12/($P12*$O12^2)),IF(BB12=$S12,(2*AZ12)/($P12*$O12),(2*AZ12)/($P12*(3*($O12/2-BB12))))))/10</f>
+        <f t="shared" ref="BC12" si="81">MAX(IF(BB12&lt;$S12,(AZ12/($P12*$O12))-(6*BA12/($P12*$O12^2)),IF(BB12=$S12,(2*AZ12)/($P12*$O12),(2*AZ12)/($P12*(3*($O12/2-BB12))))),IF(BB12&lt;$S12,(AZ12/($P12*$O12))+(6*BA12/($P12*$O12^2)),IF(BB12=$S12,(2*AZ12)/($P12*$O12),(2*AZ12)/($P12*(3*($O12/2-BB12))))))/10</f>
         <v>0.27173768043026175</v>
       </c>
       <c r="BD12" s="37">
-        <f t="shared" ref="BD12" si="83">MAX(AI12,AM12,AQ12,AU12,AY12,BC12)</f>
+        <f t="shared" ref="BD12" si="82">MAX(AI12,AM12,AQ12,AU12,AY12,BC12)</f>
         <v>7.9074221429468512</v>
       </c>
       <c r="BE12" s="53">
-        <f t="shared" ref="BE12" si="84">(BD12)/$E$3</f>
+        <f t="shared" ref="BE12" si="83">(BD12)/$E$3</f>
         <v>0.93028495799374722</v>
       </c>
       <c r="BF12" s="38">
@@ -76502,15 +76505,15 @@
         <v>0.20166666666666669</v>
       </c>
       <c r="BH12" s="34">
-        <f t="shared" ref="BH12" si="85">BF12/BG12/10</f>
+        <f t="shared" ref="BH12" si="84">BF12/BG12/10</f>
         <v>5.930566607210138</v>
       </c>
       <c r="BI12" s="32" t="str">
-        <f t="shared" ref="BI12" si="86">IF(BH12&lt;7,"NO PARRILLA","PARRILLA")</f>
+        <f t="shared" ref="BI12" si="85">IF(BH12&lt;7,"NO PARRILLA","PARRILLA")</f>
         <v>NO PARRILLA</v>
       </c>
       <c r="BJ12" s="38">
-        <f t="shared" ref="BJ12" si="87">($BD12*10*((O12-E12)/2)^2*1)/2</f>
+        <f t="shared" ref="BJ12" si="86">($BD12*10*((O12-E12)/2)^2*1)/2</f>
         <v>3.5583399643260787</v>
       </c>
       <c r="BK12" s="34">
@@ -76518,11 +76521,11 @@
         <v>0.20166666666666669</v>
       </c>
       <c r="BL12" s="34">
-        <f t="shared" ref="BL12" si="88">BJ12/BK12/10</f>
+        <f t="shared" ref="BL12" si="87">BJ12/BK12/10</f>
         <v>1.7644660980129312</v>
       </c>
       <c r="BM12" s="32" t="str">
-        <f t="shared" ref="BM12" si="89">IF(BL12&lt;7,"NO PARRILLA","PARRILLA")</f>
+        <f t="shared" ref="BM12" si="88">IF(BL12&lt;7,"NO PARRILLA","PARRILLA")</f>
         <v>NO PARRILLA</v>
       </c>
     </row>
@@ -76579,7 +76582,7 @@
         <v>0.2205</v>
       </c>
       <c r="O13" s="29">
-        <f t="shared" si="45"/>
+        <f t="shared" ref="O10:O45" si="89">0.3+E13+0.3</f>
         <v>2.5199999999999996</v>
       </c>
       <c r="P13" s="30">
@@ -76609,7 +76612,7 @@
         <v>2.1574032032284744E-2</v>
       </c>
       <c r="X13" s="32">
-        <f t="shared" si="46"/>
+        <f t="shared" si="45"/>
         <v>2.2144495464852612</v>
       </c>
       <c r="Y13" s="33">
@@ -76857,7 +76860,7 @@
         <v>7.2149671123509637E-3</v>
       </c>
       <c r="X14" s="32">
-        <f t="shared" si="46"/>
+        <f t="shared" si="45"/>
         <v>5.1003163992869869</v>
       </c>
       <c r="Y14" s="33">
@@ -77105,7 +77108,7 @@
         <v>1.3675661446024397E-2</v>
       </c>
       <c r="X15" s="32">
-        <f t="shared" si="46"/>
+        <f t="shared" si="45"/>
         <v>5.1392332114620167</v>
       </c>
       <c r="Y15" s="33">
@@ -77353,7 +77356,7 @@
         <v>6.8232742011445861E-3</v>
       </c>
       <c r="X16" s="32">
-        <f t="shared" si="46"/>
+        <f t="shared" si="45"/>
         <v>4.6843309789944048</v>
       </c>
       <c r="Y16" s="33">
@@ -77601,7 +77604,7 @@
         <v>1.2288284675756571E-2</v>
       </c>
       <c r="X17" s="32">
-        <f t="shared" si="46"/>
+        <f t="shared" si="45"/>
         <v>4.9057150709501132</v>
       </c>
       <c r="Y17" s="33">
@@ -77819,7 +77822,7 @@
         <v>0.22620000000000001</v>
       </c>
       <c r="O18" s="29">
-        <f t="shared" si="45"/>
+        <f t="shared" si="89"/>
         <v>2.5199999999999996</v>
       </c>
       <c r="P18" s="30">
@@ -77849,7 +77852,7 @@
         <v>3.521805527738834E-2</v>
       </c>
       <c r="X18" s="32">
-        <f t="shared" si="46"/>
+        <f t="shared" si="45"/>
         <v>2.061590702947846</v>
       </c>
       <c r="Y18" s="33">
@@ -78097,7 +78100,7 @@
         <v>8.4494535835025232E-3</v>
       </c>
       <c r="X19" s="32">
-        <f t="shared" si="46"/>
+        <f t="shared" si="45"/>
         <v>5.0500869629849863</v>
       </c>
       <c r="Y19" s="33">
@@ -78345,7 +78348,7 @@
         <v>7.3571539142923484E-2</v>
       </c>
       <c r="X20" s="32">
-        <f t="shared" si="46"/>
+        <f t="shared" si="45"/>
         <v>4.651116540090463</v>
       </c>
       <c r="Y20" s="33">
@@ -78563,7 +78566,7 @@
         <v>0.81320000000000003</v>
       </c>
       <c r="O21" s="29">
-        <f t="shared" si="45"/>
+        <f t="shared" si="89"/>
         <v>7.0499999999999989</v>
       </c>
       <c r="P21" s="30">
@@ -78594,7 +78597,7 @@
         <v>3.1186394657281749E-2</v>
       </c>
       <c r="X21" s="32">
-        <f t="shared" si="46"/>
+        <f t="shared" si="45"/>
         <v>2.7885966500679045</v>
       </c>
       <c r="Y21" s="33">
@@ -78812,7 +78815,7 @@
         <v>1.5344</v>
       </c>
       <c r="O22" s="29">
-        <f t="shared" si="45"/>
+        <f t="shared" si="89"/>
         <v>13.020000000000001</v>
       </c>
       <c r="P22" s="30">
@@ -78843,7 +78846,7 @@
         <v>3.3145448535823576E-3</v>
       </c>
       <c r="X22" s="32">
-        <f t="shared" si="46"/>
+        <f t="shared" si="45"/>
         <v>4.824370755378113</v>
       </c>
       <c r="Y22" s="33">
@@ -79061,7 +79064,7 @@
         <v>1.3482000000000001</v>
       </c>
       <c r="O23" s="29">
-        <f t="shared" si="45"/>
+        <f t="shared" si="89"/>
         <v>12.980000000000002</v>
       </c>
       <c r="P23" s="30">
@@ -79092,7 +79095,7 @@
         <v>2.8642235614903873E-2</v>
       </c>
       <c r="X23" s="32">
-        <f t="shared" si="46"/>
+        <f t="shared" si="45"/>
         <v>2.2968875275699721</v>
       </c>
       <c r="Y23" s="33">
@@ -79310,7 +79313,7 @@
         <v>0.10639999999999999</v>
       </c>
       <c r="O24" s="29">
-        <f t="shared" si="45"/>
+        <f t="shared" si="89"/>
         <v>1.31</v>
       </c>
       <c r="P24" s="30">
@@ -79341,7 +79344,7 @@
         <v>2.1610965227449399E-2</v>
       </c>
       <c r="X24" s="32">
-        <f t="shared" si="46"/>
+        <f t="shared" si="45"/>
         <v>3.1404613367519372</v>
       </c>
       <c r="Y24" s="33">
@@ -79559,7 +79562,7 @@
         <v>3.1415000000000002</v>
       </c>
       <c r="O25" s="45">
-        <f t="shared" si="45"/>
+        <f t="shared" si="89"/>
         <v>14.600000000000001</v>
       </c>
       <c r="P25" s="46">
@@ -79590,7 +79593,7 @@
         <v>2.3329118147877109E-2</v>
       </c>
       <c r="X25" s="32">
-        <f t="shared" si="46"/>
+        <f t="shared" si="45"/>
         <v>3.3799620848189149</v>
       </c>
       <c r="Y25" s="33">
@@ -79808,7 +79811,7 @@
         <v>0.97950000000000004</v>
       </c>
       <c r="O26" s="90">
-        <f t="shared" si="45"/>
+        <f t="shared" si="89"/>
         <v>36.380999999999993</v>
       </c>
       <c r="P26" s="42">
@@ -79838,7 +79841,7 @@
         <v>2.8342942366134305E-3</v>
       </c>
       <c r="X26" s="55">
-        <f t="shared" si="46"/>
+        <f t="shared" si="45"/>
         <v>0.79803014685745255</v>
       </c>
       <c r="Y26" s="61">
@@ -80056,7 +80059,7 @@
         <v>0.34520000000000001</v>
       </c>
       <c r="O27" s="29">
-        <f t="shared" si="45"/>
+        <f t="shared" si="89"/>
         <v>6.0299999999999994</v>
       </c>
       <c r="P27" s="30">
@@ -80086,7 +80089,7 @@
         <v>2.4994055899386785E-2</v>
       </c>
       <c r="X27" s="32">
-        <f t="shared" si="46"/>
+        <f t="shared" si="45"/>
         <v>3.8315102431457966</v>
       </c>
       <c r="Y27" s="33">
@@ -80334,7 +80337,7 @@
         <v>3.042996590892882E-3</v>
       </c>
       <c r="X28" s="32">
-        <f t="shared" si="46"/>
+        <f t="shared" si="45"/>
         <v>5.1213839999999999</v>
       </c>
       <c r="Y28" s="33">
@@ -80552,7 +80555,7 @@
         <v>2.2100000000000002E-2</v>
       </c>
       <c r="O29" s="29">
-        <f t="shared" si="45"/>
+        <f t="shared" si="89"/>
         <v>1.45</v>
       </c>
       <c r="P29" s="30">
@@ -80582,7 +80585,7 @@
         <v>1.6806773039659193E-3</v>
       </c>
       <c r="X29" s="32">
-        <f t="shared" si="46"/>
+        <f t="shared" si="45"/>
         <v>4.9672223543400715</v>
       </c>
       <c r="Y29" s="33">
@@ -80800,26 +80803,26 @@
         <v>0.51149999999999995</v>
       </c>
       <c r="O30" s="29">
-        <f>0.5+E30+0.5</f>
-        <v>12.5</v>
+        <f>1+E30+1</f>
+        <v>13.5</v>
       </c>
       <c r="P30" s="30">
-        <v>1.6</v>
+        <v>1.5</v>
       </c>
       <c r="Q30" s="30">
-        <v>1.4</v>
+        <v>2</v>
       </c>
       <c r="R30" s="34">
         <f t="shared" si="18"/>
-        <v>70</v>
+        <v>101.25</v>
       </c>
       <c r="S30" s="32">
         <f t="shared" si="19"/>
-        <v>2.0833333333333335</v>
+        <v>2.25</v>
       </c>
       <c r="U30" s="33">
         <f t="shared" si="0"/>
-        <v>1022.466</v>
+        <v>1053.7159999999999</v>
       </c>
       <c r="V30" s="34">
         <f t="shared" si="20"/>
@@ -80827,15 +80830,15 @@
       </c>
       <c r="W30" s="35">
         <f t="shared" si="21"/>
-        <v>3.9111324973153141E-4</v>
+        <v>3.7951402465180372E-4</v>
       </c>
       <c r="X30" s="32">
-        <f t="shared" si="46"/>
-        <v>5.1132897599999998</v>
+        <f t="shared" si="45"/>
+        <v>5.2044134979423866</v>
       </c>
       <c r="Y30" s="33">
         <f t="shared" si="1"/>
-        <v>1254.703</v>
+        <v>1285.953</v>
       </c>
       <c r="Z30" s="34">
         <f t="shared" si="2"/>
@@ -80843,24 +80846,24 @@
       </c>
       <c r="AA30" s="35">
         <f t="shared" si="22"/>
-        <v>1.0456657870428304E-4</v>
+        <v>1.0202550170962705E-4</v>
       </c>
       <c r="AB30" s="32">
         <f t="shared" si="23"/>
-        <v>6.2738298799999992</v>
+        <v>6.3506731412894375</v>
       </c>
       <c r="AC30" s="53">
         <f t="shared" si="90"/>
-        <v>0.7866599630769231</v>
+        <v>0.80067899968344414</v>
       </c>
       <c r="AD30" s="53">
         <f t="shared" si="91"/>
-        <v>0.96520459692307681</v>
+        <v>0.97702663712145188</v>
       </c>
       <c r="AE30" s="36"/>
       <c r="AF30" s="38">
         <f t="shared" si="5"/>
-        <v>1066.3951</v>
+        <v>1097.6451</v>
       </c>
       <c r="AG30" s="34">
         <f t="shared" si="6"/>
@@ -80868,15 +80871,15 @@
       </c>
       <c r="AH30" s="34">
         <f t="shared" si="24"/>
-        <v>8.5465508984428008E-4</v>
+        <v>8.3032302517453043E-4</v>
       </c>
       <c r="AI30" s="32">
         <f t="shared" si="25"/>
-        <v>5.3341628600000002</v>
+        <v>5.4224699588477367</v>
       </c>
       <c r="AJ30" s="38">
         <f t="shared" si="7"/>
-        <v>978.53690000000006</v>
+        <v>1009.7868999999999</v>
       </c>
       <c r="AK30" s="34">
         <f t="shared" si="8"/>
@@ -80884,15 +80887,15 @@
       </c>
       <c r="AL30" s="34">
         <f t="shared" si="26"/>
-        <v>1.140478197602972E-4</v>
+        <v>1.1051836778631212E-4</v>
       </c>
       <c r="AM30" s="32">
         <f t="shared" si="27"/>
-        <v>4.8929523399999999</v>
+        <v>4.9868469135802469</v>
       </c>
       <c r="AN30" s="38">
         <f t="shared" si="9"/>
-        <v>1229.5905749999999</v>
+        <v>1260.8405749999999</v>
       </c>
       <c r="AO30" s="34">
         <f t="shared" si="10"/>
@@ -80900,15 +80903,15 @@
       </c>
       <c r="AP30" s="34">
         <f t="shared" si="28"/>
-        <v>3.1327501026103747E-4</v>
+        <v>3.0551047264639305E-4</v>
       </c>
       <c r="AQ30" s="32">
         <f t="shared" si="29"/>
-        <v>6.1488773549999998</v>
+        <v>6.2272186419753082</v>
       </c>
       <c r="AR30" s="38">
         <f t="shared" si="11"/>
-        <v>1163.696925</v>
+        <v>1194.946925</v>
       </c>
       <c r="AS30" s="34">
         <f t="shared" si="12"/>
@@ -80916,15 +80919,15 @@
       </c>
       <c r="AT30" s="34">
         <f t="shared" si="30"/>
-        <v>3.2830713203096251E-4</v>
+        <v>3.1972131314535169E-4</v>
       </c>
       <c r="AU30" s="32">
         <f t="shared" si="31"/>
-        <v>5.8194015449999998</v>
+        <v>5.9018109876543203</v>
       </c>
       <c r="AV30" s="38">
         <f t="shared" si="13"/>
-        <v>657.40869999999995</v>
+        <v>676.15869999999995</v>
       </c>
       <c r="AW30" s="34">
         <f t="shared" si="14"/>
@@ -80932,15 +80935,15 @@
       </c>
       <c r="AX30" s="34">
         <f t="shared" si="32"/>
-        <v>1.1430332455289989E-3</v>
+        <v>1.1113367320423444E-3</v>
       </c>
       <c r="AY30" s="32">
         <f t="shared" si="33"/>
-        <v>3.2888469559999995</v>
+        <v>3.3407045596707818</v>
       </c>
       <c r="AZ30" s="38">
         <f t="shared" si="15"/>
-        <v>569.55050000000006</v>
+        <v>588.30050000000006</v>
       </c>
       <c r="BA30" s="34">
         <f t="shared" si="16"/>
@@ -80948,31 +80951,31 @@
       </c>
       <c r="BB30" s="34">
         <f t="shared" si="34"/>
-        <v>4.7679705311469298E-4</v>
+        <v>4.6160083154782284E-4</v>
       </c>
       <c r="BC30" s="32">
         <f t="shared" si="35"/>
-        <v>2.8484042440000001</v>
+        <v>2.9057836707818931</v>
       </c>
       <c r="BD30" s="37">
         <f t="shared" si="36"/>
-        <v>6.1488773549999998</v>
+        <v>6.2272186419753082</v>
       </c>
       <c r="BE30" s="53">
         <f t="shared" si="17"/>
-        <v>0.72339733588235289</v>
+        <v>0.73261395787944805</v>
       </c>
       <c r="BF30" s="38">
         <f t="shared" si="37"/>
-        <v>19.676407536000003</v>
+        <v>17.514052430555555</v>
       </c>
       <c r="BG30" s="34">
         <f t="shared" si="38"/>
-        <v>0.32666666666666661</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="BH30" s="34">
         <f t="shared" si="39"/>
-        <v>6.0233900620408187</v>
+        <v>2.6271078645833335</v>
       </c>
       <c r="BI30" s="32" t="str">
         <f t="shared" si="40"/>
@@ -80980,15 +80983,15 @@
       </c>
       <c r="BJ30" s="38">
         <f t="shared" si="41"/>
-        <v>7.6860966937499997</v>
+        <v>31.136093209876542</v>
       </c>
       <c r="BK30" s="34">
         <f t="shared" si="42"/>
-        <v>0.32666666666666661</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="BL30" s="34">
         <f t="shared" si="43"/>
-        <v>2.3528867429846945</v>
+        <v>4.6704139814814818</v>
       </c>
       <c r="BM30" s="32" t="str">
         <f t="shared" si="44"/>
@@ -81048,7 +81051,7 @@
         <v>4.0599999999999997E-2</v>
       </c>
       <c r="O31" s="29">
-        <f t="shared" si="45"/>
+        <f t="shared" si="89"/>
         <v>3.26</v>
       </c>
       <c r="P31" s="30">
@@ -81078,7 +81081,7 @@
         <v>8.996478776223199E-3</v>
       </c>
       <c r="X31" s="32">
-        <f t="shared" si="46"/>
+        <f t="shared" si="45"/>
         <v>2.8293832097557301</v>
       </c>
       <c r="Y31" s="33">
@@ -81296,7 +81299,7 @@
         <v>0.1429</v>
       </c>
       <c r="O32" s="29">
-        <f t="shared" si="45"/>
+        <f t="shared" si="89"/>
         <v>2.3499999999999996</v>
       </c>
       <c r="P32" s="30">
@@ -81326,7 +81329,7 @@
         <v>1.4758962354029997E-2</v>
       </c>
       <c r="X32" s="32">
-        <f t="shared" si="46"/>
+        <f t="shared" si="45"/>
         <v>4.8665540968764152</v>
       </c>
       <c r="Y32" s="33">
@@ -81544,18 +81547,18 @@
         <v>0.30609999999999998</v>
       </c>
       <c r="O33" s="29">
-        <f t="shared" si="45"/>
+        <f t="shared" si="89"/>
         <v>7.1</v>
       </c>
       <c r="P33" s="30">
-        <v>1</v>
+        <v>1.2</v>
       </c>
       <c r="Q33" s="30">
         <v>1</v>
       </c>
       <c r="R33" s="34">
         <f t="shared" si="18"/>
-        <v>17.75</v>
+        <v>21.3</v>
       </c>
       <c r="S33" s="32">
         <f t="shared" si="19"/>
@@ -81563,7 +81566,7 @@
       </c>
       <c r="U33" s="33">
         <f t="shared" si="0"/>
-        <v>429.24079999999998</v>
+        <v>432.79079999999999</v>
       </c>
       <c r="V33" s="34">
         <f t="shared" si="20"/>
@@ -81571,15 +81574,15 @@
       </c>
       <c r="W33" s="35">
         <f t="shared" si="21"/>
-        <v>1.0698656791246312E-2</v>
+        <v>1.0610900231705479E-2</v>
       </c>
       <c r="X33" s="32">
-        <f t="shared" si="46"/>
-        <v>6.1003044634001196</v>
+        <f t="shared" si="45"/>
+        <v>5.1252537195000993</v>
       </c>
       <c r="Y33" s="33">
         <f t="shared" si="1"/>
-        <v>526.90189999999996</v>
+        <v>530.45190000000002</v>
       </c>
       <c r="Z33" s="34">
         <f t="shared" si="2"/>
@@ -81587,24 +81590,24 @@
       </c>
       <c r="AA33" s="35">
         <f t="shared" si="22"/>
-        <v>9.1326298121149306E-3</v>
+        <v>9.0715105365821083E-3</v>
       </c>
       <c r="AB33" s="32">
         <f t="shared" si="23"/>
-        <v>7.4784278714540759</v>
+        <v>6.2736898928783971</v>
       </c>
       <c r="AC33" s="53">
         <f t="shared" si="90"/>
-        <v>0.9385083789846338</v>
+        <v>0.78850057223078451</v>
       </c>
       <c r="AD33" s="53">
         <f t="shared" si="91"/>
-        <v>1.1505273648390886</v>
+        <v>0.96518306044283031</v>
       </c>
       <c r="AE33" s="36"/>
       <c r="AF33" s="38">
         <f t="shared" si="5"/>
-        <v>484.07819999999998</v>
+        <v>487.62819999999999</v>
       </c>
       <c r="AG33" s="34">
         <f t="shared" si="6"/>
@@ -81612,15 +81615,15 @@
       </c>
       <c r="AH33" s="34">
         <f t="shared" si="24"/>
-        <v>1.0119026223449021E-2</v>
+        <v>1.0045358328332938E-2</v>
       </c>
       <c r="AI33" s="32">
         <f t="shared" si="25"/>
-        <v>6.8763055346161464</v>
+        <v>5.77192127884679</v>
       </c>
       <c r="AJ33" s="38">
         <f t="shared" si="7"/>
-        <v>374.40339999999998</v>
+        <v>377.95339999999999</v>
       </c>
       <c r="AK33" s="34">
         <f t="shared" si="8"/>
@@ -81628,15 +81631,15 @@
       </c>
       <c r="AL33" s="34">
         <f t="shared" si="26"/>
-        <v>1.1448079798420635E-2</v>
+        <v>1.1340551507143474E-2</v>
       </c>
       <c r="AM33" s="32">
         <f t="shared" si="27"/>
-        <v>5.3243033921840901</v>
+        <v>4.4785861601534087</v>
       </c>
       <c r="AN33" s="38">
         <f t="shared" si="9"/>
-        <v>543.61467500000003</v>
+        <v>547.16467499999999</v>
       </c>
       <c r="AO33" s="34">
         <f t="shared" si="10"/>
@@ -81644,15 +81647,15 @@
       </c>
       <c r="AP33" s="34">
         <f t="shared" si="28"/>
-        <v>9.1731335251389202E-3</v>
+        <v>9.1136183087842781E-3</v>
       </c>
       <c r="AQ33" s="32">
         <f t="shared" si="29"/>
-        <v>7.7158978228526092</v>
+        <v>6.4715815190438404</v>
       </c>
       <c r="AR33" s="38">
         <f t="shared" si="11"/>
-        <v>461.35857499999997</v>
+        <v>464.90857499999993</v>
       </c>
       <c r="AS33" s="34">
         <f t="shared" si="12"/>
@@ -81660,15 +81663,15 @@
       </c>
       <c r="AT33" s="34">
         <f t="shared" si="30"/>
-        <v>9.8134081500490158E-3</v>
+        <v>9.7384738494014668E-3</v>
       </c>
       <c r="AU33" s="32">
         <f t="shared" si="31"/>
-        <v>6.551896216028565</v>
+        <v>5.5015801800238036</v>
       </c>
       <c r="AV33" s="38">
         <f t="shared" si="13"/>
-        <v>312.38187999999997</v>
+        <v>314.51187999999996</v>
       </c>
       <c r="AW33" s="34">
         <f t="shared" si="14"/>
@@ -81676,15 +81679,15 @@
       </c>
       <c r="AX33" s="34">
         <f t="shared" si="32"/>
-        <v>9.8004404096678072E-3</v>
+        <v>9.7340679150180274E-3</v>
       </c>
       <c r="AY33" s="32">
         <f t="shared" si="33"/>
-        <v>4.4361837492561005</v>
+        <v>3.7218197910467503</v>
       </c>
       <c r="AZ33" s="38">
         <f t="shared" si="15"/>
-        <v>202.70707999999996</v>
+        <v>204.83707999999996</v>
       </c>
       <c r="BA33" s="34">
         <f t="shared" si="16"/>
@@ -81692,23 +81695,23 @@
       </c>
       <c r="BB33" s="34">
         <f t="shared" si="34"/>
-        <v>1.2082853741467739E-2</v>
+        <v>1.1957210091063592E-2</v>
       </c>
       <c r="BC33" s="32">
         <f t="shared" si="35"/>
-        <v>2.8841816068240425</v>
+        <v>2.4284846723533686</v>
       </c>
       <c r="BD33" s="37">
         <f t="shared" si="36"/>
-        <v>7.7158978228526092</v>
+        <v>6.4715815190438404</v>
       </c>
       <c r="BE33" s="53">
         <f t="shared" si="17"/>
-        <v>0.90775268504148343</v>
+        <v>0.76136253165221657</v>
       </c>
       <c r="BF33" s="38">
         <f t="shared" si="37"/>
-        <v>9.6448722785657619</v>
+        <v>11.648846734278912</v>
       </c>
       <c r="BG33" s="34">
         <f t="shared" si="38"/>
@@ -81716,7 +81719,7 @@
       </c>
       <c r="BH33" s="34">
         <f t="shared" si="39"/>
-        <v>5.7869233671394573</v>
+        <v>6.9893080405673471</v>
       </c>
       <c r="BI33" s="32" t="str">
         <f t="shared" si="40"/>
@@ -81724,7 +81727,7 @@
       </c>
       <c r="BJ33" s="38">
         <f t="shared" si="41"/>
-        <v>3.4721540202836705</v>
+        <v>2.9122116835697249</v>
       </c>
       <c r="BK33" s="34">
         <f t="shared" si="42"/>
@@ -81732,7 +81735,7 @@
       </c>
       <c r="BL33" s="34">
         <f t="shared" si="43"/>
-        <v>2.0832924121702026</v>
+        <v>1.747327010141835</v>
       </c>
       <c r="BM33" s="32" t="str">
         <f t="shared" si="44"/>
@@ -81792,26 +81795,26 @@
         <v>0.1028</v>
       </c>
       <c r="O34" s="29">
-        <f t="shared" si="45"/>
-        <v>4.6599999999999993</v>
+        <f>0.5+E34+0.5</f>
+        <v>5.0599999999999996</v>
       </c>
       <c r="P34" s="30">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="Q34" s="30">
-        <v>1</v>
+        <v>1.3</v>
       </c>
       <c r="R34" s="34">
         <f t="shared" si="18"/>
-        <v>11.649999999999999</v>
+        <v>24.667499999999997</v>
       </c>
       <c r="S34" s="32">
         <f t="shared" si="19"/>
-        <v>0.77666666666666651</v>
+        <v>0.84333333333333327</v>
       </c>
       <c r="U34" s="33">
         <f t="shared" si="0"/>
-        <v>383.40749999999997</v>
+        <v>396.42500000000001</v>
       </c>
       <c r="V34" s="34">
         <f t="shared" si="20"/>
@@ -81819,15 +81822,15 @@
       </c>
       <c r="W34" s="35">
         <f t="shared" si="21"/>
-        <v>1.8061722840580845E-3</v>
+        <v>1.7468625843476066E-3</v>
       </c>
       <c r="X34" s="32">
-        <f t="shared" si="46"/>
-        <v>8.246762465692866</v>
+        <f t="shared" si="45"/>
+        <v>5.2338095684461043</v>
       </c>
       <c r="Y34" s="33">
         <f t="shared" si="1"/>
-        <v>476.26409999999998</v>
+        <v>489.28160000000003</v>
       </c>
       <c r="Z34" s="34">
         <f t="shared" si="2"/>
@@ -81835,24 +81838,24 @@
       </c>
       <c r="AA34" s="35">
         <f t="shared" si="22"/>
-        <v>1.6927582826419209E-3</v>
+        <v>1.6477218844935105E-3</v>
       </c>
       <c r="AB34" s="32">
         <f t="shared" si="23"/>
-        <v>10.242534887362082</v>
+        <v>6.4589929957766357</v>
       </c>
       <c r="AC34" s="53">
         <f t="shared" si="90"/>
-        <v>1.2687326870296718</v>
+        <v>0.80520147206863146</v>
       </c>
       <c r="AD34" s="53">
         <f t="shared" si="91"/>
-        <v>1.575774598055705</v>
+        <v>0.99369123011948246</v>
       </c>
       <c r="AE34" s="36"/>
       <c r="AF34" s="38">
         <f t="shared" si="5"/>
-        <v>414.17589999999996</v>
+        <v>427.1934</v>
       </c>
       <c r="AG34" s="34">
         <f t="shared" si="6"/>
@@ -81860,15 +81863,15 @@
       </c>
       <c r="AH34" s="34">
         <f t="shared" si="24"/>
-        <v>1.9201986402395698E-3</v>
+        <v>1.8616860653746055E-3</v>
       </c>
       <c r="AI34" s="32">
         <f t="shared" si="25"/>
-        <v>8.9098689145130692</v>
+        <v>5.6407963567623307</v>
       </c>
       <c r="AJ34" s="38">
         <f t="shared" si="7"/>
-        <v>352.63909999999998</v>
+        <v>365.65660000000003</v>
       </c>
       <c r="AK34" s="34">
         <f t="shared" si="8"/>
@@ -81876,15 +81879,15 @@
       </c>
       <c r="AL34" s="34">
         <f t="shared" si="26"/>
-        <v>1.6722479157869903E-3</v>
+        <v>1.61271531814276E-3</v>
       </c>
       <c r="AM34" s="32">
         <f t="shared" si="27"/>
-        <v>7.5836560168726637</v>
+        <v>4.826822780129878</v>
       </c>
       <c r="AN34" s="38">
         <f t="shared" si="9"/>
-        <v>476.12624999999997</v>
+        <v>489.14375000000001</v>
       </c>
       <c r="AO34" s="34">
         <f t="shared" si="10"/>
@@ -81892,15 +81895,15 @@
       </c>
       <c r="AP34" s="34">
         <f t="shared" si="28"/>
-        <v>1.7954796653198602E-3</v>
+        <v>1.7476968682519198E-3</v>
       </c>
       <c r="AQ34" s="32">
         <f t="shared" si="29"/>
-        <v>10.240921618559931</v>
+        <v>6.457937230181173</v>
       </c>
       <c r="AR34" s="38">
         <f t="shared" si="11"/>
-        <v>429.97364999999996</v>
+        <v>442.99115</v>
       </c>
       <c r="AS34" s="34">
         <f t="shared" si="12"/>
@@ -81908,15 +81911,15 @@
       </c>
       <c r="AT34" s="34">
         <f t="shared" si="30"/>
-        <v>1.6295766031244007E-3</v>
+        <v>1.581690740322916E-3</v>
       </c>
       <c r="AU34" s="32">
         <f t="shared" si="31"/>
-        <v>9.2462619453296249</v>
+        <v>5.8474570477068326</v>
       </c>
       <c r="AV34" s="38">
         <f t="shared" si="13"/>
-        <v>260.81290000000001</v>
+        <v>268.6234</v>
       </c>
       <c r="AW34" s="34">
         <f t="shared" si="14"/>
@@ -81924,15 +81927,15 @@
       </c>
       <c r="AX34" s="34">
         <f t="shared" si="32"/>
-        <v>1.9872483301247752E-3</v>
+        <v>1.9294670531308888E-3</v>
       </c>
       <c r="AY34" s="32">
         <f t="shared" si="33"/>
-        <v>5.611163928235924</v>
+        <v>3.5472725293838883</v>
       </c>
       <c r="AZ34" s="38">
         <f t="shared" si="15"/>
-        <v>199.27609999999999</v>
+        <v>207.08659999999998</v>
       </c>
       <c r="BA34" s="34">
         <f t="shared" si="16"/>
@@ -81940,47 +81943,47 @@
       </c>
       <c r="BB34" s="34">
         <f t="shared" si="34"/>
-        <v>1.5691796457277115E-3</v>
+        <v>1.5099963010643857E-3</v>
       </c>
       <c r="BC34" s="32">
         <f t="shared" si="35"/>
-        <v>4.2849510305955167</v>
+        <v>2.7332989527514355</v>
       </c>
       <c r="BD34" s="37">
         <f t="shared" si="36"/>
-        <v>10.240921618559931</v>
+        <v>6.457937230181173</v>
       </c>
       <c r="BE34" s="53">
         <f t="shared" si="17"/>
-        <v>1.2048143080658742</v>
+        <v>0.75975732119778505</v>
       </c>
       <c r="BF34" s="38">
         <f t="shared" si="37"/>
-        <v>12.801152023199913</v>
+        <v>18.16294845988455</v>
       </c>
       <c r="BG34" s="34">
         <f t="shared" si="38"/>
-        <v>0.16666666666666666</v>
+        <v>0.28166666666666668</v>
       </c>
       <c r="BH34" s="34">
         <f t="shared" si="39"/>
-        <v>7.6806912139199479</v>
+        <v>6.4483840685980649</v>
       </c>
       <c r="BI34" s="32" t="str">
         <f t="shared" si="40"/>
-        <v>PARRILLA</v>
+        <v>NO PARRILLA</v>
       </c>
       <c r="BJ34" s="38">
         <f t="shared" si="41"/>
-        <v>4.6084147283519634</v>
+        <v>8.0724215377264663</v>
       </c>
       <c r="BK34" s="34">
         <f t="shared" si="42"/>
-        <v>0.16666666666666666</v>
+        <v>0.28166666666666668</v>
       </c>
       <c r="BL34" s="34">
         <f t="shared" si="43"/>
-        <v>2.7650488370111779</v>
+        <v>2.8659484749324733</v>
       </c>
       <c r="BM34" s="32" t="str">
         <f t="shared" si="44"/>
@@ -82040,18 +82043,18 @@
         <v>2.4799999999999999E-2</v>
       </c>
       <c r="O35" s="29">
-        <f t="shared" si="45"/>
+        <f t="shared" si="89"/>
         <v>1.5</v>
       </c>
       <c r="P35" s="30">
-        <v>1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="Q35" s="30">
         <v>1</v>
       </c>
       <c r="R35" s="34">
         <f t="shared" si="18"/>
-        <v>3.75</v>
+        <v>4.125</v>
       </c>
       <c r="S35" s="32">
         <f t="shared" si="19"/>
@@ -82059,7 +82062,7 @@
       </c>
       <c r="U35" s="33">
         <f t="shared" si="0"/>
-        <v>79.153300000000002</v>
+        <v>79.528300000000002</v>
       </c>
       <c r="V35" s="34">
         <f t="shared" si="20"/>
@@ -82067,15 +82070,15 @@
       </c>
       <c r="W35" s="35">
         <f t="shared" si="21"/>
-        <v>2.8299514991794402E-4</v>
+        <v>2.8166074215090728E-4</v>
       </c>
       <c r="X35" s="32">
-        <f t="shared" si="46"/>
-        <v>5.2828600000000003</v>
+        <f t="shared" si="45"/>
+        <v>4.8253272727272725</v>
       </c>
       <c r="Y35" s="33">
         <f t="shared" si="1"/>
-        <v>98.905500000000004</v>
+        <v>99.280500000000004</v>
       </c>
       <c r="Z35" s="34">
         <f t="shared" si="2"/>
@@ -82083,24 +82086,24 @@
       </c>
       <c r="AA35" s="35">
         <f t="shared" si="22"/>
-        <v>2.5377759578587642E-4</v>
+        <v>2.5281903294201781E-4</v>
       </c>
       <c r="AB35" s="32">
         <f t="shared" si="23"/>
-        <v>6.6003933333333338</v>
+        <v>6.0230848484848476</v>
       </c>
       <c r="AC35" s="53">
         <f t="shared" si="90"/>
-        <v>0.81274769230769239</v>
+        <v>0.74235804195804189</v>
       </c>
       <c r="AD35" s="53">
         <f t="shared" si="91"/>
-        <v>1.0154451282051282</v>
+        <v>0.9266284382284381</v>
       </c>
       <c r="AE35" s="36"/>
       <c r="AF35" s="38">
         <f t="shared" si="5"/>
-        <v>102.73009999999999</v>
+        <v>103.10509999999999</v>
       </c>
       <c r="AG35" s="34">
         <f t="shared" si="6"/>
@@ -82108,15 +82111,15 @@
       </c>
       <c r="AH35" s="34">
         <f t="shared" si="24"/>
-        <v>2.3362188881350252E-5</v>
+        <v>2.3277219070637625E-5</v>
       </c>
       <c r="AI35" s="32">
         <f t="shared" si="25"/>
-        <v>6.8493133333333329</v>
+        <v>6.2493757575757574</v>
       </c>
       <c r="AJ35" s="38">
         <f t="shared" si="7"/>
-        <v>55.576500000000003</v>
+        <v>55.951500000000003</v>
       </c>
       <c r="AK35" s="34">
         <f t="shared" si="8"/>
@@ -82124,15 +82127,15 @@
       </c>
       <c r="AL35" s="34">
         <f t="shared" si="26"/>
-        <v>8.4927982150729165E-4</v>
+        <v>8.4358775010500158E-4</v>
       </c>
       <c r="AM35" s="32">
         <f t="shared" si="27"/>
-        <v>3.7176866666666668</v>
+        <v>3.402442424242424</v>
       </c>
       <c r="AN35" s="38">
         <f t="shared" si="9"/>
-        <v>111.65004999999999</v>
+        <v>112.02504999999999</v>
       </c>
       <c r="AO35" s="34">
         <f t="shared" si="10"/>
@@ -82140,15 +82143,15 @@
       </c>
       <c r="AP35" s="34">
         <f t="shared" si="28"/>
-        <v>2.8504241601324859E-4</v>
+        <v>2.8408824633419051E-4</v>
       </c>
       <c r="AQ35" s="32">
         <f t="shared" si="29"/>
-        <v>7.4518233333333326</v>
+        <v>6.7971121212121206</v>
       </c>
       <c r="AR35" s="38">
         <f t="shared" si="11"/>
-        <v>76.284850000000006</v>
+        <v>76.659850000000006</v>
       </c>
       <c r="AS35" s="34">
         <f t="shared" si="12"/>
@@ -82156,15 +82159,15 @@
       </c>
       <c r="AT35" s="34">
         <f t="shared" si="30"/>
-        <v>7.0459599776364422E-5</v>
+        <v>7.0114929783974192E-5</v>
       </c>
       <c r="AU35" s="32">
         <f t="shared" si="31"/>
-        <v>5.0870900000000008</v>
+        <v>4.6473545454545455</v>
       </c>
       <c r="AV35" s="38">
         <f t="shared" si="13"/>
-        <v>71.068780000000004</v>
+        <v>71.293779999999998</v>
       </c>
       <c r="AW35" s="34">
         <f t="shared" si="14"/>
@@ -82172,15 +82175,15 @@
       </c>
       <c r="AX35" s="34">
         <f t="shared" si="32"/>
-        <v>1.5984515282237854E-4</v>
+        <v>1.5934068862669367E-4</v>
       </c>
       <c r="AY35" s="32">
         <f t="shared" si="33"/>
-        <v>4.7409480000000004</v>
+        <v>4.3235890909090902</v>
       </c>
       <c r="AZ35" s="38">
         <f t="shared" si="15"/>
-        <v>23.915179999999999</v>
+        <v>24.140180000000001</v>
       </c>
       <c r="BA35" s="34">
         <f t="shared" si="16"/>
@@ -82188,23 +82191,23 @@
       </c>
       <c r="BB35" s="34">
         <f t="shared" si="34"/>
-        <v>1.598984410738284E-3</v>
+        <v>1.5840809803406601E-3</v>
       </c>
       <c r="BC35" s="32">
         <f t="shared" si="35"/>
-        <v>1.6045426666666665</v>
+        <v>1.4723115151515151</v>
       </c>
       <c r="BD35" s="37">
         <f t="shared" si="36"/>
-        <v>7.4518233333333326</v>
+        <v>6.7971121212121206</v>
       </c>
       <c r="BE35" s="53">
         <f t="shared" si="17"/>
-        <v>0.87668509803921557</v>
+        <v>0.7996602495543671</v>
       </c>
       <c r="BF35" s="38">
         <f t="shared" si="37"/>
-        <v>9.3147791666666659</v>
+        <v>10.280632083333334</v>
       </c>
       <c r="BG35" s="34">
         <f t="shared" si="38"/>
@@ -82212,7 +82215,7 @@
       </c>
       <c r="BH35" s="34">
         <f t="shared" si="39"/>
-        <v>5.5888675000000001</v>
+        <v>6.1683792500000001</v>
       </c>
       <c r="BI35" s="32" t="str">
         <f t="shared" si="40"/>
@@ -82220,7 +82223,7 @@
       </c>
       <c r="BJ35" s="38">
         <f t="shared" si="41"/>
-        <v>3.3533204999999997</v>
+        <v>3.0587004545454541</v>
       </c>
       <c r="BK35" s="34">
         <f t="shared" si="42"/>
@@ -82228,7 +82231,7 @@
       </c>
       <c r="BL35" s="34">
         <f t="shared" si="43"/>
-        <v>2.0119923000000002</v>
+        <v>1.8352202727272726</v>
       </c>
       <c r="BM35" s="32" t="str">
         <f t="shared" si="44"/>
@@ -82288,26 +82291,26 @@
         <v>1.95E-2</v>
       </c>
       <c r="O36" s="29">
-        <f t="shared" si="45"/>
-        <v>1.6300000000000001</v>
+        <f>0.5+E36+0.5</f>
+        <v>2.0300000000000002</v>
       </c>
       <c r="P36" s="30">
-        <v>1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="Q36" s="30">
         <v>1</v>
       </c>
       <c r="R36" s="34">
         <f t="shared" si="18"/>
-        <v>4.0750000000000002</v>
+        <v>5.5825000000000014</v>
       </c>
       <c r="S36" s="32">
         <f t="shared" si="19"/>
-        <v>0.27166666666666667</v>
+        <v>0.33833333333333337</v>
       </c>
       <c r="U36" s="33">
         <f t="shared" si="0"/>
-        <v>107.8381</v>
+        <v>109.34559999999999</v>
       </c>
       <c r="V36" s="34">
         <f t="shared" si="20"/>
@@ -82315,15 +82318,15 @@
       </c>
       <c r="W36" s="35">
         <f t="shared" si="21"/>
-        <v>3.6350788821390586E-4</v>
+        <v>3.5849636382259551E-4</v>
       </c>
       <c r="X36" s="32">
-        <f t="shared" si="46"/>
-        <v>6.6246867778237783</v>
+        <f t="shared" si="45"/>
+        <v>4.9019911360933941</v>
       </c>
       <c r="Y36" s="33">
         <f t="shared" si="1"/>
-        <v>131.70429999999999</v>
+        <v>133.21179999999998</v>
       </c>
       <c r="Z36" s="34">
         <f t="shared" si="2"/>
@@ -82331,24 +82334,24 @@
       </c>
       <c r="AA36" s="35">
         <f t="shared" si="22"/>
-        <v>1.2398987732367129E-3</v>
+        <v>1.2258673781151521E-3</v>
       </c>
       <c r="AB36" s="32">
         <f t="shared" si="23"/>
-        <v>8.1168959689864124</v>
+        <v>5.9872127227282634</v>
       </c>
       <c r="AC36" s="53">
         <f t="shared" si="90"/>
-        <v>1.0191825812036581</v>
+        <v>0.75415248247590683</v>
       </c>
       <c r="AD36" s="53">
         <f t="shared" si="91"/>
-        <v>1.2487532259979095</v>
+        <v>0.92110964965050202</v>
       </c>
       <c r="AE36" s="36"/>
       <c r="AF36" s="38">
         <f t="shared" si="5"/>
-        <v>134.91399999999999</v>
+        <v>136.42149999999998</v>
       </c>
       <c r="AG36" s="34">
         <f t="shared" si="6"/>
@@ -82356,15 +82359,15 @@
       </c>
       <c r="AH36" s="34">
         <f t="shared" si="24"/>
-        <v>4.3509198452347427E-4</v>
+        <v>4.3028408278753726E-4</v>
       </c>
       <c r="AI36" s="32">
         <f t="shared" si="25"/>
-        <v>8.2901885656215875</v>
+        <v>6.1171069205976609</v>
       </c>
       <c r="AJ36" s="38">
         <f t="shared" si="7"/>
-        <v>80.762199999999993</v>
+        <v>82.269699999999986</v>
       </c>
       <c r="AK36" s="34">
         <f t="shared" si="8"/>
@@ -82372,15 +82375,15 @@
       </c>
       <c r="AL36" s="34">
         <f t="shared" si="26"/>
-        <v>2.439259950818576E-4</v>
+        <v>2.394563247465349E-4</v>
       </c>
       <c r="AM36" s="32">
         <f t="shared" si="27"/>
-        <v>4.9591849900259692</v>
+        <v>3.6868753515891264</v>
       </c>
       <c r="AN36" s="38">
         <f t="shared" si="9"/>
-        <v>146.04467500000001</v>
+        <v>147.55217500000001</v>
       </c>
       <c r="AO36" s="34">
         <f t="shared" si="10"/>
@@ -82388,15 +82391,15 @@
       </c>
       <c r="AP36" s="34">
         <f t="shared" si="28"/>
-        <v>1.005856598331983E-3</v>
+        <v>9.9558003804416984E-4</v>
       </c>
       <c r="AQ36" s="32">
         <f t="shared" si="29"/>
-        <v>8.9929700120441129</v>
+        <v>6.6272441644477471</v>
       </c>
       <c r="AR36" s="38">
         <f t="shared" si="11"/>
-        <v>105.430825</v>
+        <v>106.93832499999999</v>
       </c>
       <c r="AS36" s="34">
         <f t="shared" si="12"/>
@@ -82404,15 +82407,15 @@
       </c>
       <c r="AT36" s="34">
         <f t="shared" si="30"/>
-        <v>1.1158975565258075E-3</v>
+        <v>1.1001668485082407E-3</v>
       </c>
       <c r="AU36" s="32">
         <f t="shared" si="31"/>
-        <v>6.4947173303473971</v>
+        <v>4.8045704876913451</v>
       </c>
       <c r="AV36" s="38">
         <f t="shared" si="13"/>
-        <v>91.778759999999991</v>
+        <v>92.683260000000004</v>
       </c>
       <c r="AW36" s="34">
         <f t="shared" si="14"/>
@@ -82420,15 +82423,15 @@
       </c>
       <c r="AX36" s="34">
         <f t="shared" si="32"/>
-        <v>4.6873590360122544E-4</v>
+        <v>4.6416148935633035E-4</v>
       </c>
       <c r="AY36" s="32">
         <f t="shared" si="33"/>
-        <v>5.6403138544920761</v>
+        <v>4.1563104661603036</v>
       </c>
       <c r="AZ36" s="38">
         <f t="shared" si="15"/>
-        <v>37.626959999999983</v>
+        <v>38.531459999999996</v>
       </c>
       <c r="BA36" s="34">
         <f t="shared" si="16"/>
@@ -82436,23 +82439,23 @@
       </c>
       <c r="BB36" s="34">
         <f t="shared" si="34"/>
-        <v>1.0683828829116147E-4</v>
+        <v>1.0433033163030935E-4</v>
       </c>
       <c r="BC36" s="32">
         <f t="shared" si="35"/>
-        <v>2.309310278896457</v>
+        <v>1.7260788971517687</v>
       </c>
       <c r="BD36" s="37">
         <f t="shared" si="36"/>
-        <v>8.9929700120441129</v>
+        <v>6.6272441644477471</v>
       </c>
       <c r="BE36" s="53">
         <f t="shared" si="17"/>
-        <v>1.0579964720051898</v>
+        <v>0.77967578405267612</v>
       </c>
       <c r="BF36" s="38">
         <f t="shared" si="37"/>
-        <v>11.241212515055141</v>
+        <v>10.023706798727218</v>
       </c>
       <c r="BG36" s="34">
         <f t="shared" si="38"/>
@@ -82460,7 +82463,7 @@
       </c>
       <c r="BH36" s="34">
         <f t="shared" si="39"/>
-        <v>6.7447275090330852</v>
+        <v>6.0142240792363308</v>
       </c>
       <c r="BI36" s="32" t="str">
         <f t="shared" si="40"/>
@@ -82468,7 +82471,7 @@
       </c>
       <c r="BJ36" s="38">
         <f t="shared" si="41"/>
-        <v>4.0468365054198516</v>
+        <v>8.284055205559687</v>
       </c>
       <c r="BK36" s="34">
         <f t="shared" si="42"/>
@@ -82476,7 +82479,7 @@
       </c>
       <c r="BL36" s="34">
         <f t="shared" si="43"/>
-        <v>2.4281019032519113</v>
+        <v>4.9704331233358126</v>
       </c>
       <c r="BM36" s="32" t="str">
         <f t="shared" si="44"/>
@@ -82536,18 +82539,18 @@
         <v>6.4899999999999999E-2</v>
       </c>
       <c r="O37" s="29">
-        <f t="shared" si="45"/>
+        <f t="shared" si="89"/>
         <v>2.9499999999999997</v>
       </c>
       <c r="P37" s="30">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="Q37" s="30">
-        <v>1</v>
+        <v>1.3</v>
       </c>
       <c r="R37" s="34">
         <f t="shared" si="18"/>
-        <v>7.3749999999999991</v>
+        <v>14.381249999999998</v>
       </c>
       <c r="S37" s="32">
         <f t="shared" si="19"/>
@@ -82555,7 +82558,7 @@
       </c>
       <c r="U37" s="33">
         <f t="shared" si="0"/>
-        <v>192.5608</v>
+        <v>199.56704999999999</v>
       </c>
       <c r="V37" s="34">
         <f t="shared" si="20"/>
@@ -82563,15 +82566,15 @@
       </c>
       <c r="W37" s="35">
         <f t="shared" si="21"/>
-        <v>1.3503267539395349E-2</v>
+        <v>1.3029204971461972E-2</v>
       </c>
       <c r="X37" s="32">
-        <f t="shared" si="46"/>
-        <v>6.7067573685722497</v>
+        <f t="shared" si="45"/>
+        <v>4.6295049123814991</v>
       </c>
       <c r="Y37" s="33">
         <f t="shared" si="1"/>
-        <v>233.93709999999999</v>
+        <v>240.94335000000001</v>
       </c>
       <c r="Z37" s="34">
         <f t="shared" si="2"/>
@@ -82579,24 +82582,24 @@
       </c>
       <c r="AA37" s="35">
         <f t="shared" si="22"/>
-        <v>1.0361759635389172E-2</v>
+        <v>1.0060456119664642E-2</v>
       </c>
       <c r="AB37" s="32">
         <f t="shared" si="23"/>
-        <v>8.0971955759839123</v>
+        <v>5.5564637173226092</v>
       </c>
       <c r="AC37" s="53">
         <f t="shared" si="90"/>
-        <v>1.0318088259341922</v>
+        <v>0.71223152498176912</v>
       </c>
       <c r="AD37" s="53">
         <f t="shared" si="91"/>
-        <v>1.2457223963052173</v>
+        <v>0.85484057189578599</v>
       </c>
       <c r="AE37" s="36"/>
       <c r="AF37" s="38">
         <f t="shared" si="5"/>
-        <v>253.07999999999998</v>
+        <v>260.08625000000001</v>
       </c>
       <c r="AG37" s="34">
         <f t="shared" si="6"/>
@@ -82604,15 +82607,15 @@
       </c>
       <c r="AH37" s="34">
         <f t="shared" si="24"/>
-        <v>1.0530662241188558E-2</v>
+        <v>1.0246985375043855E-2</v>
       </c>
       <c r="AI37" s="32">
         <f t="shared" si="25"/>
-        <v>8.7627302499281825</v>
+        <v>6.0001534999521215</v>
       </c>
       <c r="AJ37" s="38">
         <f t="shared" si="7"/>
-        <v>132.04160000000002</v>
+        <v>139.04784999999998</v>
       </c>
       <c r="AK37" s="34">
         <f t="shared" si="8"/>
@@ -82620,15 +82623,15 @@
       </c>
       <c r="AL37" s="34">
         <f t="shared" si="26"/>
-        <v>1.9200767030996289E-2</v>
+        <v>1.8233291633060131E-2</v>
       </c>
       <c r="AM37" s="32">
         <f t="shared" si="27"/>
-        <v>4.6507844872163187</v>
+        <v>3.2588563248108775</v>
       </c>
       <c r="AN37" s="38">
         <f t="shared" si="9"/>
-        <v>268.98242500000003</v>
+        <v>275.988675</v>
       </c>
       <c r="AO37" s="34">
         <f t="shared" si="10"/>
@@ -82636,15 +82639,15 @@
       </c>
       <c r="AP37" s="34">
         <f t="shared" si="28"/>
-        <v>9.3564663193143535E-3</v>
+        <v>9.1189430146001449E-3</v>
       </c>
       <c r="AQ37" s="32">
         <f t="shared" si="29"/>
-        <v>9.2915656851479476</v>
+        <v>6.3527104567652968</v>
       </c>
       <c r="AR37" s="38">
         <f t="shared" si="11"/>
-        <v>178.20362500000002</v>
+        <v>185.20987500000001</v>
       </c>
       <c r="AS37" s="34">
         <f t="shared" si="12"/>
@@ -82652,15 +82655,15 @@
       </c>
       <c r="AT37" s="34">
         <f t="shared" si="30"/>
-        <v>1.3576463441750973E-2</v>
+        <v>1.3062883391071884E-2</v>
       </c>
       <c r="AU37" s="32">
         <f t="shared" si="31"/>
-        <v>6.2076063631140492</v>
+        <v>4.2967375754093649</v>
       </c>
       <c r="AV37" s="38">
         <f t="shared" si="13"/>
-        <v>176.05568</v>
+        <v>180.25943000000001</v>
       </c>
       <c r="AW37" s="34">
         <f t="shared" si="14"/>
@@ -82668,15 +82671,15 @@
       </c>
       <c r="AX37" s="34">
         <f t="shared" si="32"/>
-        <v>9.2301480986015337E-3</v>
+        <v>9.0148959197308004E-3</v>
       </c>
       <c r="AY37" s="32">
         <f t="shared" si="33"/>
-        <v>6.0800273024992828</v>
+        <v>4.1483515349995219</v>
       </c>
       <c r="AZ37" s="38">
         <f t="shared" si="15"/>
-        <v>55.01728</v>
+        <v>59.221029999999999</v>
       </c>
       <c r="BA37" s="34">
         <f t="shared" si="16"/>
@@ -82684,31 +82687,31 @@
       </c>
       <c r="BB37" s="34">
         <f t="shared" si="34"/>
-        <v>2.7177279574708165E-2</v>
+        <v>2.5248125539187684E-2</v>
       </c>
       <c r="BC37" s="32">
         <f t="shared" si="35"/>
-        <v>1.9680815397874174</v>
+        <v>1.4070543598582783</v>
       </c>
       <c r="BD37" s="37">
         <f t="shared" si="36"/>
-        <v>9.2915656851479476</v>
+        <v>6.3527104567652968</v>
       </c>
       <c r="BE37" s="53">
         <f t="shared" si="17"/>
-        <v>1.0931253747232879</v>
+        <v>0.74737770079591725</v>
       </c>
       <c r="BF37" s="38">
         <f t="shared" si="37"/>
-        <v>11.614457106434934</v>
+        <v>17.866998159652397</v>
       </c>
       <c r="BG37" s="34">
         <f t="shared" si="38"/>
-        <v>0.16666666666666666</v>
+        <v>0.28166666666666668</v>
       </c>
       <c r="BH37" s="34">
         <f t="shared" si="39"/>
-        <v>6.9686742638609598</v>
+        <v>6.3433129560896084</v>
       </c>
       <c r="BI37" s="32" t="str">
         <f t="shared" si="40"/>
@@ -82716,15 +82719,15 @@
       </c>
       <c r="BJ37" s="38">
         <f t="shared" si="41"/>
-        <v>4.1812045583165718</v>
+        <v>2.8587197055443805</v>
       </c>
       <c r="BK37" s="34">
         <f t="shared" si="42"/>
-        <v>0.16666666666666666</v>
+        <v>0.28166666666666668</v>
       </c>
       <c r="BL37" s="34">
         <f t="shared" si="43"/>
-        <v>2.5087227349899432</v>
+        <v>1.0149300729743362</v>
       </c>
       <c r="BM37" s="32" t="str">
         <f t="shared" si="44"/>
@@ -82784,18 +82787,18 @@
         <v>0.10290000000000001</v>
       </c>
       <c r="O38" s="29">
-        <f t="shared" si="45"/>
+        <f t="shared" si="89"/>
         <v>3.3099999999999996</v>
       </c>
       <c r="P38" s="30">
-        <v>1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="Q38" s="30">
         <v>1</v>
       </c>
       <c r="R38" s="34">
         <f t="shared" si="18"/>
-        <v>8.2749999999999986</v>
+        <v>9.1024999999999991</v>
       </c>
       <c r="S38" s="32">
         <f t="shared" si="19"/>
@@ -82803,7 +82806,7 @@
       </c>
       <c r="U38" s="33">
         <f t="shared" si="0"/>
-        <v>184.20580000000001</v>
+        <v>185.0333</v>
       </c>
       <c r="V38" s="34">
         <f t="shared" si="20"/>
@@ -82811,15 +82814,15 @@
       </c>
       <c r="W38" s="35">
         <f t="shared" si="21"/>
-        <v>1.0554499369726685E-2</v>
+        <v>1.0507297875571586E-2</v>
       </c>
       <c r="X38" s="32">
-        <f t="shared" si="46"/>
-        <v>5.6716021029380901</v>
+        <f t="shared" si="45"/>
+        <v>5.1787291844891721</v>
       </c>
       <c r="Y38" s="33">
         <f t="shared" si="1"/>
-        <v>224.76850000000002</v>
+        <v>225.596</v>
       </c>
       <c r="Z38" s="34">
         <f t="shared" si="2"/>
@@ -82827,24 +82830,24 @@
       </c>
       <c r="AA38" s="35">
         <f t="shared" si="22"/>
-        <v>8.5145382916200444E-3</v>
+        <v>8.4833064416035744E-3</v>
       </c>
       <c r="AB38" s="32">
         <f t="shared" si="23"/>
-        <v>6.8953964914522512</v>
+        <v>6.2912695376838643</v>
       </c>
       <c r="AC38" s="53">
         <f t="shared" si="90"/>
-        <v>0.8725541696827831</v>
+        <v>0.79672756684448798</v>
       </c>
       <c r="AD38" s="53">
         <f t="shared" si="91"/>
-        <v>1.0608302294541925</v>
+        <v>0.96788762118213301</v>
       </c>
       <c r="AE38" s="36"/>
       <c r="AF38" s="38">
         <f t="shared" si="5"/>
-        <v>206.72250000000003</v>
+        <v>207.55</v>
       </c>
       <c r="AG38" s="34">
         <f t="shared" si="6"/>
@@ -82852,15 +82855,15 @@
       </c>
       <c r="AH38" s="34">
         <f t="shared" si="24"/>
-        <v>9.9026472686814439E-3</v>
+        <v>9.8631655022886049E-3</v>
       </c>
       <c r="AI38" s="32">
         <f t="shared" si="25"/>
-        <v>6.3575001597283718</v>
+        <v>5.8022728724803372</v>
       </c>
       <c r="AJ38" s="38">
         <f t="shared" si="7"/>
-        <v>161.6891</v>
+        <v>162.51659999999998</v>
       </c>
       <c r="AK38" s="34">
         <f t="shared" si="8"/>
@@ -82868,15 +82871,15 @@
       </c>
       <c r="AL38" s="34">
         <f t="shared" si="26"/>
-        <v>1.1387904317607061E-2</v>
+        <v>1.1329919528220503E-2</v>
       </c>
       <c r="AM38" s="32">
         <f t="shared" si="27"/>
-        <v>4.9857040461478084</v>
+        <v>4.555185496498007</v>
       </c>
       <c r="AN38" s="38">
         <f t="shared" si="9"/>
-        <v>231.51535000000001</v>
+        <v>232.34285</v>
       </c>
       <c r="AO38" s="34">
         <f t="shared" si="10"/>
@@ -82884,15 +82887,15 @@
       </c>
       <c r="AP38" s="34">
         <f t="shared" si="28"/>
-        <v>8.6325809498160704E-3</v>
+        <v>8.6018356063033569E-3</v>
       </c>
       <c r="AQ38" s="32">
         <f t="shared" si="29"/>
-        <v>7.1038714369164229</v>
+        <v>6.480792215378564</v>
       </c>
       <c r="AR38" s="38">
         <f t="shared" si="11"/>
-        <v>197.74029999999999</v>
+        <v>198.56779999999998</v>
       </c>
       <c r="AS38" s="34">
         <f t="shared" si="12"/>
@@ -82900,15 +82903,15 @@
       </c>
       <c r="AT38" s="34">
         <f t="shared" si="30"/>
-        <v>9.3265004655095594E-3</v>
+        <v>9.2876337452497352E-3</v>
       </c>
       <c r="AU38" s="32">
         <f t="shared" si="31"/>
-        <v>6.0750243517309999</v>
+        <v>5.5454766833918168</v>
       </c>
       <c r="AV38" s="38">
         <f t="shared" si="13"/>
-        <v>133.04018000000002</v>
+        <v>133.53667999999999</v>
       </c>
       <c r="AW38" s="34">
         <f t="shared" si="14"/>
@@ -82916,15 +82919,15 @@
       </c>
       <c r="AX38" s="34">
         <f t="shared" si="32"/>
-        <v>9.5416287019455311E-3</v>
+        <v>9.5061521673296071E-3</v>
       </c>
       <c r="AY38" s="32">
         <f t="shared" si="33"/>
-        <v>4.0888593185531352</v>
+        <v>3.7307811986846673</v>
       </c>
       <c r="AZ38" s="38">
         <f t="shared" si="15"/>
-        <v>88.006780000000006</v>
+        <v>88.503280000000004</v>
       </c>
       <c r="BA38" s="34">
         <f t="shared" si="16"/>
@@ -82932,23 +82935,23 @@
       </c>
       <c r="BB38" s="34">
         <f t="shared" si="34"/>
-        <v>1.2085659763940914E-2</v>
+        <v>1.2017859677065076E-2</v>
       </c>
       <c r="BC38" s="32">
         <f t="shared" si="35"/>
-        <v>2.7170632049725727</v>
+        <v>2.4836938227023384</v>
       </c>
       <c r="BD38" s="37">
         <f t="shared" si="36"/>
-        <v>7.1038714369164229</v>
+        <v>6.480792215378564</v>
       </c>
       <c r="BE38" s="53">
         <f t="shared" si="17"/>
-        <v>0.83574958081369677</v>
+        <v>0.76244614298571345</v>
       </c>
       <c r="BF38" s="38">
         <f t="shared" si="37"/>
-        <v>8.8798392961455281</v>
+        <v>9.8021982257600797</v>
       </c>
       <c r="BG38" s="34">
         <f t="shared" si="38"/>
@@ -82956,7 +82959,7 @@
       </c>
       <c r="BH38" s="34">
         <f t="shared" si="39"/>
-        <v>5.3279035776873176</v>
+        <v>5.881318935456048</v>
       </c>
       <c r="BI38" s="32" t="str">
         <f t="shared" si="40"/>
@@ -82964,7 +82967,7 @@
       </c>
       <c r="BJ38" s="38">
         <f t="shared" si="41"/>
-        <v>3.1967421466123866</v>
+        <v>2.9163564969203506</v>
       </c>
       <c r="BK38" s="34">
         <f t="shared" si="42"/>
@@ -82972,7 +82975,7 @@
       </c>
       <c r="BL38" s="34">
         <f t="shared" si="43"/>
-        <v>1.9180452879674319</v>
+        <v>1.7498138981522104</v>
       </c>
       <c r="BM38" s="32" t="str">
         <f t="shared" si="44"/>
@@ -83032,7 +83035,7 @@
         <v>0.19570000000000001</v>
       </c>
       <c r="O39" s="29">
-        <f t="shared" si="45"/>
+        <f t="shared" si="89"/>
         <v>3.2199999999999998</v>
       </c>
       <c r="P39" s="30">
@@ -83062,7 +83065,7 @@
         <v>5.2498139329432487E-2</v>
       </c>
       <c r="X39" s="32">
-        <f t="shared" si="46"/>
+        <f t="shared" si="45"/>
         <v>1.1268910535858958</v>
       </c>
       <c r="Y39" s="33">
@@ -83280,7 +83283,7 @@
         <v>0.10100000000000001</v>
       </c>
       <c r="O40" s="29">
-        <f t="shared" si="45"/>
+        <f t="shared" si="89"/>
         <v>1.43</v>
       </c>
       <c r="P40" s="30">
@@ -83528,7 +83531,7 @@
         <v>7.1800000000000003E-2</v>
       </c>
       <c r="O41" s="29">
-        <f t="shared" si="45"/>
+        <f t="shared" si="89"/>
         <v>1.45</v>
       </c>
       <c r="P41" s="30">
@@ -83558,7 +83561,7 @@
         <v>3.6867176349735922E-2</v>
       </c>
       <c r="X41" s="32">
-        <f t="shared" si="46"/>
+        <f t="shared" si="45"/>
         <v>3.4975001189060642</v>
       </c>
       <c r="Y41" s="33">
@@ -83776,26 +83779,26 @@
         <v>9.1999999999999998E-2</v>
       </c>
       <c r="O42" s="29">
-        <f t="shared" si="45"/>
-        <v>5.4499999999999993</v>
+        <f>0.5+E42+0.5</f>
+        <v>5.85</v>
       </c>
       <c r="P42" s="30">
-        <v>1</v>
+        <v>1.2</v>
       </c>
       <c r="Q42" s="30">
-        <v>1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="R42" s="34">
         <f t="shared" si="18"/>
-        <v>13.624999999999998</v>
+        <v>19.305000000000003</v>
       </c>
       <c r="S42" s="32">
         <f t="shared" si="19"/>
-        <v>0.90833333333333321</v>
+        <v>0.97499999999999998</v>
       </c>
       <c r="U42" s="33">
         <f t="shared" si="0"/>
-        <v>354.21050000000002</v>
+        <v>359.89050000000003</v>
       </c>
       <c r="V42" s="34">
         <f t="shared" si="20"/>
@@ -83803,15 +83806,15 @@
       </c>
       <c r="W42" s="35">
         <f t="shared" si="21"/>
-        <v>1.6663537642164758E-2</v>
+        <v>1.6400544054372093E-2</v>
       </c>
       <c r="X42" s="32">
-        <f t="shared" si="46"/>
-        <v>6.6185055971719562</v>
+        <f t="shared" si="45"/>
+        <v>5.2128809628168611</v>
       </c>
       <c r="Y42" s="33">
         <f t="shared" si="1"/>
-        <v>439.24</v>
+        <v>444.92</v>
       </c>
       <c r="Z42" s="34">
         <f t="shared" si="2"/>
@@ -83819,24 +83822,24 @@
       </c>
       <c r="AA42" s="35">
         <f t="shared" si="22"/>
-        <v>1.7349057462890446E-2</v>
+        <v>1.7127573496358895E-2</v>
       </c>
       <c r="AB42" s="32">
         <f t="shared" si="23"/>
-        <v>8.2133840585809299</v>
+        <v>6.4492278471765658</v>
       </c>
       <c r="AC42" s="53">
         <f t="shared" si="90"/>
-        <v>1.0182316303341472</v>
+        <v>0.80198168658720936</v>
       </c>
       <c r="AD42" s="53">
         <f t="shared" si="91"/>
-        <v>1.2635975474739891</v>
+        <v>0.9921888995656255</v>
       </c>
       <c r="AE42" s="36"/>
       <c r="AF42" s="38">
         <f t="shared" si="5"/>
-        <v>463.46250000000003</v>
+        <v>469.14250000000004</v>
       </c>
       <c r="AG42" s="34">
         <f t="shared" si="6"/>
@@ -83844,15 +83847,15 @@
       </c>
       <c r="AH42" s="34">
         <f t="shared" si="24"/>
-        <v>1.2933948269816866E-2</v>
+        <v>1.2777354428558485E-2</v>
       </c>
       <c r="AI42" s="32">
         <f t="shared" si="25"/>
-        <v>8.6249878798080992</v>
+        <v>6.7705214040470469</v>
       </c>
       <c r="AJ42" s="38">
         <f t="shared" si="7"/>
-        <v>244.95850000000002</v>
+        <v>250.63850000000002</v>
       </c>
       <c r="AK42" s="34">
         <f t="shared" si="8"/>
@@ -83860,15 +83863,15 @@
       </c>
       <c r="AL42" s="34">
         <f t="shared" si="26"/>
-        <v>2.3719936234096798E-2</v>
+        <v>2.3182392170396807E-2</v>
       </c>
       <c r="AM42" s="32">
         <f t="shared" si="27"/>
-        <v>4.612023314535814</v>
+        <v>3.6552405215866757</v>
       </c>
       <c r="AN42" s="38">
         <f t="shared" si="9"/>
-        <v>499.92162500000006</v>
+        <v>505.60162500000001</v>
       </c>
       <c r="AO42" s="34">
         <f t="shared" si="10"/>
@@ -83876,15 +83879,15 @@
       </c>
       <c r="AP42" s="34">
         <f t="shared" si="28"/>
-        <v>1.4522076335465582E-2</v>
+        <v>1.4358933280722743E-2</v>
       </c>
       <c r="AQ42" s="32">
         <f t="shared" si="29"/>
-        <v>9.3195261552057929</v>
+        <v>7.3083714570092777</v>
       </c>
       <c r="AR42" s="38">
         <f t="shared" si="11"/>
-        <v>336.04362500000002</v>
+        <v>341.72362500000008</v>
       </c>
       <c r="AS42" s="34">
         <f t="shared" si="12"/>
@@ -83892,15 +83895,15 @@
       </c>
       <c r="AT42" s="34">
         <f t="shared" si="30"/>
-        <v>2.1193379282228607E-2</v>
+        <v>2.0841111000153994E-2</v>
       </c>
       <c r="AU42" s="32">
         <f t="shared" si="31"/>
-        <v>6.3098027312515788</v>
+        <v>4.9719107951640016</v>
       </c>
       <c r="AV42" s="38">
         <f t="shared" si="13"/>
-        <v>321.7783</v>
+        <v>325.18630000000002</v>
       </c>
       <c r="AW42" s="34">
         <f t="shared" si="14"/>
@@ -83908,15 +83911,15 @@
       </c>
       <c r="AX42" s="34">
         <f t="shared" si="32"/>
-        <v>1.1291749630102465E-2</v>
+        <v>1.1173410441952813E-2</v>
       </c>
       <c r="AY42" s="32">
         <f t="shared" si="33"/>
-        <v>5.9775856409393153</v>
+        <v>4.6853690189203014</v>
       </c>
       <c r="AZ42" s="38">
         <f t="shared" si="15"/>
-        <v>103.27430000000003</v>
+        <v>106.68230000000001</v>
       </c>
       <c r="BA42" s="34">
         <f t="shared" si="16"/>
@@ -83924,31 +83927,31 @@
       </c>
       <c r="BB42" s="34">
         <f t="shared" si="34"/>
-        <v>3.3400758949709647E-2</v>
+        <v>3.2333761083141246E-2</v>
       </c>
       <c r="BC42" s="32">
         <f t="shared" si="35"/>
-        <v>1.9646210756670321</v>
+        <v>1.5700881364599315</v>
       </c>
       <c r="BD42" s="37">
         <f t="shared" si="36"/>
-        <v>9.3195261552057929</v>
+        <v>7.3083714570092777</v>
       </c>
       <c r="BE42" s="53">
         <f t="shared" si="17"/>
-        <v>1.0964148417889168</v>
+        <v>0.85980840670697389</v>
       </c>
       <c r="BF42" s="38">
         <f t="shared" si="37"/>
-        <v>11.649407694007241</v>
+        <v>13.1550686226167</v>
       </c>
       <c r="BG42" s="34">
         <f t="shared" si="38"/>
-        <v>0.16666666666666666</v>
+        <v>0.20166666666666669</v>
       </c>
       <c r="BH42" s="34">
         <f t="shared" si="39"/>
-        <v>6.9896446164043455</v>
+        <v>6.5231745236115852</v>
       </c>
       <c r="BI42" s="32" t="str">
         <f t="shared" si="40"/>
@@ -83956,15 +83959,15 @@
       </c>
       <c r="BJ42" s="38">
         <f t="shared" si="41"/>
-        <v>4.1937867698426023</v>
+        <v>9.1354643212615976</v>
       </c>
       <c r="BK42" s="34">
         <f t="shared" si="42"/>
-        <v>0.16666666666666666</v>
+        <v>0.20166666666666669</v>
       </c>
       <c r="BL42" s="34">
         <f t="shared" si="43"/>
-        <v>2.5162720619055614</v>
+        <v>4.5299823080636017</v>
       </c>
       <c r="BM42" s="32" t="str">
         <f t="shared" si="44"/>
@@ -84024,7 +84027,7 @@
         <v>0.21870000000000001</v>
       </c>
       <c r="O43" s="29">
-        <f t="shared" si="45"/>
+        <f t="shared" si="89"/>
         <v>4.5999999999999996</v>
       </c>
       <c r="P43" s="30">
@@ -84054,7 +84057,7 @@
         <v>0.66923470227830106</v>
       </c>
       <c r="X43" s="32">
-        <f t="shared" si="46"/>
+        <f t="shared" si="45"/>
         <v>0.46982882797731573</v>
       </c>
       <c r="Y43" s="33">
@@ -84272,7 +84275,7 @@
         <v>0.42680000000000001</v>
       </c>
       <c r="O44" s="29">
-        <f t="shared" si="45"/>
+        <f t="shared" si="89"/>
         <v>9.2200000000000006</v>
       </c>
       <c r="P44" s="30">
@@ -84302,7 +84305,7 @@
         <v>2.1370102113124494</v>
       </c>
       <c r="X44" s="32">
-        <f t="shared" si="46"/>
+        <f t="shared" si="45"/>
         <v>3.3021190398851301</v>
       </c>
       <c r="Y44" s="33">
@@ -84519,8 +84522,8 @@
         <f>'MUROS EJE Y'!N23</f>
         <v>1.3401000000000001</v>
       </c>
-      <c r="O45" s="45">
-        <f t="shared" si="45"/>
+      <c r="O45" s="91">
+        <f t="shared" si="89"/>
         <v>38.881999999999991</v>
       </c>
       <c r="P45" s="46">
@@ -84550,7 +84553,7 @@
         <v>8.0773735184325055</v>
       </c>
       <c r="X45" s="52">
-        <f t="shared" si="46"/>
+        <f t="shared" si="45"/>
         <v>0.85258874142997843</v>
       </c>
       <c r="Y45" s="63">

</xml_diff>

<commit_message>
Actualizado con sigma 8 y 10
</commit_message>
<xml_diff>
--- a/Tarea 07/muros-fundaciones.xlsx
+++ b/Tarea 07/muros-fundaciones.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E93ADFBB-1A05-4CA4-AC11-347BC853E6AD}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4389524A-13EC-47BE-B63E-B77DF05CB571}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="697" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -647,7 +647,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -663,6 +663,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1119,7 +1125,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="95">
+  <cellXfs count="96">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1313,22 +1319,40 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1370,38 +1394,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -72083,8 +72092,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:R22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -72136,11 +72145,11 @@
       <c r="N2" s="1">
         <v>8</v>
       </c>
-      <c r="O2" s="65" t="s">
+      <c r="O2" s="70" t="s">
         <v>11</v>
       </c>
-      <c r="P2" s="65"/>
-      <c r="Q2" s="65"/>
+      <c r="P2" s="70"/>
+      <c r="Q2" s="70"/>
     </row>
     <row r="3" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B3" s="8"/>
@@ -73321,7 +73330,7 @@
   <dimension ref="B2:R23"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -73373,11 +73382,11 @@
       <c r="N2" s="1">
         <v>8</v>
       </c>
-      <c r="O2" s="65" t="s">
+      <c r="O2" s="70" t="s">
         <v>11</v>
       </c>
-      <c r="P2" s="65"/>
-      <c r="Q2" s="65"/>
+      <c r="P2" s="70"/>
+      <c r="Q2" s="70"/>
     </row>
     <row r="3" spans="2:18" x14ac:dyDescent="0.25">
       <c r="C3" s="2" t="s">
@@ -74620,7 +74629,7 @@
       <pane xSplit="17" ySplit="6" topLeftCell="BD7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="R1" sqref="R1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="O45" sqref="O45"/>
+      <selection pane="bottomRight" activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -74692,79 +74701,79 @@
   <sheetData>
     <row r="1" spans="2:65" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:65" x14ac:dyDescent="0.25">
-      <c r="B2" s="74" t="s">
+      <c r="B2" s="80" t="s">
         <v>133</v>
       </c>
-      <c r="C2" s="75"/>
-      <c r="D2" s="75"/>
+      <c r="C2" s="81"/>
+      <c r="D2" s="81"/>
       <c r="E2" s="17">
-        <v>6.5</v>
+        <v>8</v>
       </c>
       <c r="F2" s="9"/>
     </row>
     <row r="3" spans="2:65" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="76" t="s">
+      <c r="B3" s="82" t="s">
         <v>134</v>
       </c>
-      <c r="C3" s="77"/>
-      <c r="D3" s="77"/>
+      <c r="C3" s="83"/>
+      <c r="D3" s="83"/>
       <c r="E3" s="18">
-        <v>8.5</v>
+        <v>10</v>
       </c>
       <c r="F3" s="9"/>
     </row>
     <row r="4" spans="2:65" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="S4" s="50"/>
-      <c r="U4" s="78" t="s">
+      <c r="U4" s="84" t="s">
         <v>135</v>
       </c>
-      <c r="V4" s="79"/>
-      <c r="W4" s="79"/>
-      <c r="X4" s="79"/>
-      <c r="Y4" s="79"/>
-      <c r="Z4" s="79"/>
-      <c r="AA4" s="79"/>
-      <c r="AB4" s="80"/>
+      <c r="V4" s="85"/>
+      <c r="W4" s="85"/>
+      <c r="X4" s="85"/>
+      <c r="Y4" s="85"/>
+      <c r="Z4" s="85"/>
+      <c r="AA4" s="85"/>
+      <c r="AB4" s="86"/>
       <c r="AC4" s="39"/>
       <c r="AD4" s="39"/>
       <c r="AE4" s="19"/>
-      <c r="AF4" s="81" t="s">
+      <c r="AF4" s="87" t="s">
         <v>136</v>
       </c>
-      <c r="AG4" s="82"/>
-      <c r="AH4" s="82"/>
-      <c r="AI4" s="82"/>
-      <c r="AJ4" s="82"/>
-      <c r="AK4" s="82"/>
-      <c r="AL4" s="82"/>
-      <c r="AM4" s="82"/>
-      <c r="AN4" s="82"/>
-      <c r="AO4" s="82"/>
-      <c r="AP4" s="82"/>
-      <c r="AQ4" s="82"/>
-      <c r="AR4" s="82"/>
-      <c r="AS4" s="82"/>
-      <c r="AT4" s="82"/>
-      <c r="AU4" s="82"/>
-      <c r="AV4" s="82"/>
-      <c r="AW4" s="82"/>
-      <c r="AX4" s="82"/>
-      <c r="AY4" s="82"/>
-      <c r="AZ4" s="82"/>
-      <c r="BA4" s="82"/>
-      <c r="BB4" s="82"/>
-      <c r="BC4" s="82"/>
-      <c r="BD4" s="83"/>
-      <c r="BF4" s="68" t="s">
+      <c r="AG4" s="88"/>
+      <c r="AH4" s="88"/>
+      <c r="AI4" s="88"/>
+      <c r="AJ4" s="88"/>
+      <c r="AK4" s="88"/>
+      <c r="AL4" s="88"/>
+      <c r="AM4" s="88"/>
+      <c r="AN4" s="88"/>
+      <c r="AO4" s="88"/>
+      <c r="AP4" s="88"/>
+      <c r="AQ4" s="88"/>
+      <c r="AR4" s="88"/>
+      <c r="AS4" s="88"/>
+      <c r="AT4" s="88"/>
+      <c r="AU4" s="88"/>
+      <c r="AV4" s="88"/>
+      <c r="AW4" s="88"/>
+      <c r="AX4" s="88"/>
+      <c r="AY4" s="88"/>
+      <c r="AZ4" s="88"/>
+      <c r="BA4" s="88"/>
+      <c r="BB4" s="88"/>
+      <c r="BC4" s="88"/>
+      <c r="BD4" s="89"/>
+      <c r="BF4" s="90" t="s">
         <v>137</v>
       </c>
-      <c r="BG4" s="69"/>
-      <c r="BH4" s="69"/>
-      <c r="BI4" s="69"/>
-      <c r="BJ4" s="69"/>
-      <c r="BK4" s="69"/>
-      <c r="BL4" s="69"/>
-      <c r="BM4" s="70"/>
+      <c r="BG4" s="91"/>
+      <c r="BH4" s="91"/>
+      <c r="BI4" s="91"/>
+      <c r="BJ4" s="91"/>
+      <c r="BK4" s="91"/>
+      <c r="BL4" s="91"/>
+      <c r="BM4" s="92"/>
     </row>
     <row r="5" spans="2:65" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="20"/>
@@ -74772,92 +74781,92 @@
       <c r="D5" s="20"/>
       <c r="E5" s="20"/>
       <c r="F5" s="20"/>
-      <c r="G5" s="84" t="s">
+      <c r="G5" s="71" t="s">
         <v>138</v>
       </c>
-      <c r="H5" s="85"/>
-      <c r="I5" s="85"/>
-      <c r="J5" s="86"/>
-      <c r="K5" s="84" t="s">
+      <c r="H5" s="72"/>
+      <c r="I5" s="72"/>
+      <c r="J5" s="73"/>
+      <c r="K5" s="71" t="s">
         <v>139</v>
       </c>
-      <c r="L5" s="85"/>
-      <c r="M5" s="85"/>
-      <c r="N5" s="86"/>
-      <c r="O5" s="87" t="s">
+      <c r="L5" s="72"/>
+      <c r="M5" s="72"/>
+      <c r="N5" s="73"/>
+      <c r="O5" s="74" t="s">
         <v>11</v>
       </c>
-      <c r="P5" s="88"/>
-      <c r="Q5" s="88"/>
-      <c r="R5" s="88"/>
-      <c r="S5" s="89"/>
+      <c r="P5" s="75"/>
+      <c r="Q5" s="75"/>
+      <c r="R5" s="75"/>
+      <c r="S5" s="76"/>
       <c r="T5" s="7"/>
-      <c r="U5" s="71" t="s">
+      <c r="U5" s="77" t="s">
         <v>140</v>
       </c>
-      <c r="V5" s="72"/>
-      <c r="W5" s="72"/>
-      <c r="X5" s="73"/>
-      <c r="Y5" s="71" t="s">
+      <c r="V5" s="78"/>
+      <c r="W5" s="78"/>
+      <c r="X5" s="79"/>
+      <c r="Y5" s="77" t="s">
         <v>141</v>
       </c>
-      <c r="Z5" s="72"/>
-      <c r="AA5" s="72"/>
-      <c r="AB5" s="73"/>
+      <c r="Z5" s="78"/>
+      <c r="AA5" s="78"/>
+      <c r="AB5" s="79"/>
       <c r="AC5" s="39"/>
       <c r="AD5" s="39"/>
       <c r="AE5" s="19"/>
-      <c r="AF5" s="71" t="s">
+      <c r="AF5" s="77" t="s">
         <v>142</v>
       </c>
-      <c r="AG5" s="72"/>
-      <c r="AH5" s="72"/>
-      <c r="AI5" s="73"/>
-      <c r="AJ5" s="71" t="s">
+      <c r="AG5" s="78"/>
+      <c r="AH5" s="78"/>
+      <c r="AI5" s="79"/>
+      <c r="AJ5" s="77" t="s">
         <v>143</v>
       </c>
-      <c r="AK5" s="72"/>
-      <c r="AL5" s="72"/>
-      <c r="AM5" s="73"/>
-      <c r="AN5" s="71" t="s">
+      <c r="AK5" s="78"/>
+      <c r="AL5" s="78"/>
+      <c r="AM5" s="79"/>
+      <c r="AN5" s="77" t="s">
         <v>144</v>
       </c>
-      <c r="AO5" s="72"/>
-      <c r="AP5" s="72"/>
-      <c r="AQ5" s="73"/>
-      <c r="AR5" s="71" t="s">
+      <c r="AO5" s="78"/>
+      <c r="AP5" s="78"/>
+      <c r="AQ5" s="79"/>
+      <c r="AR5" s="77" t="s">
         <v>145</v>
       </c>
-      <c r="AS5" s="72"/>
-      <c r="AT5" s="72"/>
-      <c r="AU5" s="73"/>
-      <c r="AV5" s="71" t="s">
+      <c r="AS5" s="78"/>
+      <c r="AT5" s="78"/>
+      <c r="AU5" s="79"/>
+      <c r="AV5" s="77" t="s">
         <v>146</v>
       </c>
-      <c r="AW5" s="72"/>
-      <c r="AX5" s="72"/>
-      <c r="AY5" s="73"/>
-      <c r="AZ5" s="71" t="s">
+      <c r="AW5" s="78"/>
+      <c r="AX5" s="78"/>
+      <c r="AY5" s="79"/>
+      <c r="AZ5" s="77" t="s">
         <v>147</v>
       </c>
-      <c r="BA5" s="72"/>
-      <c r="BB5" s="72"/>
-      <c r="BC5" s="73"/>
-      <c r="BD5" s="66" t="s">
+      <c r="BA5" s="78"/>
+      <c r="BB5" s="78"/>
+      <c r="BC5" s="79"/>
+      <c r="BD5" s="93" t="s">
         <v>148</v>
       </c>
-      <c r="BF5" s="68" t="s">
+      <c r="BF5" s="90" t="s">
         <v>196</v>
       </c>
-      <c r="BG5" s="69"/>
-      <c r="BH5" s="69"/>
-      <c r="BI5" s="70"/>
-      <c r="BJ5" s="68" t="s">
+      <c r="BG5" s="91"/>
+      <c r="BH5" s="91"/>
+      <c r="BI5" s="92"/>
+      <c r="BJ5" s="90" t="s">
         <v>195</v>
       </c>
-      <c r="BK5" s="69"/>
-      <c r="BL5" s="69"/>
-      <c r="BM5" s="70"/>
+      <c r="BK5" s="91"/>
+      <c r="BL5" s="91"/>
+      <c r="BM5" s="92"/>
     </row>
     <row r="6" spans="2:65" x14ac:dyDescent="0.25">
       <c r="B6" s="21" t="s">
@@ -74909,7 +74918,7 @@
       <c r="Q6" s="22" t="s">
         <v>160</v>
       </c>
-      <c r="R6" s="94" t="s">
+      <c r="R6" s="69" t="s">
         <v>161</v>
       </c>
       <c r="S6" s="51" t="s">
@@ -74943,10 +74952,10 @@
       <c r="AC6" s="39"/>
       <c r="AD6" s="39"/>
       <c r="AE6" s="19"/>
-      <c r="AF6" s="92" t="s">
+      <c r="AF6" s="67" t="s">
         <v>166</v>
       </c>
-      <c r="AG6" s="93" t="s">
+      <c r="AG6" s="68" t="s">
         <v>167</v>
       </c>
       <c r="AH6" s="27" t="s">
@@ -74955,10 +74964,10 @@
       <c r="AI6" s="28" t="s">
         <v>169</v>
       </c>
-      <c r="AJ6" s="92" t="s">
+      <c r="AJ6" s="67" t="s">
         <v>170</v>
       </c>
-      <c r="AK6" s="93" t="s">
+      <c r="AK6" s="68" t="s">
         <v>171</v>
       </c>
       <c r="AL6" s="27" t="s">
@@ -74967,10 +74976,10 @@
       <c r="AM6" s="28" t="s">
         <v>173</v>
       </c>
-      <c r="AN6" s="92" t="s">
+      <c r="AN6" s="67" t="s">
         <v>174</v>
       </c>
-      <c r="AO6" s="93" t="s">
+      <c r="AO6" s="68" t="s">
         <v>175</v>
       </c>
       <c r="AP6" s="27" t="s">
@@ -74979,10 +74988,10 @@
       <c r="AQ6" s="28" t="s">
         <v>177</v>
       </c>
-      <c r="AR6" s="92" t="s">
+      <c r="AR6" s="67" t="s">
         <v>178</v>
       </c>
-      <c r="AS6" s="93" t="s">
+      <c r="AS6" s="68" t="s">
         <v>179</v>
       </c>
       <c r="AT6" s="27" t="s">
@@ -74991,10 +75000,10 @@
       <c r="AU6" s="28" t="s">
         <v>181</v>
       </c>
-      <c r="AV6" s="92" t="s">
+      <c r="AV6" s="67" t="s">
         <v>182</v>
       </c>
-      <c r="AW6" s="93" t="s">
+      <c r="AW6" s="68" t="s">
         <v>183</v>
       </c>
       <c r="AX6" s="27" t="s">
@@ -75003,10 +75012,10 @@
       <c r="AY6" s="28" t="s">
         <v>185</v>
       </c>
-      <c r="AZ6" s="92" t="s">
+      <c r="AZ6" s="67" t="s">
         <v>186</v>
       </c>
-      <c r="BA6" s="93" t="s">
+      <c r="BA6" s="68" t="s">
         <v>187</v>
       </c>
       <c r="BB6" s="27" t="s">
@@ -75015,8 +75024,8 @@
       <c r="BC6" s="28" t="s">
         <v>189</v>
       </c>
-      <c r="BD6" s="67"/>
-      <c r="BF6" s="92" t="s">
+      <c r="BD6" s="94"/>
+      <c r="BF6" s="67" t="s">
         <v>190</v>
       </c>
       <c r="BG6" s="27" t="s">
@@ -75042,7 +75051,7 @@
       </c>
     </row>
     <row r="7" spans="2:65" x14ac:dyDescent="0.25">
-      <c r="B7" s="29" t="s">
+      <c r="B7" s="95" t="s">
         <v>194</v>
       </c>
       <c r="C7" s="30" t="str">
@@ -75098,14 +75107,14 @@
         <v>2.5199999999999996</v>
       </c>
       <c r="P7" s="30">
-        <v>1</v>
+        <v>0.6</v>
       </c>
       <c r="Q7" s="30">
-        <v>1</v>
+        <v>0.6</v>
       </c>
       <c r="R7" s="34">
         <f>2.5*O7*P7*Q7</f>
-        <v>6.2999999999999989</v>
+        <v>2.2679999999999993</v>
       </c>
       <c r="S7" s="32">
         <f>O7/6</f>
@@ -75113,7 +75122,7 @@
       </c>
       <c r="U7" s="33">
         <f>ABS(R7+ABS(G7))</f>
-        <v>54.757999999999996</v>
+        <v>50.725999999999999</v>
       </c>
       <c r="V7" s="34">
         <f>ABS(K7)</f>
@@ -75121,15 +75130,15 @@
       </c>
       <c r="W7" s="35">
         <f>ABS(V7/U7)</f>
-        <v>2.4997260674239383E-2</v>
+        <v>2.698418956748019E-2</v>
       </c>
       <c r="X7" s="32">
         <f>MAX(IF(W7&lt;$S7,(U7/($P7*$O7))-(6*V7/($P7*$O7^2)),IF(W7=$S7,(2*U7)/($P7*$O7),(2*U7)/($P7*(3*($O7/2-W7))))),IF(W7&lt;$S7,(U7/($P7*$O7))+(6*V7/($P7*$O7^2)),IF(W7=$S7,(2*U7)/($P7*$O7),(2*U7)/($P7*(3*($O7/2-W7))))))/10</f>
-        <v>2.3022637944066515</v>
+        <v>3.5704396573444201</v>
       </c>
       <c r="Y7" s="33">
         <f>ABS(R7+ABS(G7)+ABS(H7))</f>
-        <v>96.814999999999998</v>
+        <v>92.783000000000001</v>
       </c>
       <c r="Z7" s="34">
         <f>ABS(K7+L7)</f>
@@ -75137,24 +75146,24 @@
       </c>
       <c r="AA7" s="35">
         <f>ABS(Z7/Y7)</f>
-        <v>1.6026442183545941E-2</v>
+        <v>1.6722891046851256E-2</v>
       </c>
       <c r="AB7" s="32">
         <f>MAX(IF(AA7&lt;$S7,(Y7/($P7*$O7))-(6*Z7/($P7*$O7^2)),IF(AA7=$S7,(2*Y7)/($P7*$O7),(2*Y7)/($P7*(3*($O7/2-AA7))))),IF(AA7&lt;$S7,(Y7/($P7*$O7))+(6*Z7/($P7*$O7^2)),IF(AA7=$S7,(2*Y7)/($P7*$O7),(2*Y7)/($P7*(3*($O7/2-AA7))))))/10</f>
-        <v>3.9884637188208623</v>
+        <v>6.380772864701437</v>
       </c>
       <c r="AC7" s="53">
         <f>X7/$E$2</f>
-        <v>0.35419442990871564</v>
+        <v>0.44630495716805252</v>
       </c>
       <c r="AD7" s="53">
         <f>AB7/$E$2</f>
-        <v>0.61360980289551725</v>
+        <v>0.79759660808767963</v>
       </c>
       <c r="AE7" s="36"/>
       <c r="AF7" s="38">
         <f>ABS(IF(B7="x",$R7+ABS($G7)+$I7,$R7+ABS($G7)+$J7))</f>
-        <v>55.146299999999997</v>
+        <v>51.1143</v>
       </c>
       <c r="AG7" s="34">
         <f>ABS(IF(B7="x",$K7+$M7,$K7+$N7))</f>
@@ -75162,15 +75171,15 @@
       </c>
       <c r="AH7" s="34">
         <f>ABS(AG7/AF7)</f>
-        <v>2.4250040347221846E-2</v>
+        <v>2.6162932877883488E-2</v>
       </c>
       <c r="AI7" s="32">
         <f>MAX(IF(AH7&lt;$S7,(AF7/($P7*$O7))-(6*AG7/($P7*$O7^2)),IF(AH7=$S7,(2*AF7)/($P7*$O7),(2*AF7)/($P7*(3*($O7/2-AH7))))),IF(AH7&lt;$S7,(AF7/($P7*$O7))+(6*AG7/($P7*$O7^2)),IF(AH7=$S7,(2*AF7)/($P7*$O7),(2*AF7)/($P7*(3*($O7/2-AH7))))))/10</f>
-        <v>2.3146963340891915</v>
+        <v>3.5911605568153191</v>
       </c>
       <c r="AJ7" s="38">
         <f>ABS(IF(B7="x",$R7+ABS($G7)-$I7,$R7+ABS($G7)-$J7))</f>
-        <v>54.369699999999995</v>
+        <v>50.337699999999998</v>
       </c>
       <c r="AK7" s="34">
         <f>ABS(IF(B7="x",$K7-$M7,$K7-$N7))</f>
@@ -75178,15 +75187,15 @@
       </c>
       <c r="AL7" s="34">
         <f>ABS(AK7/AJ7)</f>
-        <v>2.5755154065591684E-2</v>
+        <v>2.7818116441553749E-2</v>
       </c>
       <c r="AM7" s="32">
         <f>MAX(IF(AL7&lt;$S7,(AJ7/($P7*$O7))-(6*AK7/($P7*$O7^2)),IF(AL7=$S7,(2*AJ7)/($P7*$O7),(2*AJ7)/($P7*(3*($O7/2-AL7))))),IF(AL7&lt;$S7,(AJ7/($P7*$O7))+(6*AK7/($P7*$O7^2)),IF(AL7=$S7,(2*AJ7)/($P7*$O7),(2*AJ7)/($P7*(3*($O7/2-AL7))))))/10</f>
-        <v>2.289831254724112</v>
+        <v>3.5497187578735208</v>
       </c>
       <c r="AN7" s="38">
         <f>ABS(IF(B7="x",$R7+ABS($G7)+0.75*ABS($H7)+0.75*$I7,$R7+ABS($G7)+0.75*ABS($H7)+0.75*$J7))</f>
-        <v>86.591974999999991</v>
+        <v>82.559974999999994</v>
       </c>
       <c r="AO7" s="34">
         <f>ABS(IF(B7="x",$K7+0.75*$L7+0.75*$M7,$K7+0.75*$L7+0.75*$N7))</f>
@@ -75194,15 +75203,15 @@
       </c>
       <c r="AP7" s="34">
         <f>ABS(AO7/AN7)</f>
-        <v>1.7117925766215635E-2</v>
+        <v>1.7953917742828774E-2</v>
       </c>
       <c r="AQ7" s="32">
         <f>MAX(IF(AP7&lt;$S7,(AN7/($P7*$O7))-(6*AO7/($P7*$O7^2)),IF(AP7=$S7,(2*AN7)/($P7*$O7),(2*AN7)/($P7*(3*($O7/2-AP7))))),IF(AP7&lt;$S7,(AN7/($P7*$O7))+(6*AO7/($P7*$O7^2)),IF(AP7=$S7,(2*AN7)/($P7*$O7),(2*AN7)/($P7*(3*($O7/2-AP7))))))/10</f>
-        <v>3.5762381424792147</v>
+        <v>5.6937302374653571</v>
       </c>
       <c r="AR7" s="38">
         <f>ABS(IF(B7="x",$R7+ABS($G7)+0.75*ABS($H7)-0.75*$I7,$R7+ABS($G7)+0.75*ABS($H7)-0.75*$J7))</f>
-        <v>86.009524999999996</v>
+        <v>81.977525</v>
       </c>
       <c r="AS7" s="34">
         <f>ABS(IF(B7="x",$K7+0.75*$L7-0.75*$M7,$K7+0.75*$L7-0.75*$N7))</f>
@@ -75210,15 +75219,15 @@
       </c>
       <c r="AT7" s="34">
         <f>ABS(AS7/AR7)</f>
-        <v>1.7783204825279526E-2</v>
+        <v>1.8657857748205987E-2</v>
       </c>
       <c r="AU7" s="32">
         <f>MAX(IF(AT7&lt;$S7,(AR7/($P7*$O7))-(6*AS7/($P7*$O7^2)),IF(AT7=$S7,(2*AR7)/($P7*$O7),(2*AR7)/($P7*(3*($O7/2-AT7))))),IF(AT7&lt;$S7,(AR7/($P7*$O7))+(6*AS7/($P7*$O7^2)),IF(AT7=$S7,(2*AR7)/($P7*$O7),(2*AR7)/($P7*(3*($O7/2-AT7))))))/10</f>
-        <v>3.5575893329554047</v>
+        <v>5.6626488882590085</v>
       </c>
       <c r="AV7" s="38">
         <f>ABS(IF(B7="x",0.6*$R7+0.6*ABS($G7)+$I7,0.6*$R7+0.6*ABS($G7)+$J7))</f>
-        <v>33.243099999999998</v>
+        <v>30.823899999999998</v>
       </c>
       <c r="AW7" s="34">
         <f>ABS(IF(B7="x",0.6*$K7+$M7,0.6*$K7+$N7))</f>
@@ -75226,15 +75235,15 @@
       </c>
       <c r="AX7" s="34">
         <f>ABS(AW7/AV7)</f>
-        <v>2.3757712126727053E-2</v>
+        <v>2.5622325533109051E-2</v>
       </c>
       <c r="AY7" s="32">
         <f>MAX(IF(AX7&lt;$S7,(AV7/($P7*$O7))-(6*AW7/($P7*$O7^2)),IF(AX7=$S7,(2*AV7)/($P7*$O7),(2*AV7)/($P7*(3*($O7/2-AX7))))),IF(AX7&lt;$S7,(AV7/($P7*$O7))+(6*AW7/($P7*$O7^2)),IF(AX7=$S7,(2*AV7)/($P7*$O7),(2*AV7)/($P7*(3*($O7/2-AX7))))))/10</f>
-        <v>1.3937908163265309</v>
+        <v>2.1629846938775512</v>
       </c>
       <c r="AZ7" s="38">
         <f>ABS(IF(B7="x",0.6*$R7+0.6*ABS($G7)-$I7,0.6*$R7+0.6*ABS($G7)-$J7))</f>
-        <v>32.466499999999996</v>
+        <v>30.047299999999996</v>
       </c>
       <c r="BA7" s="34">
         <f>ABS(IF(B7="x",0.6*$K7-$M7,0.6*$K7-$N7))</f>
@@ -75242,31 +75251,31 @@
       </c>
       <c r="BB7" s="34">
         <f>ABS(BA7/AZ7)</f>
-        <v>2.6266459273404898E-2</v>
+        <v>2.8381252225657551E-2</v>
       </c>
       <c r="BC7" s="32">
         <f>MAX(IF(BB7&lt;$S7,(AZ7/($P7*$O7))-(6*BA7/($P7*$O7^2)),IF(BB7=$S7,(2*AZ7)/($P7*$O7),(2*AZ7)/($P7*(3*($O7/2-BB7))))),IF(BB7&lt;$S7,(AZ7/($P7*$O7))+(6*BA7/($P7*$O7^2)),IF(BB7=$S7,(2*AZ7)/($P7*$O7),(2*AZ7)/($P7*(3*($O7/2-BB7))))))/10</f>
-        <v>1.3689257369614514</v>
+        <v>2.121542894935752</v>
       </c>
       <c r="BD7" s="37">
         <f>MAX(AI7,AM7,AQ7,AU7,AY7,BC7)</f>
-        <v>3.5762381424792147</v>
+        <v>5.6937302374653571</v>
       </c>
       <c r="BE7" s="53">
         <f>(BD7)/$E$3</f>
-        <v>0.4207338991152017</v>
+        <v>0.56937302374653576</v>
       </c>
       <c r="BF7" s="38">
         <f>($BD7*10*($P7/2)^2*1)/2</f>
-        <v>4.4702976780990182</v>
+        <v>2.5621786068594106</v>
       </c>
       <c r="BG7" s="34">
         <f>($Q7^2*1)/6</f>
-        <v>0.16666666666666666</v>
+        <v>0.06</v>
       </c>
       <c r="BH7" s="34">
         <f>BF7/BG7/10</f>
-        <v>2.6821786068594111</v>
+        <v>4.2702976780990181</v>
       </c>
       <c r="BI7" s="32" t="str">
         <f>IF(BH7&lt;7,"NO PARRILLA","PARRILLA")</f>
@@ -75274,15 +75283,15 @@
       </c>
       <c r="BJ7" s="38">
         <f>($BD7*10*((O7-E7)/2)^2*1)/2</f>
-        <v>1.6093071641156447</v>
+        <v>2.5621786068594079</v>
       </c>
       <c r="BK7" s="34">
         <f>($Q7^2*1)/6</f>
-        <v>0.16666666666666666</v>
+        <v>0.06</v>
       </c>
       <c r="BL7" s="34">
         <f>BJ7/BK7/10</f>
-        <v>0.96558429846938698</v>
+        <v>4.2702976780990136</v>
       </c>
       <c r="BM7" s="32" t="str">
         <f>IF(BL7&lt;7,"NO PARRILLA","PARRILLA")</f>
@@ -75290,7 +75299,7 @@
       </c>
     </row>
     <row r="8" spans="2:65" x14ac:dyDescent="0.25">
-      <c r="B8" s="29" t="s">
+      <c r="B8" s="95" t="s">
         <v>194</v>
       </c>
       <c r="C8" s="30" t="str">
@@ -75342,26 +75351,26 @@
         <v>0.2382</v>
       </c>
       <c r="O8" s="29">
-        <f>1.1+E8+1.1</f>
-        <v>4.12</v>
+        <f>0.6+E8+0.6</f>
+        <v>3.12</v>
       </c>
       <c r="P8" s="30">
         <v>1.2</v>
       </c>
       <c r="Q8" s="30">
-        <v>2</v>
+        <v>1.3</v>
       </c>
       <c r="R8" s="34">
         <f>2.5*O8*P8*Q8</f>
-        <v>24.720000000000002</v>
+        <v>12.168000000000003</v>
       </c>
       <c r="S8" s="32">
         <f>O8/6</f>
-        <v>0.68666666666666665</v>
+        <v>0.52</v>
       </c>
       <c r="U8" s="33">
         <f t="shared" ref="U8:U45" si="0">ABS(R8+ABS(G8))</f>
-        <v>232.7782</v>
+        <v>220.22620000000001</v>
       </c>
       <c r="V8" s="34">
         <f>ABS(K8)</f>
@@ -75369,15 +75378,15 @@
       </c>
       <c r="W8" s="35">
         <f>ABS(V8/U8)</f>
-        <v>9.5713430209529941E-3</v>
+        <v>1.0116870744716115E-2</v>
       </c>
       <c r="X8" s="32">
         <f>MAX(IF(W8&lt;$S8,(U8/($P8*$O8))-(6*V8/($P8*$O8^2)),IF(W8=$S8,(2*U8)/($P8*$O8),(2*U8)/($P8*(3*($O8/2-W8))))),IF(W8&lt;$S8,(U8/($P8*$O8))+(6*V8/($P8*$O8^2)),IF(W8=$S8,(2*U8)/($P8*$O8),(2*U8)/($P8*(3*($O8/2-W8))))))/10</f>
-        <v>4.7739251657397812</v>
+        <v>5.9965495562130178</v>
       </c>
       <c r="Y8" s="33">
         <f t="shared" ref="Y8:Y45" si="1">ABS(R8+ABS(G8)+ABS(H8))</f>
-        <v>289.90879999999999</v>
+        <v>277.35680000000002</v>
       </c>
       <c r="Z8" s="34">
         <f t="shared" ref="Z8:Z45" si="2">ABS(K8+L8)</f>
@@ -75385,24 +75394,24 @@
       </c>
       <c r="AA8" s="35">
         <f>ABS(Z8/Y8)</f>
-        <v>9.265327578879979E-3</v>
+        <v>9.6846372614624917E-3</v>
       </c>
       <c r="AB8" s="32">
         <f>MAX(IF(AA8&lt;$S8,(Y8/($P8*$O8))-(6*Z8/($P8*$O8^2)),IF(AA8=$S8,(2*Y8)/($P8*$O8),(2*Y8)/($P8*(3*($O8/2-AA8))))),IF(AA8&lt;$S8,(Y8/($P8*$O8))+(6*Z8/($P8*$O8^2)),IF(AA8=$S8,(2*Y8)/($P8*$O8),(2*Y8)/($P8*(3*($O8/2-AA8))))))/10</f>
-        <v>5.9429732224212142</v>
+        <v>7.5460036571334657</v>
       </c>
       <c r="AC8" s="53">
         <f t="shared" ref="AC8:AC13" si="3">X8/$E$2</f>
-        <v>0.73445002549842786</v>
+        <v>0.74956869452662722</v>
       </c>
       <c r="AD8" s="53">
         <f t="shared" ref="AD8:AD13" si="4">AB8/$E$2</f>
-        <v>0.9143035726801868</v>
+        <v>0.94325045714168321</v>
       </c>
       <c r="AE8" s="36"/>
       <c r="AF8" s="38">
         <f t="shared" ref="AF8:AF45" si="5">ABS(IF(B8="x",$R8+ABS($G8)+$I8,$R8+ABS($G8)+$J8))</f>
-        <v>368.14030000000002</v>
+        <v>355.5883</v>
       </c>
       <c r="AG8" s="34">
         <f t="shared" ref="AG8:AG45" si="6">ABS(IF(B8="x",$K8+$M8,$K8+$N8))</f>
@@ -75410,15 +75419,15 @@
       </c>
       <c r="AH8" s="34">
         <f>ABS(AG8/AF8)</f>
-        <v>5.6592554523370578E-3</v>
+        <v>5.8590229206079052E-3</v>
       </c>
       <c r="AI8" s="32">
         <f>MAX(IF(AH8&lt;$S8,(AF8/($P8*$O8))-(6*AG8/($P8*$O8^2)),IF(AH8=$S8,(2*AF8)/($P8*$O8),(2*AF8)/($P8*(3*($O8/2-AH8))))),IF(AH8&lt;$S8,(AF8/($P8*$O8))+(6*AG8/($P8*$O8^2)),IF(AH8=$S8,(2*AF8)/($P8*$O8),(2*AF8)/($P8*(3*($O8/2-AH8))))))/10</f>
-        <v>7.5075723638734413</v>
+        <v>9.6045629930966463</v>
       </c>
       <c r="AJ8" s="38">
         <f t="shared" ref="AJ8:AJ45" si="7">ABS(IF(B8="x",$R8+ABS($G8)-$I8,$R8+ABS($G8)-$J8))</f>
-        <v>97.4161</v>
+        <v>84.864100000000008</v>
       </c>
       <c r="AK8" s="34">
         <f t="shared" ref="AK8:AK45" si="8">ABS(IF(B8="x",$K8-$M8,$K8-$N8))</f>
@@ -75426,15 +75435,15 @@
       </c>
       <c r="AL8" s="34">
         <f>ABS(AK8/AJ8)</f>
-        <v>2.4355317036916898E-2</v>
+        <v>2.7957640509944724E-2</v>
       </c>
       <c r="AM8" s="32">
         <f>MAX(IF(AL8&lt;$S8,(AJ8/($P8*$O8))-(6*AK8/($P8*$O8^2)),IF(AL8=$S8,(2*AJ8)/($P8*$O8),(2*AJ8)/($P8*(3*($O8/2-AL8))))),IF(AL8&lt;$S8,(AJ8/($P8*$O8))+(6*AK8/($P8*$O8^2)),IF(AL8=$S8,(2*AJ8)/($P8*$O8),(2*AJ8)/($P8*(3*($O8/2-AL8))))))/10</f>
-        <v>2.0402779676061207</v>
+        <v>2.3885361193293888</v>
       </c>
       <c r="AN8" s="38">
         <f t="shared" ref="AN8:AN45" si="9">ABS(IF(B8="x",$R8+ABS($G8)+0.75*ABS($H8)+0.75*$I8,$R8+ABS($G8)+0.75*ABS($H8)+0.75*$J8))</f>
-        <v>377.14772499999998</v>
+        <v>364.59572500000002</v>
       </c>
       <c r="AO8" s="34">
         <f t="shared" ref="AO8:AO45" si="10">ABS(IF(B8="x",$K8+0.75*$L8+0.75*$M8,$K8+0.75*$L8+0.75*$N8))</f>
@@ -75442,15 +75451,15 @@
       </c>
       <c r="AP8" s="34">
         <f>ABS(AO8/AN8)</f>
-        <v>6.5309289615892562E-3</v>
+        <v>6.7557703810158503E-3</v>
       </c>
       <c r="AQ8" s="32">
         <f>MAX(IF(AP8&lt;$S8,(AN8/($P8*$O8))-(6*AO8/($P8*$O8^2)),IF(AP8=$S8,(2*AN8)/($P8*$O8),(2*AN8)/($P8*(3*($O8/2-AP8))))),IF(AP8&lt;$S8,(AN8/($P8*$O8))+(6*AO8/($P8*$O8^2)),IF(AP8=$S8,(2*AN8)/($P8*$O8),(2*AN8)/($P8*(3*($O8/2-AP8))))))/10</f>
-        <v>7.7009466068511001</v>
+        <v>9.8646502095660757</v>
       </c>
       <c r="AR8" s="38">
         <f t="shared" ref="AR8:AR45" si="11">ABS(IF(B8="x",$R8+ABS($G8)+0.75*ABS($H8)-0.75*$I8,$R8+ABS($G8)+0.75*ABS($H8)-0.75*$J8))</f>
-        <v>174.10457500000001</v>
+        <v>161.55257500000005</v>
       </c>
       <c r="AS8" s="34">
         <f t="shared" ref="AS8:AS45" si="12">ABS(IF(B8="x",$K8+0.75*$L8-0.75*$M8,$K8+0.75*$L8-0.75*$N8))</f>
@@ -75458,15 +75467,15 @@
       </c>
       <c r="AT8" s="34">
         <f>ABS(AS8/AR8)</f>
-        <v>1.5393191132398445E-2</v>
+        <v>1.6589181571386277E-2</v>
       </c>
       <c r="AU8" s="32">
         <f>MAX(IF(AT8&lt;$S8,(AR8/($P8*$O8))-(6*AS8/($P8*$O8^2)),IF(AT8=$S8,(2*AR8)/($P8*$O8),(2*AR8)/($P8*(3*($O8/2-AT8))))),IF(AT8&lt;$S8,(AR8/($P8*$O8))+(6*AS8/($P8*$O8^2)),IF(AT8=$S8,(2*AR8)/($P8*$O8),(2*AR8)/($P8*(3*($O8/2-AT8))))))/10</f>
-        <v>3.6004758096506118</v>
+        <v>4.4526300542406325</v>
       </c>
       <c r="AV8" s="38">
         <f t="shared" ref="AV8:AV45" si="13">ABS(IF(B8="x",0.6*$R8+0.6*ABS($G8)+$I8,0.6*$R8+0.6*ABS($G8)+$J8))</f>
-        <v>275.02902</v>
+        <v>267.49781999999999</v>
       </c>
       <c r="AW8" s="34">
         <f t="shared" ref="AW8:AW45" si="14">ABS(IF(B8="x",0.6*$K8+$M8,0.6*$K8+$N8))</f>
@@ -75474,15 +75483,15 @@
       </c>
       <c r="AX8" s="34">
         <f>ABS(AW8/AV8)</f>
-        <v>4.3348152860378146E-3</v>
+        <v>4.4568587512227205E-3</v>
       </c>
       <c r="AY8" s="32">
         <f>MAX(IF(AX8&lt;$S8,(AV8/($P8*$O8))-(6*AW8/($P8*$O8^2)),IF(AX8=$S8,(2*AV8)/($P8*$O8),(2*AV8)/($P8*(3*($O8/2-AX8))))),IF(AX8&lt;$S8,(AV8/($P8*$O8))+(6*AW8/($P8*$O8^2)),IF(AX8=$S8,(2*AV8)/($P8*$O8),(2*AV8)/($P8*(3*($O8/2-AX8))))))/10</f>
-        <v>5.598002297577529</v>
+        <v>7.2059431706114392</v>
       </c>
       <c r="AZ8" s="38">
         <f t="shared" ref="AZ8:AZ45" si="15">ABS(IF(B8="x",0.6*$R8+0.6*ABS($G8)-$I8,0.6*$R8+0.6*ABS($G8)-$J8))</f>
-        <v>4.3048200000000065</v>
+        <v>3.226380000000006</v>
       </c>
       <c r="BA8" s="34">
         <f t="shared" ref="BA8:BA45" si="16">ABS(IF(B8="x",0.6*$K8-$M8,0.6*$K8-$N8))</f>
@@ -75490,31 +75499,31 @@
       </c>
       <c r="BB8" s="34">
         <f>ABS(BA8/AZ8)</f>
-        <v>0.34412588679665995</v>
+        <v>0.45915236270990933</v>
       </c>
       <c r="BC8" s="32">
         <f>MAX(IF(BB8&lt;$S8,(AZ8/($P8*$O8))-(6*BA8/($P8*$O8^2)),IF(BB8=$S8,(2*AZ8)/($P8*$O8),(2*AZ8)/($P8*(3*($O8/2-BB8))))),IF(BB8&lt;$S8,(AZ8/($P8*$O8))+(6*BA8/($P8*$O8^2)),IF(BB8=$S8,(2*AZ8)/($P8*$O8),(2*AZ8)/($P8*(3*($O8/2-BB8))))))/10</f>
-        <v>0.13070790131020843</v>
+        <v>0.16226565581854061</v>
       </c>
       <c r="BD8" s="37">
         <f>MAX(AI8,AM8,AQ8,AU8,AY8,BC8)</f>
-        <v>7.7009466068511001</v>
+        <v>9.8646502095660757</v>
       </c>
       <c r="BE8" s="53">
         <f t="shared" ref="BE8:BE45" si="17">(BD8)/$E$3</f>
-        <v>0.90599371845307064</v>
+        <v>0.9864650209566076</v>
       </c>
       <c r="BF8" s="38">
         <f>($BD8*10*($P8/2)^2*1)/2</f>
-        <v>13.861703892331979</v>
+        <v>17.756370377218936</v>
       </c>
       <c r="BG8" s="34">
         <f>($Q8^2*1)/6</f>
-        <v>0.66666666666666663</v>
+        <v>0.28166666666666668</v>
       </c>
       <c r="BH8" s="34">
         <f>BF8/BG8/10</f>
-        <v>2.0792555838497973</v>
+        <v>6.3040368203144146</v>
       </c>
       <c r="BI8" s="32" t="str">
         <f>IF(BH8&lt;7,"NO PARRILLA","PARRILLA")</f>
@@ -75522,15 +75531,15 @@
       </c>
       <c r="BJ8" s="38">
         <f>($BD8*10*((O8-E8)/2)^2*1)/2</f>
-        <v>46.590726971449165</v>
+        <v>17.756370377218943</v>
       </c>
       <c r="BK8" s="34">
         <f>($Q8^2*1)/6</f>
-        <v>0.66666666666666663</v>
+        <v>0.28166666666666668</v>
       </c>
       <c r="BL8" s="34">
         <f>BJ8/BK8/10</f>
-        <v>6.9886090457173751</v>
+        <v>6.3040368203144173</v>
       </c>
       <c r="BM8" s="32" t="str">
         <f>IF(BL8&lt;7,"NO PARRILLA","PARRILLA")</f>
@@ -75538,7 +75547,7 @@
       </c>
     </row>
     <row r="9" spans="2:65" x14ac:dyDescent="0.25">
-      <c r="B9" s="29" t="s">
+      <c r="B9" s="95" t="s">
         <v>194</v>
       </c>
       <c r="C9" s="30" t="str">
@@ -75594,14 +75603,14 @@
         <v>6.05</v>
       </c>
       <c r="P9" s="30">
-        <v>1.6</v>
+        <v>1.4</v>
       </c>
       <c r="Q9" s="30">
-        <v>1.7</v>
+        <v>1.4</v>
       </c>
       <c r="R9" s="34">
         <f t="shared" ref="R9:R45" si="18">2.5*O9*P9*Q9</f>
-        <v>41.14</v>
+        <v>29.644999999999992</v>
       </c>
       <c r="S9" s="32">
         <f t="shared" ref="S9:S45" si="19">O9/6</f>
@@ -75609,7 +75618,7 @@
       </c>
       <c r="U9" s="33">
         <f t="shared" si="0"/>
-        <v>484.27769999999998</v>
+        <v>472.78269999999998</v>
       </c>
       <c r="V9" s="34">
         <f t="shared" ref="V9:V45" si="20">ABS(K9)</f>
@@ -75617,15 +75626,15 @@
       </c>
       <c r="W9" s="35">
         <f t="shared" ref="W9:W45" si="21">ABS(V9/U9)</f>
-        <v>9.0741324657319551E-3</v>
+        <v>9.29475634366486E-3</v>
       </c>
       <c r="X9" s="32">
         <f>MAX(IF(W9&lt;$S9,(U9/($P9*$O9))-(6*V9/($P9*$O9^2)),IF(W9=$S9,(2*U9)/($P9*$O9),(2*U9)/($P9*(3*($O9/2-W9))))),IF(W9&lt;$S9,(U9/($P9*$O9))+(6*V9/($P9*$O9^2)),IF(W9=$S9,(2*U9)/($P9*$O9),(2*U9)/($P9*(3*($O9/2-W9))))))/10</f>
-        <v>5.0478903165767361</v>
+        <v>5.6333032189448424</v>
       </c>
       <c r="Y9" s="33">
         <f t="shared" si="1"/>
-        <v>596.16009999999994</v>
+        <v>584.66509999999994</v>
       </c>
       <c r="Z9" s="34">
         <f t="shared" si="2"/>
@@ -75633,24 +75642,24 @@
       </c>
       <c r="AA9" s="35">
         <f t="shared" ref="AA9:AA45" si="22">ABS(Z9/Y9)</f>
-        <v>7.4115996692834694E-3</v>
+        <v>7.5573178559828532E-3</v>
       </c>
       <c r="AB9" s="32">
         <f t="shared" ref="AB9:AB45" si="23">MAX(IF(AA9&lt;$S9,(Y9/($P9*$O9))-(6*Z9/($P9*$O9^2)),IF(AA9=$S9,(2*Y9)/($P9*$O9),(2*Y9)/($P9*(3*($O9/2-AA9))))),IF(AA9&lt;$S9,(Y9/($P9*$O9))+(6*Z9/($P9*$O9^2)),IF(AA9=$S9,(2*Y9)/($P9*$O9),(2*Y9)/($P9*(3*($O9/2-AA9))))))/10</f>
-        <v>6.2039471432962223</v>
+        <v>6.954511020909969</v>
       </c>
       <c r="AC9" s="53">
         <f t="shared" si="3"/>
-        <v>0.77659851024257476</v>
+        <v>0.7041629023681053</v>
       </c>
       <c r="AD9" s="53">
         <f t="shared" si="4"/>
-        <v>0.95445340666095724</v>
+        <v>0.86931387761374612</v>
       </c>
       <c r="AE9" s="36"/>
       <c r="AF9" s="38">
         <f t="shared" si="5"/>
-        <v>777.149</v>
+        <v>765.654</v>
       </c>
       <c r="AG9" s="34">
         <f t="shared" si="6"/>
@@ -75658,15 +75667,15 @@
       </c>
       <c r="AH9" s="34">
         <f t="shared" ref="AH9:AH45" si="24">ABS(AG9/AF9)</f>
-        <v>5.3592039621745639E-3</v>
+        <v>5.4396633466291568E-3</v>
       </c>
       <c r="AI9" s="32">
         <f t="shared" ref="AI9:AI45" si="25">MAX(IF(AH9&lt;$S9,(AF9/($P9*$O9))-(6*AG9/($P9*$O9^2)),IF(AH9=$S9,(2*AF9)/($P9*$O9),(2*AF9)/($P9*(3*($O9/2-AH9))))),IF(AH9&lt;$S9,(AF9/($P9*$O9))+(6*AG9/($P9*$O9^2)),IF(AH9=$S9,(2*AF9)/($P9*$O9),(2*AF9)/($P9*(3*($O9/2-AH9))))))/10</f>
-        <v>8.0710690014343278</v>
+        <v>9.0883645730678051</v>
       </c>
       <c r="AJ9" s="38">
         <f t="shared" si="7"/>
-        <v>191.40639999999996</v>
+        <v>179.91139999999996</v>
       </c>
       <c r="AK9" s="34">
         <f t="shared" si="8"/>
@@ -75674,15 +75683,15 @@
       </c>
       <c r="AL9" s="34">
         <f t="shared" ref="AL9:AL45" si="26">ABS(AK9/AJ9)</f>
-        <v>2.4157499435755549E-2</v>
+        <v>2.5700983928756048E-2</v>
       </c>
       <c r="AM9" s="32">
         <f t="shared" ref="AM9:AM45" si="27">MAX(IF(AL9&lt;$S9,(AJ9/($P9*$O9))-(6*AK9/($P9*$O9^2)),IF(AL9=$S9,(2*AJ9)/($P9*$O9),(2*AJ9)/($P9*(3*($O9/2-AL9))))),IF(AL9&lt;$S9,(AJ9/($P9*$O9))+(6*AK9/($P9*$O9^2)),IF(AL9=$S9,(2*AJ9)/($P9*$O9),(2*AJ9)/($P9*(3*($O9/2-AL9))))))/10</f>
-        <v>2.0247116317191445</v>
+        <v>2.1782418648218798</v>
       </c>
       <c r="AN9" s="38">
         <f t="shared" si="9"/>
-        <v>787.84297500000002</v>
+        <v>776.34797499999991</v>
       </c>
       <c r="AO9" s="34">
         <f t="shared" si="10"/>
@@ -75690,15 +75699,15 @@
       </c>
       <c r="AP9" s="34">
         <f t="shared" ref="AP9:AP45" si="28">ABS(AO9/AN9)</f>
-        <v>5.3822273404164067E-3</v>
+        <v>5.4619193152400502E-3</v>
       </c>
       <c r="AQ9" s="32">
         <f t="shared" ref="AQ9:AQ45" si="29">MAX(IF(AP9&lt;$S9,(AN9/($P9*$O9))-(6*AO9/($P9*$O9^2)),IF(AP9=$S9,(2*AN9)/($P9*$O9),(2*AN9)/($P9*(3*($O9/2-AP9))))),IF(AP9&lt;$S9,(AN9/($P9*$O9))+(6*AO9/($P9*$O9^2)),IF(AP9=$S9,(2*AN9)/($P9*$O9),(2*AN9)/($P9*(3*($O9/2-AP9))))))/10</f>
-        <v>8.1823169502595459</v>
+        <v>9.2155050860109089</v>
       </c>
       <c r="AR9" s="38">
         <f t="shared" si="11"/>
-        <v>348.53602499999994</v>
+        <v>337.04102499999993</v>
       </c>
       <c r="AS9" s="34">
         <f t="shared" si="12"/>
@@ -75706,15 +75715,15 @@
       </c>
       <c r="AT9" s="34">
         <f t="shared" ref="AT9:AT45" si="30">ABS(AS9/AR9)</f>
-        <v>1.3153876991625187E-2</v>
+        <v>1.3602498390218227E-2</v>
       </c>
       <c r="AU9" s="32">
         <f t="shared" ref="AU9:AU45" si="31">MAX(IF(AT9&lt;$S9,(AR9/($P9*$O9))-(6*AS9/($P9*$O9^2)),IF(AT9=$S9,(2*AR9)/($P9*$O9),(2*AR9)/($P9*(3*($O9/2-AT9))))),IF(AT9&lt;$S9,(AR9/($P9*$O9))+(6*AS9/($P9*$O9^2)),IF(AT9=$S9,(2*AR9)/($P9*$O9),(2*AR9)/($P9*(3*($O9/2-AT9))))))/10</f>
-        <v>3.647548922973157</v>
+        <v>4.0329130548264649</v>
       </c>
       <c r="AV9" s="38">
         <f t="shared" si="13"/>
-        <v>583.43792000000008</v>
+        <v>576.54091999999991</v>
       </c>
       <c r="AW9" s="34">
         <f t="shared" si="14"/>
@@ -75722,15 +75731,15 @@
       </c>
       <c r="AX9" s="34">
         <f t="shared" ref="AX9:AX45" si="32">ABS(AW9/AV9)</f>
-        <v>4.1257859962204714E-3</v>
+        <v>4.1751416360871667E-3</v>
       </c>
       <c r="AY9" s="32">
         <f t="shared" ref="AY9:AY45" si="33">MAX(IF(AX9&lt;$S9,(AV9/($P9*$O9))-(6*AW9/($P9*$O9^2)),IF(AX9=$S9,(2*AV9)/($P9*$O9),(2*AV9)/($P9*(3*($O9/2-AX9))))),IF(AX9&lt;$S9,(AV9/($P9*$O9))+(6*AW9/($P9*$O9^2)),IF(AX9=$S9,(2*AV9)/($P9*$O9),(2*AV9)/($P9*(3*($O9/2-AX9))))))/10</f>
-        <v>6.0519128748036346</v>
+        <v>6.8350432854898671</v>
       </c>
       <c r="AZ9" s="38">
         <f t="shared" si="15"/>
-        <v>2.3046800000000189</v>
+        <v>9.2016800000000671</v>
       </c>
       <c r="BA9" s="34">
         <f t="shared" si="16"/>
@@ -75738,31 +75747,31 @@
       </c>
       <c r="BB9" s="34">
         <f t="shared" ref="BB9:BB45" si="34">ABS(BA9/AZ9)</f>
-        <v>1.2436173351614872</v>
+        <v>0.31148007755105361</v>
       </c>
       <c r="BC9" s="32">
         <f t="shared" ref="BC9:BC45" si="35">MAX(IF(BB9&lt;$S9,(AZ9/($P9*$O9))-(6*BA9/($P9*$O9^2)),IF(BB9=$S9,(2*AZ9)/($P9*$O9),(2*AZ9)/($P9*(3*($O9/2-BB9))))),IF(BB9&lt;$S9,(AZ9/($P9*$O9))+(6*BA9/($P9*$O9^2)),IF(BB9=$S9,(2*AZ9)/($P9*$O9),(2*AZ9)/($P9*(3*($O9/2-BB9))))))/10</f>
-        <v>5.3906628389717361E-2</v>
+        <v>0.14219755481183061</v>
       </c>
       <c r="BD9" s="37">
         <f t="shared" ref="BD9:BD45" si="36">MAX(AI9,AM9,AQ9,AU9,AY9,BC9)</f>
-        <v>8.1823169502595459</v>
+        <v>9.2155050860109089</v>
       </c>
       <c r="BE9" s="53">
         <f t="shared" si="17"/>
-        <v>0.96262552355994657</v>
+        <v>0.92155050860109089</v>
       </c>
       <c r="BF9" s="38">
         <f t="shared" ref="BF9:BF45" si="37">($BD9*10*($P9/2)^2*1)/2</f>
-        <v>26.183414240830555</v>
+        <v>22.577987460726725</v>
       </c>
       <c r="BG9" s="34">
         <f t="shared" ref="BG9:BG45" si="38">($Q9^2*1)/6</f>
-        <v>0.48166666666666663</v>
+        <v>0.32666666666666661</v>
       </c>
       <c r="BH9" s="34">
         <f t="shared" ref="BH9:BH45" si="39">BF9/BG9/10</f>
-        <v>5.4360029565738177</v>
+        <v>6.9116288145081821</v>
       </c>
       <c r="BI9" s="32" t="str">
         <f t="shared" ref="BI9:BI45" si="40">IF(BH9&lt;7,"NO PARRILLA","PARRILLA")</f>
@@ -75770,15 +75779,15 @@
       </c>
       <c r="BJ9" s="38">
         <f t="shared" ref="BJ9:BJ45" si="41">($BD9*10*((O9-E9)/2)^2*1)/2</f>
-        <v>10.227896187824433</v>
+        <v>11.519381357513636</v>
       </c>
       <c r="BK9" s="34">
         <f t="shared" ref="BK9:BK45" si="42">($Q9^2*1)/6</f>
-        <v>0.48166666666666663</v>
+        <v>0.32666666666666661</v>
       </c>
       <c r="BL9" s="34">
         <f t="shared" ref="BL9:BL45" si="43">BJ9/BK9/10</f>
-        <v>2.1234386549116473</v>
+        <v>3.5263412318919301</v>
       </c>
       <c r="BM9" s="32" t="str">
         <f t="shared" ref="BM9:BM45" si="44">IF(BL9&lt;7,"NO PARRILLA","PARRILLA")</f>
@@ -75786,7 +75795,7 @@
       </c>
     </row>
     <row r="10" spans="2:65" x14ac:dyDescent="0.25">
-      <c r="B10" s="29" t="s">
+      <c r="B10" s="95" t="s">
         <v>194</v>
       </c>
       <c r="C10" s="30" t="str">
@@ -75838,26 +75847,26 @@
         <v>0.44340000000000002</v>
       </c>
       <c r="O10" s="29">
-        <f>0.55+E10+0.55</f>
-        <v>7.8599999999999994</v>
+        <f>0.3+E10+0.3</f>
+        <v>7.3599999999999994</v>
       </c>
       <c r="P10" s="30">
-        <v>1.1000000000000001</v>
+        <v>1</v>
       </c>
       <c r="Q10" s="30">
         <v>1.1000000000000001</v>
       </c>
       <c r="R10" s="34">
         <f t="shared" si="18"/>
-        <v>23.776499999999999</v>
+        <v>20.239999999999998</v>
       </c>
       <c r="S10" s="32">
         <f t="shared" si="19"/>
-        <v>1.3099999999999998</v>
+        <v>1.2266666666666666</v>
       </c>
       <c r="U10" s="33">
         <f t="shared" si="0"/>
-        <v>439.75959999999998</v>
+        <v>436.22309999999999</v>
       </c>
       <c r="V10" s="34">
         <f t="shared" si="20"/>
@@ -75865,15 +75874,15 @@
       </c>
       <c r="W10" s="35">
         <f t="shared" si="21"/>
-        <v>1.6022390415126812E-2</v>
+        <v>1.6152285378743126E-2</v>
       </c>
       <c r="X10" s="32">
         <f t="shared" ref="X10:X45" si="45">MAX(IF(W10&lt;$S10,(U10/($P10*$O10))-(6*V10/($P10*$O10^2)),IF(W10=$S10,(2*U10)/($P10*$O10),(2*U10)/($P10*(3*($O10/2-W10))))),IF(W10&lt;$S10,(U10/($P10*$O10))+(6*V10/($P10*$O10^2)),IF(W10=$S10,(2*U10)/($P10*$O10),(2*U10)/($P10*(3*($O10/2-W10))))))/10</f>
-        <v>5.1484874618806193</v>
+        <v>6.0049880671077505</v>
       </c>
       <c r="Y10" s="33">
         <f t="shared" si="1"/>
-        <v>557.85579999999993</v>
+        <v>554.3193</v>
       </c>
       <c r="Z10" s="34">
         <f t="shared" si="2"/>
@@ -75881,24 +75890,24 @@
       </c>
       <c r="AA10" s="35">
         <f t="shared" si="22"/>
-        <v>1.2803846442037532E-2</v>
+        <v>1.2885533662638123E-2</v>
       </c>
       <c r="AB10" s="32">
-        <f>MAX(IF(AA10&lt;$S10,(Y10/($P10*$O10))-(6*Z10/($P10*$O10^2)),IF(AA10=$S10,(2*Y10)/($P10*$O10),(2*Y10)/($P10*(3*($O10/2-AA10))))),IF(AA10&lt;$S10,(Y10/($P10*$O10))+(6*Z10/($P10*$O10^2)),IF(AA10=$S10,(2*Y10)/($P10*$O10),(2*Y10)/($P10*(3*($O10/2-AA10))))))/10-0.016</f>
-        <v>6.4992468511229644</v>
+        <f>MAX(IF(AA10&lt;$S10,(Y10/($P10*$O10))-(6*Z10/($P10*$O10^2)),IF(AA10=$S10,(2*Y10)/($P10*$O10),(2*Y10)/($P10*(3*($O10/2-AA10))))),IF(AA10&lt;$S10,(Y10/($P10*$O10))+(6*Z10/($P10*$O10^2)),IF(AA10=$S10,(2*Y10)/($P10*$O10),(2*Y10)/($P10*(3*($O10/2-AA10))))))/10</f>
+        <v>7.6106270823487723</v>
       </c>
       <c r="AC10" s="53">
         <f t="shared" si="3"/>
-        <v>0.79207499413547988</v>
+        <v>0.75062350838846881</v>
       </c>
       <c r="AD10" s="53">
         <f t="shared" si="4"/>
-        <v>0.99988413094199458</v>
+        <v>0.95132838529359653</v>
       </c>
       <c r="AE10" s="36"/>
       <c r="AF10" s="38">
         <f t="shared" si="5"/>
-        <v>656.47919999999999</v>
+        <v>652.94270000000006</v>
       </c>
       <c r="AG10" s="34">
         <f t="shared" si="6"/>
@@ -75906,15 +75915,15 @@
       </c>
       <c r="AH10" s="34">
         <f t="shared" si="24"/>
-        <v>1.0401852792898847E-2</v>
+        <v>1.045819181376865E-2</v>
       </c>
       <c r="AI10" s="32">
         <f t="shared" si="25"/>
-        <v>7.6531560462147254</v>
+        <v>8.9471398570415897</v>
       </c>
       <c r="AJ10" s="38">
         <f t="shared" si="7"/>
-        <v>223.03999999999996</v>
+        <v>219.50349999999997</v>
       </c>
       <c r="AK10" s="34">
         <f t="shared" si="8"/>
@@ -75922,15 +75931,15 @@
       </c>
       <c r="AL10" s="34">
         <f t="shared" si="26"/>
-        <v>3.2565459110473462E-2</v>
+        <v>3.3090132959155555E-2</v>
       </c>
       <c r="AM10" s="32">
         <f t="shared" si="27"/>
-        <v>2.643818877546515</v>
+        <v>3.0628362771739126</v>
       </c>
       <c r="AN10" s="38">
         <f t="shared" si="9"/>
-        <v>690.87144999999998</v>
+        <v>687.33495000000005</v>
       </c>
       <c r="AO10" s="34">
         <f t="shared" si="10"/>
@@ -75938,15 +75947,15 @@
       </c>
       <c r="AP10" s="34">
         <f t="shared" si="28"/>
-        <v>1.0067683358459811E-2</v>
+        <v>1.011948395756683E-2</v>
       </c>
       <c r="AQ10" s="32">
         <f t="shared" si="29"/>
-        <v>8.0520584420629575</v>
+        <v>9.4158311709888967</v>
       </c>
       <c r="AR10" s="38">
         <f t="shared" si="11"/>
-        <v>365.7920499999999</v>
+        <v>362.25554999999997</v>
       </c>
       <c r="AS10" s="34">
         <f t="shared" si="12"/>
@@ -75954,15 +75963,15 @@
       </c>
       <c r="AT10" s="34">
         <f t="shared" si="30"/>
-        <v>1.9906323825244432E-2</v>
+        <v>2.0100658223179742E-2</v>
       </c>
       <c r="AU10" s="32">
         <f t="shared" si="31"/>
-        <v>4.2950555655617988</v>
+        <v>5.0026034860881383</v>
       </c>
       <c r="AV10" s="38">
         <f t="shared" si="13"/>
-        <v>480.57535999999999</v>
+        <v>478.45346000000001</v>
       </c>
       <c r="AW10" s="34">
         <f t="shared" si="14"/>
@@ -75970,15 +75979,15 @@
       </c>
       <c r="AX10" s="34">
         <f t="shared" si="32"/>
-        <v>8.3445809622865394E-3</v>
+        <v>8.3815884621254496E-3</v>
       </c>
       <c r="AY10" s="32">
         <f t="shared" si="33"/>
-        <v>5.5937610614624775</v>
+        <v>6.5451446301984886</v>
       </c>
       <c r="AZ10" s="38">
         <f t="shared" si="15"/>
-        <v>47.136159999999961</v>
+        <v>45.014259999999979</v>
       </c>
       <c r="BA10" s="34">
         <f t="shared" si="16"/>
@@ -75986,23 +75995,23 @@
       </c>
       <c r="BB10" s="34">
         <f t="shared" si="34"/>
-        <v>9.4301275284198016E-2</v>
+        <v>9.8746486113511611E-2</v>
       </c>
       <c r="BC10" s="32">
         <f t="shared" si="35"/>
-        <v>0.58442389279426687</v>
+        <v>0.66084105033081264</v>
       </c>
       <c r="BD10" s="37">
         <f t="shared" si="36"/>
-        <v>8.0520584420629575</v>
+        <v>9.4158311709888967</v>
       </c>
       <c r="BE10" s="53">
         <f t="shared" si="17"/>
-        <v>0.94730099318387739</v>
+        <v>0.94158311709888964</v>
       </c>
       <c r="BF10" s="38">
         <f t="shared" si="37"/>
-        <v>12.178738393620225</v>
+        <v>11.76978896373612</v>
       </c>
       <c r="BG10" s="34">
         <f t="shared" si="38"/>
@@ -76010,7 +76019,7 @@
       </c>
       <c r="BH10" s="34">
         <f t="shared" si="39"/>
-        <v>6.039043831547219</v>
+        <v>5.8362589902823725</v>
       </c>
       <c r="BI10" s="32" t="str">
         <f t="shared" si="40"/>
@@ -76018,7 +76027,7 @@
       </c>
       <c r="BJ10" s="38">
         <f t="shared" si="41"/>
-        <v>12.178738393620216</v>
+        <v>4.2371240269449988</v>
       </c>
       <c r="BK10" s="34">
         <f t="shared" si="42"/>
@@ -76026,7 +76035,7 @@
       </c>
       <c r="BL10" s="34">
         <f t="shared" si="43"/>
-        <v>6.0390438315472137</v>
+        <v>2.1010532365016519</v>
       </c>
       <c r="BM10" s="32" t="str">
         <f t="shared" si="44"/>
@@ -76034,7 +76043,7 @@
       </c>
     </row>
     <row r="11" spans="2:65" x14ac:dyDescent="0.25">
-      <c r="B11" s="29" t="s">
+      <c r="B11" s="95" t="s">
         <v>194</v>
       </c>
       <c r="C11" s="30" t="str">
@@ -76090,14 +76099,14 @@
         <v>1.77</v>
       </c>
       <c r="P11" s="30">
-        <v>1</v>
+        <v>0.6</v>
       </c>
       <c r="Q11" s="30">
-        <v>1</v>
+        <v>0.6</v>
       </c>
       <c r="R11" s="34">
         <f t="shared" si="18"/>
-        <v>4.4249999999999998</v>
+        <v>1.5929999999999997</v>
       </c>
       <c r="S11" s="32">
         <f t="shared" si="19"/>
@@ -76105,7 +76114,7 @@
       </c>
       <c r="U11" s="33">
         <f t="shared" si="0"/>
-        <v>63.206699999999998</v>
+        <v>60.374699999999997</v>
       </c>
       <c r="V11" s="34">
         <f t="shared" si="20"/>
@@ -76113,15 +76122,15 @@
       </c>
       <c r="W11" s="35">
         <f t="shared" si="21"/>
-        <v>1.0952952772411786E-2</v>
+        <v>1.1466723644175459E-2</v>
       </c>
       <c r="X11" s="32">
         <f t="shared" si="45"/>
-        <v>3.7035864215263814</v>
+        <v>5.9059773692106345</v>
       </c>
       <c r="Y11" s="33">
         <f t="shared" si="1"/>
-        <v>73.247199999999992</v>
+        <v>70.415199999999999</v>
       </c>
       <c r="Z11" s="34">
         <f t="shared" si="2"/>
@@ -76129,24 +76138,24 @@
       </c>
       <c r="AA11" s="35">
         <f t="shared" si="22"/>
-        <v>8.5723413318188283E-3</v>
+        <v>8.917108806053238E-3</v>
       </c>
       <c r="AB11" s="32">
         <f t="shared" si="23"/>
-        <v>4.2585126879249255</v>
+        <v>6.8308544798748754</v>
       </c>
       <c r="AC11" s="53">
         <f t="shared" si="3"/>
-        <v>0.5697825263886741</v>
+        <v>0.73824717115132932</v>
       </c>
       <c r="AD11" s="53">
         <f t="shared" si="4"/>
-        <v>0.65515579814229619</v>
+        <v>0.85385680998435942</v>
       </c>
       <c r="AE11" s="36"/>
       <c r="AF11" s="38">
         <f t="shared" si="5"/>
-        <v>68.383700000000005</v>
+        <v>65.551699999999997</v>
       </c>
       <c r="AG11" s="34">
         <f t="shared" si="6"/>
@@ -76154,15 +76163,15 @@
       </c>
       <c r="AH11" s="34">
         <f t="shared" si="24"/>
-        <v>9.5402851849197973E-3</v>
+        <v>9.9524497457731832E-3</v>
       </c>
       <c r="AI11" s="32">
         <f t="shared" si="25"/>
-        <v>3.988430814899933</v>
+        <v>6.3807180248332207</v>
       </c>
       <c r="AJ11" s="38">
         <f t="shared" si="7"/>
-        <v>58.029699999999998</v>
+        <v>55.197699999999998</v>
       </c>
       <c r="AK11" s="34">
         <f t="shared" si="8"/>
@@ -76170,15 +76179,15 @@
       </c>
       <c r="AL11" s="34">
         <f t="shared" si="26"/>
-        <v>1.2617676810322991E-2</v>
+        <v>1.3265045463850851E-2</v>
       </c>
       <c r="AM11" s="32">
         <f t="shared" si="27"/>
-        <v>3.4187420281528298</v>
+        <v>5.4312367135880484</v>
       </c>
       <c r="AN11" s="38">
         <f t="shared" si="9"/>
-        <v>74.619825000000006</v>
+        <v>71.787824999999998</v>
       </c>
       <c r="AO11" s="34">
         <f t="shared" si="10"/>
@@ -76186,15 +76195,15 @@
       </c>
       <c r="AP11" s="34">
         <f t="shared" si="28"/>
-        <v>8.2293814009882765E-3</v>
+        <v>8.5540270930342301E-3</v>
       </c>
       <c r="AQ11" s="32">
         <f t="shared" si="29"/>
-        <v>4.3334144163554535</v>
+        <v>6.9556906939257557</v>
       </c>
       <c r="AR11" s="38">
         <f t="shared" si="11"/>
-        <v>66.854325000000003</v>
+        <v>64.022324999999995</v>
       </c>
       <c r="AS11" s="34">
         <f t="shared" si="12"/>
@@ -76202,15 +76211,15 @@
       </c>
       <c r="AT11" s="34">
         <f t="shared" si="30"/>
-        <v>1.0080499653537748E-2</v>
+        <v>1.0526406218455828E-2</v>
       </c>
       <c r="AU11" s="32">
         <f t="shared" si="31"/>
-        <v>3.9061478262951264</v>
+        <v>6.2435797104918755</v>
       </c>
       <c r="AV11" s="38">
         <f t="shared" si="13"/>
-        <v>43.101019999999998</v>
+        <v>41.401819999999994</v>
       </c>
       <c r="AW11" s="34">
         <f t="shared" si="14"/>
@@ -76218,15 +76227,15 @@
       </c>
       <c r="AX11" s="34">
         <f t="shared" si="32"/>
-        <v>8.7116267782061784E-3</v>
+        <v>9.0691665245634153E-3</v>
       </c>
       <c r="AY11" s="32">
         <f t="shared" si="33"/>
-        <v>2.50699624628938</v>
+        <v>4.0183270771489665</v>
       </c>
       <c r="AZ11" s="38">
         <f t="shared" si="15"/>
-        <v>32.747019999999999</v>
+        <v>31.047819999999994</v>
       </c>
       <c r="BA11" s="34">
         <f t="shared" si="16"/>
@@ -76234,31 +76243,31 @@
       </c>
       <c r="BB11" s="34">
         <f t="shared" si="34"/>
-        <v>1.3902944451128683E-2</v>
+        <v>1.4663831470293247E-2</v>
       </c>
       <c r="BC11" s="32">
         <f t="shared" si="35"/>
-        <v>1.9373074595422772</v>
+        <v>3.0688457659037942</v>
       </c>
       <c r="BD11" s="37">
         <f t="shared" si="36"/>
-        <v>4.3334144163554535</v>
+        <v>6.9556906939257557</v>
       </c>
       <c r="BE11" s="53">
         <f t="shared" si="17"/>
-        <v>0.5098134607477004</v>
+        <v>0.69556906939257557</v>
       </c>
       <c r="BF11" s="38">
         <f t="shared" si="37"/>
-        <v>5.4167680204443167</v>
+        <v>3.1300608122665898</v>
       </c>
       <c r="BG11" s="34">
         <f t="shared" si="38"/>
-        <v>0.16666666666666666</v>
+        <v>0.06</v>
       </c>
       <c r="BH11" s="34">
         <f t="shared" si="39"/>
-        <v>3.2500608122665904</v>
+        <v>5.2167680204443165</v>
       </c>
       <c r="BI11" s="32" t="str">
         <f t="shared" si="40"/>
@@ -76266,15 +76275,15 @@
       </c>
       <c r="BJ11" s="38">
         <f t="shared" si="41"/>
-        <v>1.9500364873599545</v>
+        <v>3.1300608122665912</v>
       </c>
       <c r="BK11" s="34">
         <f t="shared" si="42"/>
-        <v>0.16666666666666666</v>
+        <v>0.06</v>
       </c>
       <c r="BL11" s="34">
         <f t="shared" si="43"/>
-        <v>1.1700218924159729</v>
+        <v>5.2167680204443183</v>
       </c>
       <c r="BM11" s="32" t="str">
         <f t="shared" si="44"/>
@@ -76282,7 +76291,7 @@
       </c>
     </row>
     <row r="12" spans="2:65" x14ac:dyDescent="0.25">
-      <c r="B12" s="29" t="s">
+      <c r="B12" s="95" t="s">
         <v>194</v>
       </c>
       <c r="C12" s="30" t="str">
@@ -76338,14 +76347,14 @@
         <v>6.01</v>
       </c>
       <c r="P12" s="30">
-        <v>1.1000000000000001</v>
+        <v>0.9</v>
       </c>
       <c r="Q12" s="30">
-        <v>1.1000000000000001</v>
+        <v>1</v>
       </c>
       <c r="R12" s="34">
         <f t="shared" ref="R12" si="46">2.5*O12*P12*Q12</f>
-        <v>18.180250000000001</v>
+        <v>13.522499999999999</v>
       </c>
       <c r="S12" s="32">
         <f t="shared" ref="S12" si="47">O12/6</f>
@@ -76353,7 +76362,7 @@
       </c>
       <c r="U12" s="33">
         <f t="shared" ref="U12" si="48">ABS(R12+ABS(G12))</f>
-        <v>303.83114999999998</v>
+        <v>299.17339999999996</v>
       </c>
       <c r="V12" s="34">
         <f t="shared" ref="V12" si="49">ABS(K12)</f>
@@ -76361,15 +76370,15 @@
       </c>
       <c r="W12" s="35">
         <f t="shared" ref="W12" si="50">ABS(V12/U12)</f>
-        <v>1.9113576734972697E-2</v>
+        <v>1.9411150857663151E-2</v>
       </c>
       <c r="X12" s="32">
         <f t="shared" ref="X12" si="51">MAX(IF(W12&lt;$S12,(U12/($P12*$O12))-(6*V12/($P12*$O12^2)),IF(W12=$S12,(2*U12)/($P12*$O12),(2*U12)/($P12*(3*($O12/2-W12))))),IF(W12&lt;$S12,(U12/($P12*$O12))+(6*V12/($P12*$O12^2)),IF(W12=$S12,(2*U12)/($P12*$O12),(2*U12)/($P12*(3*($O12/2-W12))))))/10</f>
-        <v>4.6835393627471582</v>
+        <v>5.6382147766909707</v>
       </c>
       <c r="Y12" s="33">
         <f t="shared" ref="Y12" si="52">ABS(R12+ABS(G12)+ABS(H12))</f>
-        <v>391.48204999999996</v>
+        <v>386.82429999999994</v>
       </c>
       <c r="Z12" s="34">
         <f t="shared" ref="Z12" si="53">ABS(K12+L12)</f>
@@ -76377,24 +76386,24 @@
       </c>
       <c r="AA12" s="35">
         <f t="shared" ref="AA12" si="54">ABS(Z12/Y12)</f>
-        <v>1.4824179039626467E-2</v>
+        <v>1.5002676925932525E-2</v>
       </c>
       <c r="AB12" s="32">
         <f t="shared" ref="AB12" si="55">MAX(IF(AA12&lt;$S12,(Y12/($P12*$O12))-(6*Z12/($P12*$O12^2)),IF(AA12=$S12,(2*Y12)/($P12*$O12),(2*Y12)/($P12*(3*($O12/2-AA12))))),IF(AA12&lt;$S12,(Y12/($P12*$O12))+(6*Z12/($P12*$O12^2)),IF(AA12=$S12,(2*Y12)/($P12*$O12),(2*Y12)/($P12*(3*($O12/2-AA12))))))/10</f>
-        <v>6.0093146840175349</v>
+        <v>7.2586068360214329</v>
       </c>
       <c r="AC12" s="53">
         <f t="shared" ref="AC12" si="56">X12/$E$2</f>
-        <v>0.72054451734571667</v>
+        <v>0.70477684708637134</v>
       </c>
       <c r="AD12" s="53">
         <f t="shared" ref="AD12" si="57">AB12/$E$2</f>
-        <v>0.92450995138731307</v>
+        <v>0.90732585450267911</v>
       </c>
       <c r="AE12" s="36"/>
       <c r="AF12" s="38">
         <f t="shared" ref="AF12" si="58">ABS(IF(B12="x",$R12+ABS($G12)+$I12,$R12+ABS($G12)+$J12))</f>
-        <v>500.48725000000002</v>
+        <v>495.82949999999994</v>
       </c>
       <c r="AG12" s="34">
         <f t="shared" ref="AG12" si="59">ABS(IF(B12="x",$K12+$M12,$K12+$N12))</f>
@@ -76402,15 +76411,15 @@
       </c>
       <c r="AH12" s="34">
         <f t="shared" ref="AH12" si="60">ABS(AG12/AF12)</f>
-        <v>1.1345943378177965E-2</v>
+        <v>1.1452525515323312E-2</v>
       </c>
       <c r="AI12" s="32">
         <f t="shared" ref="AI12" si="61">MAX(IF(AH12&lt;$S12,(AF12/($P12*$O12))-(6*AG12/($P12*$O12^2)),IF(AH12=$S12,(2*AF12)/($P12*$O12),(2*AF12)/($P12*(3*($O12/2-AH12))))),IF(AH12&lt;$S12,(AF12/($P12*$O12))+(6*AG12/($P12*$O12^2)),IF(AH12=$S12,(2*AF12)/($P12*$O12),(2*AF12)/($P12*(3*($O12/2-AH12))))))/10</f>
-        <v>7.6562744150763695</v>
+        <v>9.271557618426673</v>
       </c>
       <c r="AJ12" s="38">
         <f t="shared" ref="AJ12" si="62">ABS(IF(B12="x",$R12+ABS($G12)-$I12,$R12+ABS($G12)-$J12))</f>
-        <v>107.17504999999997</v>
+        <v>102.51729999999995</v>
       </c>
       <c r="AK12" s="34">
         <f t="shared" ref="AK12" si="63">ABS(IF(B12="x",$K12-$M12,$K12-$N12))</f>
@@ -76418,15 +76427,15 @@
       </c>
       <c r="AL12" s="34">
         <f t="shared" ref="AL12" si="64">ABS(AK12/AJ12)</f>
-        <v>5.5386958065333315E-2</v>
+        <v>5.7903397767986503E-2</v>
       </c>
       <c r="AM12" s="32">
         <f t="shared" ref="AM12" si="65">MAX(IF(AL12&lt;$S12,(AJ12/($P12*$O12))-(6*AK12/($P12*$O12^2)),IF(AL12=$S12,(2*AJ12)/($P12*$O12),(2*AJ12)/($P12*(3*($O12/2-AL12))))),IF(AL12&lt;$S12,(AJ12/($P12*$O12))+(6*AK12/($P12*$O12^2)),IF(AL12=$S12,(2*AJ12)/($P12*$O12),(2*AJ12)/($P12*(3*($O12/2-AL12))))))/10</f>
-        <v>1.7108043104179462</v>
+        <v>2.0048719349552675</v>
       </c>
       <c r="AN12" s="38">
         <f t="shared" ref="AN12" si="66">ABS(IF(B12="x",$R12+ABS($G12)+0.75*ABS($H12)+0.75*$I12,$R12+ABS($G12)+0.75*ABS($H12)+0.75*$J12))</f>
-        <v>517.06140000000005</v>
+        <v>512.40364999999997</v>
       </c>
       <c r="AO12" s="34">
         <f t="shared" ref="AO12" si="67">ABS(IF(B12="x",$K12+0.75*$L12+0.75*$M12,$K12+0.75*$L12+0.75*$N12))</f>
@@ -76434,15 +76443,15 @@
       </c>
       <c r="AP12" s="34">
         <f t="shared" ref="AP12" si="68">ABS(AO12/AN12)</f>
-        <v>1.1038872752829739E-2</v>
+        <v>1.1139216123850796E-2</v>
       </c>
       <c r="AQ12" s="32">
         <f t="shared" ref="AQ12" si="69">MAX(IF(AP12&lt;$S12,(AN12/($P12*$O12))-(6*AO12/($P12*$O12^2)),IF(AP12=$S12,(2*AN12)/($P12*$O12),(2*AN12)/($P12*(3*($O12/2-AP12))))),IF(AP12&lt;$S12,(AN12/($P12*$O12))+(6*AO12/($P12*$O12^2)),IF(AP12=$S12,(2*AN12)/($P12*$O12),(2*AN12)/($P12*(3*($O12/2-AP12))))))/10</f>
-        <v>7.9074221429468512</v>
+        <v>9.5785159524905943</v>
       </c>
       <c r="AR12" s="38">
         <f t="shared" ref="AR12" si="70">ABS(IF(B12="x",$R12+ABS($G12)+0.75*ABS($H12)-0.75*$I12,$R12+ABS($G12)+0.75*ABS($H12)-0.75*$J12))</f>
-        <v>222.07724999999999</v>
+        <v>217.41949999999997</v>
       </c>
       <c r="AS12" s="34">
         <f t="shared" ref="AS12" si="71">ABS(IF(B12="x",$K12+0.75*$L12-0.75*$M12,$K12+0.75*$L12-0.75*$N12))</f>
@@ -76450,15 +76459,15 @@
       </c>
       <c r="AT12" s="34">
         <f t="shared" ref="AT12" si="72">ABS(AS12/AR12)</f>
-        <v>2.6571722227288024E-2</v>
+        <v>2.7140964816863251E-2</v>
       </c>
       <c r="AU12" s="32">
         <f t="shared" ref="AU12" si="73">MAX(IF(AT12&lt;$S12,(AR12/($P12*$O12))-(6*AS12/($P12*$O12^2)),IF(AT12=$S12,(2*AR12)/($P12*$O12),(2*AR12)/($P12*(3*($O12/2-AT12))))),IF(AT12&lt;$S12,(AR12/($P12*$O12))+(6*AS12/($P12*$O12^2)),IF(AT12=$S12,(2*AR12)/($P12*$O12),(2*AR12)/($P12*(3*($O12/2-AT12))))))/10</f>
-        <v>3.4483195644530324</v>
+        <v>4.1285016898870399</v>
       </c>
       <c r="AV12" s="38">
         <f t="shared" ref="AV12" si="74">ABS(IF(B12="x",0.6*$R12+0.6*ABS($G12)+$I12,0.6*$R12+0.6*ABS($G12)+$J12))</f>
-        <v>378.95479</v>
+        <v>376.16013999999996</v>
       </c>
       <c r="AW12" s="34">
         <f t="shared" ref="AW12" si="75">ABS(IF(B12="x",0.6*$K12+$M12,0.6*$K12+$N12))</f>
@@ -76466,15 +76475,15 @@
       </c>
       <c r="AX12" s="34">
         <f t="shared" ref="AX12" si="76">ABS(AW12/AV12)</f>
-        <v>8.8548293584044674E-3</v>
+        <v>8.9206155654876149E-3</v>
       </c>
       <c r="AY12" s="32">
         <f t="shared" ref="AY12" si="77">MAX(IF(AX12&lt;$S12,(AV12/($P12*$O12))-(6*AW12/($P12*$O12^2)),IF(AX12=$S12,(2*AV12)/($P12*$O12),(2*AV12)/($P12*(3*($O12/2-AX12))))),IF(AX12&lt;$S12,(AV12/($P12*$O12))+(6*AW12/($P12*$O12^2)),IF(AX12=$S12,(2*AV12)/($P12*$O12),(2*AV12)/($P12*(3*($O12/2-AX12))))))/10</f>
-        <v>5.7828586699775064</v>
+        <v>7.0162717077502847</v>
       </c>
       <c r="AZ12" s="38">
         <f t="shared" ref="AZ12" si="78">ABS(IF(B12="x",0.6*$R12+0.6*ABS($G12)-$I12,0.6*$R12+0.6*ABS($G12)-$J12))</f>
-        <v>14.357410000000016</v>
+        <v>17.152060000000034</v>
       </c>
       <c r="BA12" s="34">
         <f t="shared" ref="BA12" si="79">ABS(IF(B12="x",0.6*$K12-$M12,0.6*$K12-$N12))</f>
@@ -76482,31 +76491,31 @@
       </c>
       <c r="BB12" s="34">
         <f t="shared" ref="BB12" si="80">ABS(BA12/AZ12)</f>
-        <v>0.25165959598562665</v>
+        <v>0.21065574630685718</v>
       </c>
       <c r="BC12" s="32">
         <f t="shared" ref="BC12" si="81">MAX(IF(BB12&lt;$S12,(AZ12/($P12*$O12))-(6*BA12/($P12*$O12^2)),IF(BB12=$S12,(2*AZ12)/($P12*$O12),(2*AZ12)/($P12*(3*($O12/2-BB12))))),IF(BB12&lt;$S12,(AZ12/($P12*$O12))+(6*BA12/($P12*$O12^2)),IF(BB12=$S12,(2*AZ12)/($P12*$O12),(2*AZ12)/($P12*(3*($O12/2-BB12))))))/10</f>
-        <v>0.27173768043026175</v>
+        <v>0.38379049830365364</v>
       </c>
       <c r="BD12" s="37">
         <f t="shared" ref="BD12" si="82">MAX(AI12,AM12,AQ12,AU12,AY12,BC12)</f>
-        <v>7.9074221429468512</v>
+        <v>9.5785159524905943</v>
       </c>
       <c r="BE12" s="53">
         <f t="shared" ref="BE12" si="83">(BD12)/$E$3</f>
-        <v>0.93028495799374722</v>
+        <v>0.95785159524905938</v>
       </c>
       <c r="BF12" s="38">
         <f t="shared" si="37"/>
-        <v>11.959975991207113</v>
+        <v>9.698247401896726</v>
       </c>
       <c r="BG12" s="34">
         <f t="shared" si="38"/>
-        <v>0.20166666666666669</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="BH12" s="34">
         <f t="shared" ref="BH12" si="84">BF12/BG12/10</f>
-        <v>5.930566607210138</v>
+        <v>5.8189484411380352</v>
       </c>
       <c r="BI12" s="32" t="str">
         <f t="shared" ref="BI12" si="85">IF(BH12&lt;7,"NO PARRILLA","PARRILLA")</f>
@@ -76514,15 +76523,15 @@
       </c>
       <c r="BJ12" s="38">
         <f t="shared" ref="BJ12" si="86">($BD12*10*((O12-E12)/2)^2*1)/2</f>
-        <v>3.5583399643260787</v>
+        <v>4.3103321786207625</v>
       </c>
       <c r="BK12" s="34">
         <f t="shared" si="42"/>
-        <v>0.20166666666666669</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="BL12" s="34">
         <f t="shared" ref="BL12" si="87">BJ12/BK12/10</f>
-        <v>1.7644660980129312</v>
+        <v>2.5861993071724578</v>
       </c>
       <c r="BM12" s="32" t="str">
         <f t="shared" ref="BM12" si="88">IF(BL12&lt;7,"NO PARRILLA","PARRILLA")</f>
@@ -76530,7 +76539,7 @@
       </c>
     </row>
     <row r="13" spans="2:65" x14ac:dyDescent="0.25">
-      <c r="B13" s="29" t="s">
+      <c r="B13" s="95" t="s">
         <v>194</v>
       </c>
       <c r="C13" s="30" t="str">
@@ -76582,18 +76591,18 @@
         <v>0.2205</v>
       </c>
       <c r="O13" s="29">
-        <f t="shared" ref="O10:O45" si="89">0.3+E13+0.3</f>
+        <f t="shared" ref="O13:O45" si="89">0.3+E13+0.3</f>
         <v>2.5199999999999996</v>
       </c>
       <c r="P13" s="30">
-        <v>1</v>
+        <v>0.6</v>
       </c>
       <c r="Q13" s="30">
-        <v>1</v>
+        <v>0.6</v>
       </c>
       <c r="R13" s="34">
         <f t="shared" si="18"/>
-        <v>6.2999999999999989</v>
+        <v>2.2679999999999993</v>
       </c>
       <c r="S13" s="32">
         <f t="shared" si="19"/>
@@ -76601,7 +76610,7 @@
       </c>
       <c r="U13" s="33">
         <f t="shared" si="0"/>
-        <v>53.0777</v>
+        <v>49.045700000000004</v>
       </c>
       <c r="V13" s="34">
         <f t="shared" si="20"/>
@@ -76609,15 +76618,15 @@
       </c>
       <c r="W13" s="35">
         <f t="shared" si="21"/>
-        <v>2.1574032032284744E-2</v>
+        <v>2.334761253280104E-2</v>
       </c>
       <c r="X13" s="32">
         <f t="shared" si="45"/>
-        <v>2.2144495464852612</v>
+        <v>3.4240825774754349</v>
       </c>
       <c r="Y13" s="33">
         <f t="shared" si="1"/>
-        <v>93.101500000000001</v>
+        <v>89.069500000000005</v>
       </c>
       <c r="Z13" s="34">
         <f t="shared" si="2"/>
@@ -76625,24 +76634,24 @@
       </c>
       <c r="AA13" s="35">
         <f t="shared" si="22"/>
-        <v>1.1660392152650601E-2</v>
+        <v>1.2188235029948521E-2</v>
       </c>
       <c r="AB13" s="32">
         <f t="shared" si="23"/>
-        <v>3.7970738851096</v>
+        <v>6.061789808516</v>
       </c>
       <c r="AC13" s="53">
         <f t="shared" si="3"/>
-        <v>0.34068454561311712</v>
+        <v>0.42801032218442936</v>
       </c>
       <c r="AD13" s="53">
         <f t="shared" si="4"/>
-        <v>0.58416521309378466</v>
+        <v>0.7577237260645</v>
       </c>
       <c r="AE13" s="36"/>
       <c r="AF13" s="38">
         <f t="shared" si="5"/>
-        <v>53.843299999999999</v>
+        <v>49.811300000000003</v>
       </c>
       <c r="AG13" s="34">
         <f t="shared" si="6"/>
@@ -76650,15 +76659,15 @@
       </c>
       <c r="AH13" s="34">
         <f t="shared" si="24"/>
-        <v>2.0489085921553841E-2</v>
+        <v>2.2147584985736168E-2</v>
       </c>
       <c r="AI13" s="32">
         <f t="shared" si="25"/>
-        <v>2.2408716931216932</v>
+        <v>3.4681194885361557</v>
       </c>
       <c r="AJ13" s="38">
         <f t="shared" si="7"/>
-        <v>52.312100000000001</v>
+        <v>48.280100000000004</v>
       </c>
       <c r="AK13" s="34">
         <f t="shared" si="8"/>
@@ -76666,15 +76675,15 @@
       </c>
       <c r="AL13" s="34">
         <f t="shared" si="26"/>
-        <v>2.2690735030709914E-2</v>
+        <v>2.4585698869720649E-2</v>
       </c>
       <c r="AM13" s="32">
         <f t="shared" si="27"/>
-        <v>2.1880273998488287</v>
+        <v>3.3800456664147149</v>
       </c>
       <c r="AN13" s="38">
         <f t="shared" si="9"/>
-        <v>83.669750000000008</v>
+        <v>79.637750000000011</v>
       </c>
       <c r="AO13" s="34">
         <f t="shared" si="10"/>
@@ -76682,15 +76691,15 @@
       </c>
       <c r="AP13" s="34">
         <f t="shared" si="28"/>
-        <v>1.2777019173596192E-2</v>
+        <v>1.34239101431168E-2</v>
       </c>
       <c r="AQ13" s="32">
         <f t="shared" si="29"/>
-        <v>3.4212344104308392</v>
+        <v>5.4353906840514004</v>
       </c>
       <c r="AR13" s="38">
         <f t="shared" si="11"/>
-        <v>82.521349999999998</v>
+        <v>78.489350000000002</v>
       </c>
       <c r="AS13" s="34">
         <f t="shared" si="12"/>
@@ -76698,15 +76707,15 @@
       </c>
       <c r="AT13" s="34">
         <f t="shared" si="30"/>
-        <v>1.3716450348909708E-2</v>
+        <v>1.4421064768659699E-2</v>
       </c>
       <c r="AU13" s="32">
         <f t="shared" si="31"/>
-        <v>3.3816011904761907</v>
+        <v>5.3693353174603189</v>
       </c>
       <c r="AV13" s="38">
         <f t="shared" si="13"/>
-        <v>32.612220000000001</v>
+        <v>30.193020000000001</v>
       </c>
       <c r="AW13" s="34">
         <f t="shared" si="14"/>
@@ -76714,15 +76723,15 @@
       </c>
       <c r="AX13" s="34">
         <f t="shared" si="32"/>
-        <v>1.9782768545042316E-2</v>
+        <v>2.1367852569898604E-2</v>
       </c>
       <c r="AY13" s="32">
         <f t="shared" si="33"/>
-        <v>1.3550918745275891</v>
+        <v>2.0984864575459818</v>
       </c>
       <c r="AZ13" s="38">
         <f t="shared" si="15"/>
-        <v>31.081020000000002</v>
+        <v>28.661820000000002</v>
       </c>
       <c r="BA13" s="34">
         <f t="shared" si="16"/>
@@ -76730,31 +76739,31 @@
       </c>
       <c r="BB13" s="34">
         <f t="shared" si="34"/>
-        <v>2.3453541743482034E-2</v>
+        <v>2.5433137183891324E-2</v>
       </c>
       <c r="BC13" s="32">
         <f t="shared" si="35"/>
-        <v>1.3022475812547245</v>
+        <v>2.0104126354245406</v>
       </c>
       <c r="BD13" s="37">
         <f t="shared" si="36"/>
-        <v>3.4212344104308392</v>
+        <v>5.4353906840514004</v>
       </c>
       <c r="BE13" s="53">
         <f t="shared" si="17"/>
-        <v>0.40249816593303989</v>
+        <v>0.54353906840513999</v>
       </c>
       <c r="BF13" s="38">
         <f t="shared" si="37"/>
-        <v>4.2765430130385491</v>
+        <v>2.4459258078231301</v>
       </c>
       <c r="BG13" s="34">
         <f t="shared" si="38"/>
-        <v>0.16666666666666666</v>
+        <v>0.06</v>
       </c>
       <c r="BH13" s="34">
         <f t="shared" si="39"/>
-        <v>2.5659258078231297</v>
+        <v>4.0765430130385507</v>
       </c>
       <c r="BI13" s="32" t="str">
         <f t="shared" si="40"/>
@@ -76762,15 +76771,15 @@
       </c>
       <c r="BJ13" s="38">
         <f t="shared" si="41"/>
-        <v>1.5395554846938759</v>
+        <v>2.4459258078231274</v>
       </c>
       <c r="BK13" s="34">
         <f t="shared" si="42"/>
-        <v>0.16666666666666666</v>
+        <v>0.06</v>
       </c>
       <c r="BL13" s="34">
         <f t="shared" si="43"/>
-        <v>0.92373329081632571</v>
+        <v>4.0765430130385463</v>
       </c>
       <c r="BM13" s="32" t="str">
         <f t="shared" si="44"/>
@@ -76778,7 +76787,7 @@
       </c>
     </row>
     <row r="14" spans="2:65" x14ac:dyDescent="0.25">
-      <c r="B14" s="29" t="s">
+      <c r="B14" s="95" t="s">
         <v>194</v>
       </c>
       <c r="C14" s="30" t="str">
@@ -76830,26 +76839,26 @@
         <v>0.42549999999999999</v>
       </c>
       <c r="O14" s="29">
-        <f>0.65+E14+0.65</f>
-        <v>6.6000000000000005</v>
+        <f>0.3+E14+0.3</f>
+        <v>5.8999999999999995</v>
       </c>
       <c r="P14" s="30">
-        <v>1.7</v>
+        <v>1.6</v>
       </c>
       <c r="Q14" s="30">
         <v>1.7</v>
       </c>
       <c r="R14" s="34">
         <f t="shared" si="18"/>
-        <v>47.685000000000002</v>
+        <v>40.119999999999997</v>
       </c>
       <c r="S14" s="32">
         <f t="shared" si="19"/>
-        <v>1.1000000000000001</v>
+        <v>0.98333333333333328</v>
       </c>
       <c r="U14" s="33">
         <f t="shared" si="0"/>
-        <v>568.52649999999994</v>
+        <v>560.9615</v>
       </c>
       <c r="V14" s="34">
         <f t="shared" si="20"/>
@@ -76857,15 +76866,15 @@
       </c>
       <c r="W14" s="35">
         <f t="shared" si="21"/>
-        <v>7.2149671123509637E-3</v>
+        <v>7.3122665280950646E-3</v>
       </c>
       <c r="X14" s="32">
         <f t="shared" si="45"/>
-        <v>5.1003163992869869</v>
+        <v>5.9865775818730258</v>
       </c>
       <c r="Y14" s="33">
         <f t="shared" si="1"/>
-        <v>706.27309999999989</v>
+        <v>698.70810000000006</v>
       </c>
       <c r="Z14" s="34">
         <f t="shared" si="2"/>
@@ -76873,24 +76882,24 @@
       </c>
       <c r="AA14" s="35">
         <f t="shared" si="22"/>
-        <v>5.5873570719315235E-3</v>
+        <v>5.6478520858710517E-3</v>
       </c>
       <c r="AB14" s="32">
         <f t="shared" si="23"/>
-        <v>6.3267429103872939</v>
+        <v>7.444080346883081</v>
       </c>
       <c r="AC14" s="53">
         <f t="shared" ref="AC14:AC45" si="90">X14/$E$2</f>
-        <v>0.78466406142876721</v>
+        <v>0.74832219773412822</v>
       </c>
       <c r="AD14" s="53">
         <f t="shared" ref="AD14:AD45" si="91">AB14/$E$2</f>
-        <v>0.97334506313650671</v>
+        <v>0.93051004336038512</v>
       </c>
       <c r="AE14" s="36"/>
       <c r="AF14" s="38">
         <f t="shared" si="5"/>
-        <v>921.4864</v>
+        <v>913.92139999999995</v>
       </c>
       <c r="AG14" s="34">
         <f t="shared" si="6"/>
@@ -76898,15 +76907,15 @@
       </c>
       <c r="AH14" s="34">
         <f t="shared" si="24"/>
-        <v>4.2797159024810351E-3</v>
+        <v>4.3151413239694352E-3</v>
       </c>
       <c r="AI14" s="32">
         <f t="shared" si="25"/>
-        <v>8.2448447577378055</v>
+        <v>9.7238553217466244</v>
       </c>
       <c r="AJ14" s="38">
         <f t="shared" si="7"/>
-        <v>215.56659999999994</v>
+        <v>208.0016</v>
       </c>
       <c r="AK14" s="34">
         <f t="shared" si="8"/>
@@ -76914,15 +76923,15 @@
       </c>
       <c r="AL14" s="34">
         <f t="shared" si="26"/>
-        <v>1.976233795031327E-2</v>
+        <v>2.0481092453134973E-2</v>
       </c>
       <c r="AM14" s="32">
         <f t="shared" si="27"/>
-        <v>1.9557880408361688</v>
+        <v>2.2492998419994255</v>
       </c>
       <c r="AN14" s="38">
         <f t="shared" si="9"/>
-        <v>936.55637499999989</v>
+        <v>928.99137499999995</v>
       </c>
       <c r="AO14" s="34">
         <f t="shared" si="10"/>
@@ -76930,15 +76939,15 @@
       </c>
       <c r="AP14" s="34">
         <f t="shared" si="28"/>
-        <v>4.1283953675506184E-3</v>
+        <v>4.1620138830675358E-3</v>
       </c>
       <c r="AQ14" s="32">
         <f t="shared" si="29"/>
-        <v>8.3785325514503306</v>
+        <v>9.8826629605357645</v>
       </c>
       <c r="AR14" s="38">
         <f t="shared" si="11"/>
-        <v>407.11652499999991</v>
+        <v>399.55152499999997</v>
       </c>
       <c r="AS14" s="34">
         <f t="shared" si="12"/>
@@ -76946,15 +76955,15 @@
       </c>
       <c r="AT14" s="34">
         <f t="shared" si="30"/>
-        <v>1.0080099303264589E-2</v>
+        <v>1.02709531643009E-2</v>
       </c>
       <c r="AU14" s="32">
         <f t="shared" si="31"/>
-        <v>3.6617400137741036</v>
+        <v>4.2767463507253662</v>
       </c>
       <c r="AV14" s="38">
         <f t="shared" si="13"/>
-        <v>694.07579999999996</v>
+        <v>689.53679999999997</v>
       </c>
       <c r="AW14" s="34">
         <f t="shared" si="14"/>
@@ -76962,15 +76971,15 @@
       </c>
       <c r="AX14" s="34">
         <f t="shared" si="32"/>
-        <v>3.31799495098374E-3</v>
+        <v>3.3398362494938632E-3</v>
       </c>
       <c r="AY14" s="32">
         <f t="shared" si="33"/>
-        <v>6.2047181980230102</v>
+        <v>7.3292242889974144</v>
       </c>
       <c r="AZ14" s="38">
         <f t="shared" si="15"/>
-        <v>11.844000000000051</v>
+        <v>16.383000000000038</v>
       </c>
       <c r="BA14" s="34">
         <f t="shared" si="16"/>
@@ -76978,23 +76987,23 @@
       </c>
       <c r="BB14" s="34">
         <f t="shared" si="34"/>
-        <v>0.22115332657885753</v>
+        <v>0.15988158456937029</v>
       </c>
       <c r="BC14" s="32">
         <f t="shared" si="35"/>
-        <v>0.12678447577378102</v>
+        <v>0.20176626687733451</v>
       </c>
       <c r="BD14" s="37">
         <f t="shared" si="36"/>
-        <v>8.3785325514503306</v>
+        <v>9.8826629605357645</v>
       </c>
       <c r="BE14" s="53">
         <f t="shared" si="17"/>
-        <v>0.98570971193533297</v>
+        <v>0.98826629605357641</v>
       </c>
       <c r="BF14" s="38">
         <f t="shared" si="37"/>
-        <v>30.26744884211432</v>
+        <v>31.624521473714456</v>
       </c>
       <c r="BG14" s="34">
         <f t="shared" si="38"/>
@@ -77002,7 +77011,7 @@
       </c>
       <c r="BH14" s="34">
         <f t="shared" si="39"/>
-        <v>6.2838994135877488</v>
+        <v>6.5656445966189185</v>
       </c>
       <c r="BI14" s="32" t="str">
         <f t="shared" si="40"/>
@@ -77010,7 +77019,7 @@
       </c>
       <c r="BJ14" s="38">
         <f t="shared" si="41"/>
-        <v>17.699650014938847</v>
+        <v>4.4471983322410891</v>
       </c>
       <c r="BK14" s="34">
         <f t="shared" si="42"/>
@@ -77018,7 +77027,7 @@
       </c>
       <c r="BL14" s="34">
         <f t="shared" si="43"/>
-        <v>3.6746678231706951</v>
+        <v>0.92329377139953406</v>
       </c>
       <c r="BM14" s="32" t="str">
         <f t="shared" si="44"/>
@@ -77026,7 +77035,7 @@
       </c>
     </row>
     <row r="15" spans="2:65" x14ac:dyDescent="0.25">
-      <c r="B15" s="29" t="s">
+      <c r="B15" s="95" t="s">
         <v>194</v>
       </c>
       <c r="C15" s="30" t="str">
@@ -77078,26 +77087,26 @@
         <v>0.311</v>
       </c>
       <c r="O15" s="29">
-        <f>0.4+E15+0.4</f>
-        <v>7.5500000000000007</v>
+        <f>0.3+E15+0.3</f>
+        <v>7.35</v>
       </c>
       <c r="P15" s="30">
-        <v>1.1000000000000001</v>
+        <v>0.9</v>
       </c>
       <c r="Q15" s="30">
-        <v>1.1000000000000001</v>
+        <v>1</v>
       </c>
       <c r="R15" s="34">
         <f t="shared" si="18"/>
-        <v>22.838750000000005</v>
+        <v>16.537500000000001</v>
       </c>
       <c r="S15" s="32">
         <f t="shared" si="19"/>
-        <v>1.2583333333333335</v>
+        <v>1.2249999999999999</v>
       </c>
       <c r="U15" s="33">
         <f t="shared" si="0"/>
-        <v>422.22455000000002</v>
+        <v>415.92330000000004</v>
       </c>
       <c r="V15" s="34">
         <f t="shared" si="20"/>
@@ -77105,15 +77114,15 @@
       </c>
       <c r="W15" s="35">
         <f t="shared" si="21"/>
-        <v>1.3675661446024397E-2</v>
+        <v>1.3882848111659048E-2</v>
       </c>
       <c r="X15" s="32">
         <f t="shared" si="45"/>
-        <v>5.1392332114620167</v>
+        <v>6.3588349607416665</v>
       </c>
       <c r="Y15" s="33">
         <f t="shared" si="1"/>
-        <v>530.74205000000006</v>
+        <v>524.44080000000008</v>
       </c>
       <c r="Z15" s="34">
         <f t="shared" si="2"/>
@@ -77121,24 +77130,24 @@
       </c>
       <c r="AA15" s="35">
         <f t="shared" si="22"/>
-        <v>1.0333079883156045E-2</v>
+        <v>1.0457233685861206E-2</v>
       </c>
       <c r="AB15" s="32">
         <f t="shared" si="23"/>
-        <v>6.4431108324595012</v>
+        <v>7.9957323954525119</v>
       </c>
       <c r="AC15" s="53">
         <f t="shared" si="90"/>
-        <v>0.79065126330184876</v>
+        <v>0.79485437009270832</v>
       </c>
       <c r="AD15" s="53">
         <f t="shared" si="91"/>
-        <v>0.99124782037838477</v>
+        <v>0.99946654943156399</v>
       </c>
       <c r="AE15" s="36"/>
       <c r="AF15" s="38">
         <f t="shared" si="5"/>
-        <v>608.93095000000005</v>
+        <v>602.62970000000007</v>
       </c>
       <c r="AG15" s="34">
         <f t="shared" si="6"/>
@@ -77146,15 +77155,15 @@
       </c>
       <c r="AH15" s="34">
         <f t="shared" si="24"/>
-        <v>8.7241418751994784E-3</v>
+        <v>8.8153637299987035E-3</v>
       </c>
       <c r="AI15" s="32">
         <f t="shared" si="25"/>
-        <v>7.3829346759113434</v>
+        <v>9.1756062443117834</v>
       </c>
       <c r="AJ15" s="38">
         <f t="shared" si="7"/>
-        <v>235.51815000000002</v>
+        <v>229.21690000000004</v>
       </c>
       <c r="AK15" s="34">
         <f t="shared" si="8"/>
@@ -77162,15 +77171,15 @@
       </c>
       <c r="AL15" s="34">
         <f t="shared" si="26"/>
-        <v>2.6477789503696426E-2</v>
+        <v>2.7205672880141037E-2</v>
       </c>
       <c r="AM15" s="32">
         <f t="shared" si="27"/>
-        <v>2.8955317470126904</v>
+        <v>3.5420636771715492</v>
       </c>
       <c r="AN15" s="38">
         <f t="shared" si="9"/>
-        <v>643.64247499999999</v>
+        <v>637.34122500000001</v>
       </c>
       <c r="AO15" s="34">
         <f t="shared" si="10"/>
@@ -77178,15 +77187,15 @@
       </c>
       <c r="AP15" s="34">
         <f t="shared" si="28"/>
-        <v>8.0950996902434073E-3</v>
+        <v>8.1751341285039268E-3</v>
       </c>
       <c r="AQ15" s="32">
         <f t="shared" si="29"/>
-        <v>7.7999175255471247</v>
+        <v>9.6990864994523882</v>
       </c>
       <c r="AR15" s="38">
         <f t="shared" si="11"/>
-        <v>363.58287500000006</v>
+        <v>357.28162500000008</v>
       </c>
       <c r="AS15" s="34">
         <f t="shared" si="12"/>
@@ -77194,15 +77203,15 @@
       </c>
       <c r="AT15" s="34">
         <f t="shared" si="30"/>
-        <v>1.6235775681129095E-2</v>
+        <v>1.6522120330145721E-2</v>
       </c>
       <c r="AU15" s="32">
         <f t="shared" si="31"/>
-        <v>4.4343653288731355</v>
+        <v>5.4739295740972134</v>
       </c>
       <c r="AV15" s="38">
         <f t="shared" si="13"/>
-        <v>440.04113000000001</v>
+        <v>436.26038000000005</v>
       </c>
       <c r="AW15" s="34">
         <f t="shared" si="14"/>
@@ -77210,15 +77219,15 @@
       </c>
       <c r="AX15" s="34">
         <f t="shared" si="32"/>
-        <v>6.8237257730885291E-3</v>
+        <v>6.8828620192372264E-3</v>
       </c>
       <c r="AY15" s="32">
         <f t="shared" si="33"/>
-        <v>5.3272413913265355</v>
+        <v>6.6320722600151187</v>
       </c>
       <c r="AZ15" s="38">
         <f t="shared" si="15"/>
-        <v>66.628330000000005</v>
+        <v>62.847580000000022</v>
       </c>
       <c r="BA15" s="34">
         <f t="shared" si="16"/>
@@ -77226,31 +77235,31 @@
       </c>
       <c r="BB15" s="34">
         <f t="shared" si="34"/>
-        <v>5.8928686941425668E-2</v>
+        <v>6.247368633764417E-2</v>
       </c>
       <c r="BC15" s="32">
         <f t="shared" si="35"/>
-        <v>0.83983846242788385</v>
+        <v>0.99852969287488258</v>
       </c>
       <c r="BD15" s="37">
         <f t="shared" si="36"/>
-        <v>7.7999175255471247</v>
+        <v>9.6990864994523882</v>
       </c>
       <c r="BE15" s="53">
         <f t="shared" si="17"/>
-        <v>0.91763735594672058</v>
+        <v>0.96990864994523884</v>
       </c>
       <c r="BF15" s="38">
         <f t="shared" si="37"/>
-        <v>11.797375257390028</v>
+        <v>9.8203250806955449</v>
       </c>
       <c r="BG15" s="34">
         <f t="shared" si="38"/>
-        <v>0.20166666666666669</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="BH15" s="34">
         <f t="shared" si="39"/>
-        <v>5.849938144160344</v>
+        <v>5.8921950484173271</v>
       </c>
       <c r="BI15" s="32" t="str">
         <f t="shared" si="40"/>
@@ -77258,15 +77267,15 @@
       </c>
       <c r="BJ15" s="38">
         <f t="shared" si="41"/>
-        <v>6.2399340204377101</v>
+        <v>4.3645889247535701</v>
       </c>
       <c r="BK15" s="34">
         <f t="shared" si="42"/>
-        <v>0.20166666666666669</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="BL15" s="34">
         <f t="shared" si="43"/>
-        <v>3.094182158894732</v>
+        <v>2.6187533548521422</v>
       </c>
       <c r="BM15" s="32" t="str">
         <f t="shared" si="44"/>
@@ -77274,7 +77283,7 @@
       </c>
     </row>
     <row r="16" spans="2:65" x14ac:dyDescent="0.25">
-      <c r="B16" s="29" t="s">
+      <c r="B16" s="95" t="s">
         <v>194</v>
       </c>
       <c r="C16" s="30" t="str">
@@ -77326,26 +77335,26 @@
         <v>0.15659999999999999</v>
       </c>
       <c r="O16" s="29">
-        <f>0.4+E16+0.4</f>
-        <v>2.68</v>
+        <f>0.3+E16+0.3</f>
+        <v>2.48</v>
       </c>
       <c r="P16" s="30">
-        <v>1.7</v>
+        <v>1.5</v>
       </c>
       <c r="Q16" s="30">
         <v>1.6</v>
       </c>
       <c r="R16" s="34">
         <f t="shared" si="18"/>
-        <v>18.224</v>
+        <v>14.880000000000003</v>
       </c>
       <c r="S16" s="32">
         <f t="shared" si="19"/>
-        <v>0.44666666666666671</v>
+        <v>0.41333333333333333</v>
       </c>
       <c r="U16" s="33">
         <f t="shared" si="0"/>
-        <v>210.20699999999999</v>
+        <v>206.863</v>
       </c>
       <c r="V16" s="34">
         <f t="shared" si="20"/>
@@ -77353,15 +77362,15 @@
       </c>
       <c r="W16" s="35">
         <f t="shared" si="21"/>
-        <v>6.8232742011445861E-3</v>
+        <v>6.9335743946476649E-3</v>
       </c>
       <c r="X16" s="32">
         <f t="shared" si="45"/>
-        <v>4.6843309789944048</v>
+        <v>5.6541150711064869</v>
       </c>
       <c r="Y16" s="33">
         <f t="shared" si="1"/>
-        <v>256.26499999999999</v>
+        <v>252.92099999999999</v>
       </c>
       <c r="Z16" s="34">
         <f t="shared" si="2"/>
@@ -77369,24 +77378,24 @@
       </c>
       <c r="AA16" s="35">
         <f t="shared" si="22"/>
-        <v>6.1050084873080605E-3</v>
+        <v>6.1857259776768245E-3</v>
       </c>
       <c r="AB16" s="32">
         <f t="shared" si="23"/>
-        <v>5.7016596123858321</v>
+        <v>6.9007010926118637</v>
       </c>
       <c r="AC16" s="53">
         <f t="shared" si="90"/>
-        <v>0.7206663044606777</v>
+        <v>0.70676438388831087</v>
       </c>
       <c r="AD16" s="53">
         <f t="shared" si="91"/>
-        <v>0.87717840190551266</v>
+        <v>0.86258763657648296</v>
       </c>
       <c r="AE16" s="36"/>
       <c r="AF16" s="38">
         <f t="shared" si="5"/>
-        <v>366.01080000000002</v>
+        <v>362.66679999999997</v>
       </c>
       <c r="AG16" s="34">
         <f t="shared" si="6"/>
@@ -77394,15 +77403,15 @@
       </c>
       <c r="AH16" s="34">
         <f t="shared" si="24"/>
-        <v>3.7252999091830072E-3</v>
+        <v>3.7596493530700908E-3</v>
       </c>
       <c r="AI16" s="32">
         <f t="shared" si="25"/>
-        <v>8.1006016668195464</v>
+        <v>9.8377846860908775</v>
       </c>
       <c r="AJ16" s="38">
         <f t="shared" si="7"/>
-        <v>54.403199999999998</v>
+        <v>51.059200000000004</v>
       </c>
       <c r="AK16" s="34">
         <f t="shared" si="8"/>
@@ -77410,15 +77419,15 @@
       </c>
       <c r="AL16" s="34">
         <f t="shared" si="26"/>
-        <v>2.7665652020469382E-2</v>
+        <v>2.9477547630985205E-2</v>
       </c>
       <c r="AM16" s="32">
         <f t="shared" si="27"/>
-        <v>1.2680602911692636</v>
+        <v>1.4704454561220952</v>
       </c>
       <c r="AN16" s="38">
         <f t="shared" si="9"/>
-        <v>361.60334999999998</v>
+        <v>358.25934999999998</v>
       </c>
       <c r="AO16" s="34">
         <f t="shared" si="10"/>
@@ -77426,15 +77435,15 @@
       </c>
       <c r="AP16" s="34">
         <f t="shared" si="28"/>
-        <v>4.0897021556907595E-3</v>
+        <v>4.1278755181127866E-3</v>
       </c>
       <c r="AQ16" s="32">
         <f t="shared" si="29"/>
-        <v>8.0095304699068315</v>
+        <v>9.7268067984738131</v>
       </c>
       <c r="AR16" s="38">
         <f t="shared" si="11"/>
-        <v>127.89765</v>
+        <v>124.55365</v>
       </c>
       <c r="AS16" s="34">
         <f t="shared" si="12"/>
@@ -77442,15 +77451,15 @@
       </c>
       <c r="AT16" s="34">
         <f t="shared" si="30"/>
-        <v>1.2393112774159649E-2</v>
+        <v>1.2725841434594648E-2</v>
       </c>
       <c r="AU16" s="32">
         <f t="shared" si="31"/>
-        <v>2.885124438169119</v>
+        <v>3.4513023759972254</v>
       </c>
       <c r="AV16" s="38">
         <f t="shared" si="13"/>
-        <v>281.928</v>
+        <v>279.92160000000001</v>
       </c>
       <c r="AW16" s="34">
         <f t="shared" si="14"/>
@@ -77458,15 +77467,15 @@
       </c>
       <c r="AX16" s="34">
         <f t="shared" si="32"/>
-        <v>2.801353537073295E-3</v>
+        <v>2.821432858343193E-3</v>
       </c>
       <c r="AY16" s="32">
         <f t="shared" si="33"/>
-        <v>6.2268692752217838</v>
+        <v>7.5761386576482836</v>
       </c>
       <c r="AZ16" s="38">
         <f t="shared" si="15"/>
-        <v>29.679600000000008</v>
+        <v>31.686000000000007</v>
       </c>
       <c r="BA16" s="34">
         <f t="shared" si="16"/>
@@ -77474,23 +77483,23 @@
       </c>
       <c r="BB16" s="34">
         <f t="shared" si="34"/>
-        <v>3.1381150689362376E-2</v>
+        <v>2.9394054156409759E-2</v>
       </c>
       <c r="BC16" s="32">
         <f t="shared" si="35"/>
-        <v>0.69720761862330161</v>
+        <v>0.9123478147762748</v>
       </c>
       <c r="BD16" s="37">
         <f t="shared" si="36"/>
-        <v>8.1006016668195464</v>
+        <v>9.8377846860908775</v>
       </c>
       <c r="BE16" s="53">
         <f t="shared" si="17"/>
-        <v>0.95301196080229955</v>
+        <v>0.9837784686090878</v>
       </c>
       <c r="BF16" s="38">
         <f t="shared" si="37"/>
-        <v>29.263423521385604</v>
+        <v>27.668769429630593</v>
       </c>
       <c r="BG16" s="34">
         <f t="shared" si="38"/>
@@ -77498,7 +77507,7 @@
       </c>
       <c r="BH16" s="34">
         <f t="shared" si="39"/>
-        <v>6.8586148878247499</v>
+        <v>6.4848678350696689</v>
       </c>
       <c r="BI16" s="32" t="str">
         <f t="shared" si="40"/>
@@ -77506,7 +77515,7 @@
       </c>
       <c r="BJ16" s="38">
         <f t="shared" si="41"/>
-        <v>6.4804813334556375</v>
+        <v>4.4270031087408928</v>
       </c>
       <c r="BK16" s="34">
         <f t="shared" si="42"/>
@@ -77514,7 +77523,7 @@
       </c>
       <c r="BL16" s="34">
         <f t="shared" si="43"/>
-        <v>1.5188628125286647</v>
+        <v>1.0375788536111465</v>
       </c>
       <c r="BM16" s="32" t="str">
         <f t="shared" si="44"/>
@@ -77522,7 +77531,7 @@
       </c>
     </row>
     <row r="17" spans="2:65" x14ac:dyDescent="0.25">
-      <c r="B17" s="29" t="s">
+      <c r="B17" s="95" t="s">
         <v>194</v>
       </c>
       <c r="C17" s="30" t="str">
@@ -77574,26 +77583,26 @@
         <v>0.4995</v>
       </c>
       <c r="O17" s="29">
-        <f>0.4+E17+0.4</f>
-        <v>3.1699999999999995</v>
+        <f>0.3+E17+0.3</f>
+        <v>2.9699999999999993</v>
       </c>
       <c r="P17" s="30">
-        <v>1.7</v>
+        <v>1.5</v>
       </c>
       <c r="Q17" s="30">
         <v>1.6</v>
       </c>
       <c r="R17" s="34">
         <f t="shared" si="18"/>
-        <v>21.555999999999997</v>
+        <v>17.819999999999997</v>
       </c>
       <c r="S17" s="32">
         <f t="shared" si="19"/>
-        <v>0.52833333333333321</v>
+        <v>0.49499999999999988</v>
       </c>
       <c r="U17" s="33">
         <f t="shared" si="0"/>
-        <v>258.35989999999998</v>
+        <v>254.62389999999999</v>
       </c>
       <c r="V17" s="34">
         <f t="shared" si="20"/>
@@ -77601,15 +77610,15 @@
       </c>
       <c r="W17" s="35">
         <f t="shared" si="21"/>
-        <v>1.2288284675756571E-2</v>
+        <v>1.246858602040107E-2</v>
       </c>
       <c r="X17" s="32">
         <f t="shared" si="45"/>
-        <v>4.9057150709501132</v>
+        <v>5.8594306930131861</v>
       </c>
       <c r="Y17" s="33">
         <f t="shared" si="1"/>
-        <v>310.74429999999995</v>
+        <v>307.00829999999996</v>
       </c>
       <c r="Z17" s="34">
         <f t="shared" si="2"/>
@@ -77617,24 +77626,24 @@
       </c>
       <c r="AA17" s="35">
         <f t="shared" si="22"/>
-        <v>1.1135522035319716E-2</v>
+        <v>1.1271030783206839E-2</v>
       </c>
       <c r="AB17" s="32">
         <f t="shared" si="23"/>
-        <v>5.8878041143514102</v>
+        <v>7.0482335589338971</v>
       </c>
       <c r="AC17" s="53">
         <f t="shared" si="90"/>
-        <v>0.75472539553078666</v>
+        <v>0.73242883662664826</v>
       </c>
       <c r="AD17" s="53">
         <f t="shared" si="91"/>
-        <v>0.90581601759252461</v>
+        <v>0.88102919486673714</v>
       </c>
       <c r="AE17" s="36"/>
       <c r="AF17" s="38">
         <f t="shared" si="5"/>
-        <v>332.46429999999998</v>
+        <v>328.72829999999999</v>
       </c>
       <c r="AG17" s="34">
         <f t="shared" si="6"/>
@@ -77642,15 +77651,15 @@
       </c>
       <c r="AH17" s="34">
         <f t="shared" si="24"/>
-        <v>8.9711887862847228E-3</v>
+        <v>9.0731464251784834E-3</v>
       </c>
       <c r="AI17" s="32">
         <f t="shared" si="25"/>
-        <v>6.2740693947771868</v>
+        <v>7.5141134578104287</v>
       </c>
       <c r="AJ17" s="38">
         <f t="shared" si="7"/>
-        <v>184.25549999999998</v>
+        <v>180.51949999999999</v>
       </c>
       <c r="AK17" s="34">
         <f t="shared" si="8"/>
@@ -77658,15 +77667,15 @@
       </c>
       <c r="AL17" s="34">
         <f t="shared" si="26"/>
-        <v>1.8273538646064839E-2</v>
+        <v>1.8651724605928999E-2</v>
       </c>
       <c r="AM17" s="32">
         <f t="shared" si="27"/>
-        <v>3.5373607471230386</v>
+        <v>4.2047479282159426</v>
       </c>
       <c r="AN17" s="38">
         <f t="shared" si="9"/>
-        <v>353.22649999999999</v>
+        <v>349.4905</v>
       </c>
       <c r="AO17" s="34">
         <f t="shared" si="10"/>
@@ -77674,15 +77683,15 @@
       </c>
       <c r="AP17" s="34">
         <f t="shared" si="28"/>
-        <v>9.1861029679256787E-3</v>
+        <v>9.2843010038899474E-3</v>
       </c>
       <c r="AQ17" s="32">
         <f t="shared" si="29"/>
-        <v>6.6685475963713916</v>
+        <v>7.9920449160516513</v>
       </c>
       <c r="AR17" s="38">
         <f t="shared" si="11"/>
-        <v>242.06989999999996</v>
+        <v>238.33389999999997</v>
       </c>
       <c r="AS17" s="34">
         <f t="shared" si="12"/>
@@ -77690,15 +77699,15 @@
       </c>
       <c r="AT17" s="34">
         <f t="shared" si="30"/>
-        <v>1.4595267730519163E-2</v>
+        <v>1.4824055663084441E-2</v>
       </c>
       <c r="AU17" s="32">
         <f t="shared" si="31"/>
-        <v>4.6160161106307802</v>
+        <v>5.510020768855787</v>
       </c>
       <c r="AV17" s="38">
         <f t="shared" si="13"/>
-        <v>229.12034</v>
+        <v>226.87873999999999</v>
       </c>
       <c r="AW17" s="34">
         <f t="shared" si="14"/>
@@ -77706,15 +77715,15 @@
       </c>
       <c r="AX17" s="34">
         <f t="shared" si="32"/>
-        <v>7.4750238237251219E-3</v>
+        <v>7.5488783127057209E-3</v>
       </c>
       <c r="AY17" s="32">
         <f t="shared" si="33"/>
-        <v>4.3117833663971421</v>
+        <v>5.1703411806051545</v>
       </c>
       <c r="AZ17" s="38">
         <f t="shared" si="15"/>
-        <v>80.911540000000002</v>
+        <v>78.669939999999997</v>
       </c>
       <c r="BA17" s="34">
         <f t="shared" si="16"/>
@@ -77722,23 +77731,23 @@
       </c>
       <c r="BB17" s="34">
         <f t="shared" si="34"/>
-        <v>2.5918181757509498E-2</v>
+        <v>2.6656687420887826E-2</v>
       </c>
       <c r="BC17" s="32">
         <f t="shared" si="35"/>
-        <v>1.5750747187429941</v>
+        <v>1.8609756510106681</v>
       </c>
       <c r="BD17" s="37">
         <f t="shared" si="36"/>
-        <v>6.6685475963713916</v>
+        <v>7.9920449160516513</v>
       </c>
       <c r="BE17" s="53">
         <f t="shared" si="17"/>
-        <v>0.78453501133781078</v>
+        <v>0.79920449160516516</v>
       </c>
       <c r="BF17" s="38">
         <f t="shared" si="37"/>
-        <v>24.090128191891647</v>
+        <v>22.477626326395267</v>
       </c>
       <c r="BG17" s="34">
         <f t="shared" si="38"/>
@@ -77746,7 +77755,7 @@
       </c>
       <c r="BH17" s="34">
         <f t="shared" si="39"/>
-        <v>5.6461237949746037</v>
+        <v>5.2681936702488894</v>
       </c>
       <c r="BI17" s="32" t="str">
         <f t="shared" si="40"/>
@@ -77754,7 +77763,7 @@
       </c>
       <c r="BJ17" s="38">
         <f t="shared" si="41"/>
-        <v>5.3348380770971104</v>
+        <v>3.5964202122232392</v>
       </c>
       <c r="BK17" s="34">
         <f t="shared" si="42"/>
@@ -77762,7 +77771,7 @@
       </c>
       <c r="BL17" s="34">
         <f t="shared" si="43"/>
-        <v>1.2503526743196349</v>
+        <v>0.8429109872398215</v>
       </c>
       <c r="BM17" s="32" t="str">
         <f t="shared" si="44"/>
@@ -77873,11 +77882,11 @@
       </c>
       <c r="AC18" s="53">
         <f t="shared" si="90"/>
-        <v>0.31716780045351478</v>
+        <v>0.25769883786848075</v>
       </c>
       <c r="AD18" s="53">
         <f t="shared" si="91"/>
-        <v>0.54132908890051745</v>
+        <v>0.43982988473167045</v>
       </c>
       <c r="AE18" s="36"/>
       <c r="AF18" s="38">
@@ -77982,7 +77991,7 @@
       </c>
       <c r="BE18" s="53">
         <f t="shared" si="17"/>
-        <v>0.37237880152060832</v>
+        <v>0.31652198129251707</v>
       </c>
       <c r="BF18" s="38">
         <f t="shared" si="37"/>
@@ -78121,11 +78130,11 @@
       </c>
       <c r="AC19" s="53">
         <f t="shared" si="90"/>
-        <v>0.77693645584384408</v>
+        <v>0.63126087037312328</v>
       </c>
       <c r="AD19" s="53">
         <f t="shared" si="91"/>
-        <v>0.95101152836064395</v>
+        <v>0.77269686679302318</v>
       </c>
       <c r="AE19" s="36"/>
       <c r="AF19" s="38">
@@ -78230,7 +78239,7 @@
       </c>
       <c r="BE19" s="53">
         <f t="shared" si="17"/>
-        <v>0.96313197365314518</v>
+        <v>0.81866217760517335</v>
       </c>
       <c r="BF19" s="38">
         <f t="shared" si="37"/>
@@ -78369,11 +78378,11 @@
       </c>
       <c r="AC20" s="53">
         <f t="shared" si="90"/>
-        <v>0.71555639078314814</v>
+        <v>0.58138956751130788</v>
       </c>
       <c r="AD20" s="53">
         <f t="shared" si="91"/>
-        <v>0.86572117749555411</v>
+        <v>0.70339845671513768</v>
       </c>
       <c r="AE20" s="36"/>
       <c r="AF20" s="38">
@@ -78478,7 +78487,7 @@
       </c>
       <c r="BE20" s="53">
         <f t="shared" si="17"/>
-        <v>0.73671974301184329</v>
+        <v>0.62621178156006674</v>
       </c>
       <c r="BF20" s="38">
         <f t="shared" si="37"/>
@@ -78618,11 +78627,11 @@
       </c>
       <c r="AC21" s="53">
         <f t="shared" si="90"/>
-        <v>0.42901486924121607</v>
+        <v>0.34857458125848806</v>
       </c>
       <c r="AD21" s="53">
         <f t="shared" si="91"/>
-        <v>0.52987294865991119</v>
+        <v>0.43052177078617787</v>
       </c>
       <c r="AE21" s="36"/>
       <c r="AF21" s="38">
@@ -78727,7 +78736,7 @@
       </c>
       <c r="BE21" s="53">
         <f t="shared" si="17"/>
-        <v>0.4582102654914389</v>
+        <v>0.38947872566772307</v>
       </c>
       <c r="BF21" s="38">
         <f t="shared" si="37"/>
@@ -78867,11 +78876,11 @@
       </c>
       <c r="AC22" s="53">
         <f t="shared" si="90"/>
-        <v>0.74221088544278657</v>
+        <v>0.60304634442226412</v>
       </c>
       <c r="AD22" s="53">
         <f t="shared" si="91"/>
-        <v>0.80488941017854343</v>
+        <v>0.65397264577006653</v>
       </c>
       <c r="AE22" s="36"/>
       <c r="AF22" s="38">
@@ -78976,7 +78985,7 @@
       </c>
       <c r="BE22" s="53">
         <f t="shared" si="17"/>
-        <v>0.63247046612609648</v>
+        <v>0.53759989620718207</v>
       </c>
       <c r="BF22" s="38">
         <f t="shared" si="37"/>
@@ -79116,11 +79125,11 @@
       </c>
       <c r="AC23" s="53">
         <f t="shared" si="90"/>
-        <v>0.35336731193384185</v>
+        <v>0.28711094094624651</v>
       </c>
       <c r="AD23" s="53">
         <f t="shared" si="91"/>
-        <v>0.42782581895396904</v>
+        <v>0.34760847790009985</v>
       </c>
       <c r="AE23" s="36"/>
       <c r="AF23" s="38">
@@ -79225,7 +79234,7 @@
       </c>
       <c r="BE23" s="53">
         <f t="shared" si="17"/>
-        <v>0.33905390551974834</v>
+        <v>0.28819581969178609</v>
       </c>
       <c r="BF23" s="38">
         <f t="shared" si="37"/>
@@ -79365,11 +79374,11 @@
       </c>
       <c r="AC24" s="53">
         <f t="shared" si="90"/>
-        <v>0.48314789796183649</v>
+        <v>0.39255766709399215</v>
       </c>
       <c r="AD24" s="53">
         <f t="shared" si="91"/>
-        <v>0.61797844844974947</v>
+        <v>0.50210748936542149</v>
       </c>
       <c r="AE24" s="36"/>
       <c r="AF24" s="38">
@@ -79474,7 +79483,7 @@
       </c>
       <c r="BE24" s="53">
         <f t="shared" si="17"/>
-        <v>0.55718685151352076</v>
+        <v>0.47360882378649266</v>
       </c>
       <c r="BF24" s="38">
         <f t="shared" si="37"/>
@@ -79614,11 +79623,11 @@
       </c>
       <c r="AC25" s="53">
         <f t="shared" si="90"/>
-        <v>0.51999416689521771</v>
+        <v>0.42249526060236436</v>
       </c>
       <c r="AD25" s="53">
         <f t="shared" si="91"/>
-        <v>0.60783438370599185</v>
+        <v>0.49386543676111838</v>
       </c>
       <c r="AE25" s="36"/>
       <c r="AF25" s="38">
@@ -79723,7 +79732,7 @@
       </c>
       <c r="BE25" s="53">
         <f t="shared" si="17"/>
-        <v>0.48656206108639743</v>
+        <v>0.41357775192343782</v>
       </c>
       <c r="BF25" s="38">
         <f t="shared" si="37"/>
@@ -79810,7 +79819,7 @@
         <f>'MUROS EJE Y'!N4</f>
         <v>0.97950000000000004</v>
       </c>
-      <c r="O26" s="90">
+      <c r="O26" s="65">
         <f t="shared" si="89"/>
         <v>36.380999999999993</v>
       </c>
@@ -79862,11 +79871,11 @@
       </c>
       <c r="AC26" s="53">
         <f t="shared" si="90"/>
-        <v>0.1227738687473004</v>
+        <v>9.9753768357181569E-2</v>
       </c>
       <c r="AD26" s="53">
         <f t="shared" si="91"/>
-        <v>0.15296024548129841</v>
+        <v>0.12428019945355495</v>
       </c>
       <c r="AE26" s="36"/>
       <c r="AF26" s="56">
@@ -79971,7 +79980,7 @@
       </c>
       <c r="BE26" s="53">
         <f t="shared" si="17"/>
-        <v>0.11960764734031874</v>
+        <v>0.10166650023927093</v>
       </c>
       <c r="BF26" s="56">
         <f t="shared" si="37"/>
@@ -80110,11 +80119,11 @@
       </c>
       <c r="AC27" s="53">
         <f t="shared" si="90"/>
-        <v>0.58946311433012255</v>
+        <v>0.47893878039322457</v>
       </c>
       <c r="AD27" s="53">
         <f t="shared" si="91"/>
-        <v>0.70132639900383276</v>
+        <v>0.56982769919061416</v>
       </c>
       <c r="AE27" s="36"/>
       <c r="AF27" s="38">
@@ -80219,7 +80228,7 @@
       </c>
       <c r="BE27" s="53">
         <f t="shared" si="17"/>
-        <v>0.55758329026023912</v>
+        <v>0.47394579672120329</v>
       </c>
       <c r="BF27" s="38">
         <f t="shared" si="37"/>
@@ -80358,11 +80367,11 @@
       </c>
       <c r="AC28" s="53">
         <f t="shared" si="90"/>
-        <v>0.7879052307692308</v>
+        <v>0.64017299999999999</v>
       </c>
       <c r="AD28" s="53">
         <f t="shared" si="91"/>
-        <v>0.94486130620061537</v>
+        <v>0.76769981128800002</v>
       </c>
       <c r="AE28" s="36"/>
       <c r="AF28" s="38">
@@ -80467,7 +80476,7 @@
       </c>
       <c r="BE28" s="53">
         <f t="shared" si="17"/>
-        <v>0.83052431385035297</v>
+        <v>0.70594566677280002</v>
       </c>
       <c r="BF28" s="38">
         <f t="shared" si="37"/>
@@ -80606,11 +80615,11 @@
       </c>
       <c r="AC29" s="53">
         <f t="shared" si="90"/>
-        <v>0.76418805451385718</v>
+        <v>0.62090279429250894</v>
       </c>
       <c r="AD29" s="53">
         <f t="shared" si="91"/>
-        <v>0.94823216735701898</v>
+        <v>0.77043863597757789</v>
       </c>
       <c r="AE29" s="36"/>
       <c r="AF29" s="38">
@@ -80715,7 +80724,7 @@
       </c>
       <c r="BE29" s="53">
         <f t="shared" si="17"/>
-        <v>0.80463557289741117</v>
+        <v>0.68394023696279949</v>
       </c>
       <c r="BF29" s="38">
         <f t="shared" si="37"/>
@@ -80854,11 +80863,11 @@
       </c>
       <c r="AC30" s="53">
         <f t="shared" si="90"/>
-        <v>0.80067899968344414</v>
+        <v>0.65055168724279833</v>
       </c>
       <c r="AD30" s="53">
         <f t="shared" si="91"/>
-        <v>0.97702663712145188</v>
+        <v>0.79383414266117969</v>
       </c>
       <c r="AE30" s="36"/>
       <c r="AF30" s="38">
@@ -80963,7 +80972,7 @@
       </c>
       <c r="BE30" s="53">
         <f t="shared" si="17"/>
-        <v>0.73261395787944805</v>
+        <v>0.62272186419753084</v>
       </c>
       <c r="BF30" s="38">
         <f t="shared" si="37"/>
@@ -81102,11 +81111,11 @@
       </c>
       <c r="AC31" s="53">
         <f t="shared" si="90"/>
-        <v>0.43528972457780463</v>
+        <v>0.35367290121946626</v>
       </c>
       <c r="AD31" s="53">
         <f t="shared" si="91"/>
-        <v>0.53844055391332291</v>
+        <v>0.43748295005457488</v>
       </c>
       <c r="AE31" s="36"/>
       <c r="AF31" s="38">
@@ -81211,7 +81220,7 @@
       </c>
       <c r="BE31" s="53">
         <f t="shared" si="17"/>
-        <v>0.59331402585498794</v>
+        <v>0.50431692197673983</v>
       </c>
       <c r="BF31" s="38">
         <f t="shared" si="37"/>
@@ -81350,11 +81359,11 @@
       </c>
       <c r="AC32" s="53">
         <f t="shared" si="90"/>
-        <v>0.74870063028867928</v>
+        <v>0.60831926210955189</v>
       </c>
       <c r="AD32" s="53">
         <f t="shared" si="91"/>
-        <v>0.90485943517776946</v>
+        <v>0.73519829108193768</v>
       </c>
       <c r="AE32" s="36"/>
       <c r="AF32" s="38">
@@ -81459,7 +81468,7 @@
       </c>
       <c r="BE32" s="53">
         <f t="shared" si="17"/>
-        <v>0.84369600830825775</v>
+        <v>0.71714160706201913</v>
       </c>
       <c r="BF32" s="38">
         <f t="shared" si="37"/>
@@ -81598,11 +81607,11 @@
       </c>
       <c r="AC33" s="53">
         <f t="shared" si="90"/>
-        <v>0.78850057223078451</v>
+        <v>0.64065671493751242</v>
       </c>
       <c r="AD33" s="53">
         <f t="shared" si="91"/>
-        <v>0.96518306044283031</v>
+        <v>0.78421123660979963</v>
       </c>
       <c r="AE33" s="36"/>
       <c r="AF33" s="38">
@@ -81707,7 +81716,7 @@
       </c>
       <c r="BE33" s="53">
         <f t="shared" si="17"/>
-        <v>0.76136253165221657</v>
+        <v>0.64715815190438408</v>
       </c>
       <c r="BF33" s="38">
         <f t="shared" si="37"/>
@@ -81846,11 +81855,11 @@
       </c>
       <c r="AC34" s="53">
         <f t="shared" si="90"/>
-        <v>0.80520147206863146</v>
+        <v>0.65422619605576304</v>
       </c>
       <c r="AD34" s="53">
         <f t="shared" si="91"/>
-        <v>0.99369123011948246</v>
+        <v>0.80737412447207946</v>
       </c>
       <c r="AE34" s="36"/>
       <c r="AF34" s="38">
@@ -81955,7 +81964,7 @@
       </c>
       <c r="BE34" s="53">
         <f t="shared" si="17"/>
-        <v>0.75975732119778505</v>
+        <v>0.64579372301811733</v>
       </c>
       <c r="BF34" s="38">
         <f t="shared" si="37"/>
@@ -82094,11 +82103,11 @@
       </c>
       <c r="AC35" s="53">
         <f t="shared" si="90"/>
-        <v>0.74235804195804189</v>
+        <v>0.60316590909090906</v>
       </c>
       <c r="AD35" s="53">
         <f t="shared" si="91"/>
-        <v>0.9266284382284381</v>
+        <v>0.75288560606060595</v>
       </c>
       <c r="AE35" s="36"/>
       <c r="AF35" s="38">
@@ -82203,7 +82212,7 @@
       </c>
       <c r="BE35" s="53">
         <f t="shared" si="17"/>
-        <v>0.7996602495543671</v>
+        <v>0.6797112121212121</v>
       </c>
       <c r="BF35" s="38">
         <f t="shared" si="37"/>
@@ -82342,11 +82351,11 @@
       </c>
       <c r="AC36" s="53">
         <f t="shared" si="90"/>
-        <v>0.75415248247590683</v>
+        <v>0.61274889201167426</v>
       </c>
       <c r="AD36" s="53">
         <f t="shared" si="91"/>
-        <v>0.92110964965050202</v>
+        <v>0.74840159034103293</v>
       </c>
       <c r="AE36" s="36"/>
       <c r="AF36" s="38">
@@ -82451,7 +82460,7 @@
       </c>
       <c r="BE36" s="53">
         <f t="shared" si="17"/>
-        <v>0.77967578405267612</v>
+        <v>0.66272441644477476</v>
       </c>
       <c r="BF36" s="38">
         <f t="shared" si="37"/>
@@ -82590,11 +82599,11 @@
       </c>
       <c r="AC37" s="53">
         <f t="shared" si="90"/>
-        <v>0.71223152498176912</v>
+        <v>0.57868811404768739</v>
       </c>
       <c r="AD37" s="53">
         <f t="shared" si="91"/>
-        <v>0.85484057189578599</v>
+        <v>0.69455796466532616</v>
       </c>
       <c r="AE37" s="36"/>
       <c r="AF37" s="38">
@@ -82699,7 +82708,7 @@
       </c>
       <c r="BE37" s="53">
         <f t="shared" si="17"/>
-        <v>0.74737770079591725</v>
+        <v>0.6352710456765297</v>
       </c>
       <c r="BF37" s="38">
         <f t="shared" si="37"/>
@@ -82838,11 +82847,11 @@
       </c>
       <c r="AC38" s="53">
         <f t="shared" si="90"/>
-        <v>0.79672756684448798</v>
+        <v>0.64734114806114651</v>
       </c>
       <c r="AD38" s="53">
         <f t="shared" si="91"/>
-        <v>0.96788762118213301</v>
+        <v>0.78640869221048304</v>
       </c>
       <c r="AE38" s="36"/>
       <c r="AF38" s="38">
@@ -82947,7 +82956,7 @@
       </c>
       <c r="BE38" s="53">
         <f t="shared" si="17"/>
-        <v>0.76244614298571345</v>
+        <v>0.64807922153785635</v>
       </c>
       <c r="BF38" s="38">
         <f t="shared" si="37"/>
@@ -83086,11 +83095,11 @@
       </c>
       <c r="AC39" s="53">
         <f t="shared" si="90"/>
-        <v>0.17336785439783012</v>
+        <v>0.14086138169823698</v>
       </c>
       <c r="AD39" s="53">
         <f t="shared" si="91"/>
-        <v>0.21361305505188843</v>
+        <v>0.17356060722965935</v>
       </c>
       <c r="AE39" s="36"/>
       <c r="AF39" s="38">
@@ -83195,7 +83204,7 @@
       </c>
       <c r="BE39" s="53">
         <f t="shared" si="17"/>
-        <v>0.19531750488475169</v>
+        <v>0.16601987915203892</v>
       </c>
       <c r="BF39" s="38">
         <f t="shared" si="37"/>
@@ -83334,11 +83343,11 @@
       </c>
       <c r="AC40" s="53">
         <f t="shared" si="90"/>
-        <v>0.53522213988271017</v>
+        <v>0.43486798865470205</v>
       </c>
       <c r="AD40" s="53">
         <f t="shared" si="91"/>
-        <v>0.68854738053769815</v>
+        <v>0.55944474668687971</v>
       </c>
       <c r="AE40" s="36"/>
       <c r="AF40" s="38">
@@ -83443,7 +83452,7 @@
       </c>
       <c r="BE40" s="53">
         <f t="shared" si="17"/>
-        <v>0.63640058337384542</v>
+        <v>0.5409404958677686</v>
       </c>
       <c r="BF40" s="38">
         <f t="shared" si="37"/>
@@ -83582,11 +83591,11 @@
       </c>
       <c r="AC41" s="53">
         <f t="shared" si="90"/>
-        <v>0.53807694137016371</v>
+        <v>0.43718751486325802</v>
       </c>
       <c r="AD41" s="53">
         <f t="shared" si="91"/>
-        <v>0.69812735754138855</v>
+        <v>0.56722847800237819</v>
       </c>
       <c r="AE41" s="36"/>
       <c r="AF41" s="38">
@@ -83691,7 +83700,7 @@
       </c>
       <c r="BE41" s="53">
         <f t="shared" si="17"/>
-        <v>0.5896033923200672</v>
+        <v>0.50116288347205706</v>
       </c>
       <c r="BF41" s="38">
         <f t="shared" si="37"/>
@@ -83830,11 +83839,11 @@
       </c>
       <c r="AC42" s="53">
         <f t="shared" si="90"/>
-        <v>0.80198168658720936</v>
+        <v>0.65161012035210764</v>
       </c>
       <c r="AD42" s="53">
         <f t="shared" si="91"/>
-        <v>0.9921888995656255</v>
+        <v>0.80615348089707073</v>
       </c>
       <c r="AE42" s="36"/>
       <c r="AF42" s="38">
@@ -83939,7 +83948,7 @@
       </c>
       <c r="BE42" s="53">
         <f t="shared" si="17"/>
-        <v>0.85980840670697389</v>
+        <v>0.73083714570092773</v>
       </c>
       <c r="BF42" s="38">
         <f t="shared" si="37"/>
@@ -84078,11 +84087,11 @@
       </c>
       <c r="AC43" s="53">
         <f t="shared" si="90"/>
-        <v>7.2281358150356273E-2</v>
+        <v>5.8728603497164467E-2</v>
       </c>
       <c r="AD43" s="53">
         <f t="shared" si="91"/>
-        <v>8.0907052493819992E-2</v>
+        <v>6.5736980151228738E-2</v>
       </c>
       <c r="AE43" s="36"/>
       <c r="AF43" s="38">
@@ -84187,7 +84196,7 @@
       </c>
       <c r="BE43" s="53">
         <f t="shared" si="17"/>
-        <v>8.2470299121538984E-2</v>
+        <v>7.0099754253308139E-2</v>
       </c>
       <c r="BF43" s="38">
         <f t="shared" si="37"/>
@@ -84326,11 +84335,11 @@
       </c>
       <c r="AC44" s="53">
         <f t="shared" si="90"/>
-        <v>0.5080183138284815</v>
+        <v>0.41276487998564126</v>
       </c>
       <c r="AD44" s="53">
         <f t="shared" si="91"/>
-        <v>0.52748654041062637</v>
+        <v>0.42858281408363397</v>
       </c>
       <c r="AE44" s="36"/>
       <c r="AF44" s="38">
@@ -84435,7 +84444,7 @@
       </c>
       <c r="BE44" s="53">
         <f t="shared" si="17"/>
-        <v>0.3997723090750433</v>
+        <v>0.33980646271378678</v>
       </c>
       <c r="BF44" s="38">
         <f t="shared" si="37"/>
@@ -84522,7 +84531,7 @@
         <f>'MUROS EJE Y'!N23</f>
         <v>1.3401000000000001</v>
       </c>
-      <c r="O45" s="91">
+      <c r="O45" s="66">
         <f t="shared" si="89"/>
         <v>38.881999999999991</v>
       </c>
@@ -84574,11 +84583,11 @@
       </c>
       <c r="AC45" s="53">
         <f t="shared" si="90"/>
-        <v>0.13116749868153516</v>
+        <v>0.1065735926787473</v>
       </c>
       <c r="AD45" s="53">
         <f t="shared" si="91"/>
-        <v>0.13935022585599485</v>
+        <v>0.11322205850799583</v>
       </c>
       <c r="AE45" s="36"/>
       <c r="AF45" s="58">
@@ -84683,7 +84692,7 @@
       </c>
       <c r="BE45" s="53">
         <f t="shared" si="17"/>
-        <v>0.10715459959959492</v>
+        <v>9.1081409659655679E-2</v>
       </c>
       <c r="BF45" s="58">
         <f t="shared" si="37"/>
@@ -84827,16 +84836,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="G5:J5"/>
-    <mergeCell ref="K5:N5"/>
-    <mergeCell ref="O5:S5"/>
-    <mergeCell ref="U5:X5"/>
-    <mergeCell ref="Y5:AB5"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="U4:AB4"/>
-    <mergeCell ref="AF4:BD4"/>
-    <mergeCell ref="BF4:BM4"/>
     <mergeCell ref="BD5:BD6"/>
     <mergeCell ref="BF5:BI5"/>
     <mergeCell ref="BJ5:BM5"/>
@@ -84846,6 +84845,16 @@
     <mergeCell ref="AR5:AU5"/>
     <mergeCell ref="AV5:AY5"/>
     <mergeCell ref="AZ5:BC5"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="U4:AB4"/>
+    <mergeCell ref="AF4:BD4"/>
+    <mergeCell ref="BF4:BM4"/>
+    <mergeCell ref="G5:J5"/>
+    <mergeCell ref="K5:N5"/>
+    <mergeCell ref="O5:S5"/>
+    <mergeCell ref="U5:X5"/>
+    <mergeCell ref="Y5:AB5"/>
   </mergeCells>
   <conditionalFormatting sqref="BI7">
     <cfRule type="containsText" dxfId="11" priority="36" operator="containsText" text="NO PARRILLA">

</xml_diff>

<commit_message>
Zapatas listas, falta verificar FSV y FSD
</commit_message>
<xml_diff>
--- a/Tarea 07/muros-fundaciones.xlsx
+++ b/Tarea 07/muros-fundaciones.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DBE51CE-F0D7-4528-8AA3-EA9BD0991DB6}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{607B2BD1-DF19-4B4A-881E-DF62EBEA384D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="697" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,35 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Tuve que aumentarle mucho el tamaño para alcanzar sufiviente masa para contorlar las tracciones</t>
+          <t>Resulta con esfuerzos negativos</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B43" authorId="0" shapeId="0" xr:uid="{E295C206-4979-49BC-A7C5-C75A854C0C9E}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Resulta con esfuerzos negativos</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B44" authorId="0" shapeId="0" xr:uid="{C01114D8-1194-4480-845A-A30214A34D4F}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Resulta con esfuerzos negativos</t>
         </r>
       </text>
     </comment>
@@ -691,7 +719,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -713,12 +741,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1181,7 +1203,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="105">
+  <cellXfs count="104">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1468,19 +1490,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1489,10 +1502,16 @@
     <xf numFmtId="164" fontId="3" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -73413,7 +73432,7 @@
   <dimension ref="B2:R23"/>
   <sheetViews>
     <sheetView topLeftCell="C4" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -74592,7 +74611,7 @@
         <v>F38Y</v>
       </c>
       <c r="E22" s="10">
-        <v>8.6199999999999992</v>
+        <v>8.64</v>
       </c>
       <c r="F22" s="9">
         <v>0.3</v>
@@ -74708,11 +74727,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AA70DD8-84E8-4BDF-9E1A-DF05C3E71277}">
   <dimension ref="A1:BM50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="17" ySplit="6" topLeftCell="R27" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="R1" sqref="R1"/>
-      <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="P43" sqref="P43"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -74722,61 +74738,61 @@
     <col min="3" max="3" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.85546875" style="1" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="14.5703125" style="1" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="18.85546875" style="1" hidden="1" customWidth="1"/>
-    <col min="9" max="10" width="15.7109375" style="1" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="30.28515625" style="1" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="30.140625" style="1" hidden="1" customWidth="1"/>
-    <col min="13" max="14" width="28.7109375" style="1" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="14.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="14.5703125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="18.85546875" style="1" customWidth="1"/>
+    <col min="9" max="10" width="15.7109375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="30.28515625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="30.140625" style="1" customWidth="1"/>
+    <col min="13" max="14" width="28.7109375" style="1" customWidth="1"/>
     <col min="15" max="15" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="16" max="17" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="20.28515625" style="49" hidden="1" customWidth="1"/>
-    <col min="19" max="19" width="9.5703125" style="49" hidden="1" customWidth="1"/>
-    <col min="20" max="20" width="2.85546875" style="1" hidden="1" customWidth="1"/>
-    <col min="21" max="21" width="19.7109375" style="1" hidden="1" customWidth="1"/>
-    <col min="22" max="22" width="20" style="1" hidden="1" customWidth="1"/>
-    <col min="23" max="23" width="16.85546875" style="1" hidden="1" customWidth="1"/>
+    <col min="18" max="18" width="20.28515625" style="49" customWidth="1"/>
+    <col min="19" max="19" width="9.5703125" style="49" customWidth="1"/>
+    <col min="20" max="20" width="2.85546875" style="1" customWidth="1"/>
+    <col min="21" max="21" width="19.7109375" style="1" customWidth="1"/>
+    <col min="22" max="22" width="20" style="1" customWidth="1"/>
+    <col min="23" max="23" width="16.85546875" style="1" customWidth="1"/>
     <col min="24" max="24" width="31.140625" style="1" customWidth="1"/>
-    <col min="25" max="25" width="19.7109375" style="1" hidden="1" customWidth="1"/>
-    <col min="26" max="26" width="20" style="1" hidden="1" customWidth="1"/>
-    <col min="27" max="27" width="16.85546875" style="1" hidden="1" customWidth="1"/>
+    <col min="25" max="25" width="19.7109375" style="1" customWidth="1"/>
+    <col min="26" max="26" width="20" style="1" customWidth="1"/>
+    <col min="27" max="27" width="16.85546875" style="1" customWidth="1"/>
     <col min="28" max="28" width="31.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="8.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="2.85546875" style="16" hidden="1" customWidth="1"/>
-    <col min="32" max="32" width="20.28515625" style="49" hidden="1" customWidth="1"/>
-    <col min="33" max="33" width="30" style="49" hidden="1" customWidth="1"/>
-    <col min="34" max="34" width="17.42578125" style="1" hidden="1" customWidth="1"/>
-    <col min="35" max="35" width="32" style="1" hidden="1" customWidth="1"/>
-    <col min="36" max="36" width="20.7109375" style="49" hidden="1" customWidth="1"/>
-    <col min="37" max="37" width="30.28515625" style="49" hidden="1" customWidth="1"/>
-    <col min="38" max="38" width="17.85546875" style="1" hidden="1" customWidth="1"/>
-    <col min="39" max="39" width="32.42578125" style="1" hidden="1" customWidth="1"/>
-    <col min="40" max="40" width="20.7109375" style="49" hidden="1" customWidth="1"/>
-    <col min="41" max="41" width="30.28515625" style="49" hidden="1" customWidth="1"/>
-    <col min="42" max="42" width="17.85546875" style="1" hidden="1" customWidth="1"/>
-    <col min="43" max="43" width="32.42578125" style="1" hidden="1" customWidth="1"/>
-    <col min="44" max="44" width="20.7109375" style="49" hidden="1" customWidth="1"/>
-    <col min="45" max="45" width="30.28515625" style="49" hidden="1" customWidth="1"/>
-    <col min="46" max="46" width="17.85546875" style="1" hidden="1" customWidth="1"/>
-    <col min="47" max="47" width="32.42578125" style="1" hidden="1" customWidth="1"/>
-    <col min="48" max="48" width="20.7109375" style="49" hidden="1" customWidth="1"/>
-    <col min="49" max="49" width="30.28515625" style="49" hidden="1" customWidth="1"/>
-    <col min="50" max="50" width="17.85546875" style="1" hidden="1" customWidth="1"/>
-    <col min="51" max="51" width="32.42578125" style="1" hidden="1" customWidth="1"/>
-    <col min="52" max="52" width="20.7109375" style="49" hidden="1" customWidth="1"/>
-    <col min="53" max="53" width="30.28515625" style="49" hidden="1" customWidth="1"/>
-    <col min="54" max="54" width="17.85546875" style="1" hidden="1" customWidth="1"/>
-    <col min="55" max="55" width="32.42578125" style="1" hidden="1" customWidth="1"/>
+    <col min="30" max="30" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="2.85546875" style="16" customWidth="1"/>
+    <col min="32" max="32" width="20.28515625" style="49" customWidth="1"/>
+    <col min="33" max="33" width="30" style="49" customWidth="1"/>
+    <col min="34" max="34" width="17.42578125" style="1" customWidth="1"/>
+    <col min="35" max="35" width="32" style="1" customWidth="1"/>
+    <col min="36" max="36" width="20.7109375" style="49" customWidth="1"/>
+    <col min="37" max="37" width="30.28515625" style="49" customWidth="1"/>
+    <col min="38" max="38" width="17.85546875" style="1" customWidth="1"/>
+    <col min="39" max="39" width="32.42578125" style="1" customWidth="1"/>
+    <col min="40" max="40" width="20.7109375" style="49" customWidth="1"/>
+    <col min="41" max="41" width="30.28515625" style="49" customWidth="1"/>
+    <col min="42" max="42" width="17.85546875" style="1" customWidth="1"/>
+    <col min="43" max="43" width="32.42578125" style="1" customWidth="1"/>
+    <col min="44" max="44" width="20.7109375" style="49" customWidth="1"/>
+    <col min="45" max="45" width="30.28515625" style="49" customWidth="1"/>
+    <col min="46" max="46" width="17.85546875" style="1" customWidth="1"/>
+    <col min="47" max="47" width="32.42578125" style="1" customWidth="1"/>
+    <col min="48" max="48" width="20.7109375" style="49" customWidth="1"/>
+    <col min="49" max="49" width="30.28515625" style="49" customWidth="1"/>
+    <col min="50" max="50" width="17.85546875" style="1" customWidth="1"/>
+    <col min="51" max="51" width="32.42578125" style="1" customWidth="1"/>
+    <col min="52" max="52" width="20.7109375" style="49" customWidth="1"/>
+    <col min="53" max="53" width="30.28515625" style="49" customWidth="1"/>
+    <col min="54" max="54" width="17.85546875" style="1" customWidth="1"/>
+    <col min="55" max="55" width="32.42578125" style="1" customWidth="1"/>
     <col min="56" max="56" width="30.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="57" max="57" width="8.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="22.5703125" style="49" hidden="1" customWidth="1"/>
-    <col min="59" max="59" width="13" style="1" hidden="1" customWidth="1"/>
+    <col min="58" max="58" width="22.5703125" style="49" customWidth="1"/>
+    <col min="59" max="59" width="13" style="1" customWidth="1"/>
     <col min="60" max="60" width="20.140625" style="1" customWidth="1"/>
     <col min="61" max="61" width="17.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="22.5703125" style="1" hidden="1" customWidth="1"/>
-    <col min="63" max="63" width="13" style="1" hidden="1" customWidth="1"/>
+    <col min="62" max="62" width="22.5703125" style="1" customWidth="1"/>
+    <col min="63" max="63" width="13" style="1" customWidth="1"/>
     <col min="64" max="64" width="20.140625" style="1" customWidth="1"/>
     <col min="65" max="65" width="17.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="66" max="16384" width="8.85546875" style="1"/>
@@ -75134,7 +75150,7 @@
       </c>
     </row>
     <row r="7" spans="2:65" x14ac:dyDescent="0.25">
-      <c r="B7" s="99" t="s">
+      <c r="B7" s="96" t="s">
         <v>194</v>
       </c>
       <c r="C7" s="30" t="str">
@@ -75376,13 +75392,13 @@
         <f>BJ7/BK7/10</f>
         <v>5.5702020148337059</v>
       </c>
-      <c r="BM7" s="101" t="str">
+      <c r="BM7" s="98" t="str">
         <f>IF(BL7&lt;7,"NO PARRILLA","PARRILLA")</f>
         <v>NO PARRILLA</v>
       </c>
     </row>
     <row r="8" spans="2:65" x14ac:dyDescent="0.25">
-      <c r="B8" s="99" t="s">
+      <c r="B8" s="96" t="s">
         <v>194</v>
       </c>
       <c r="C8" s="30" t="str">
@@ -75624,13 +75640,13 @@
         <f>BJ8/BK8/10</f>
         <v>2.5259880573753182</v>
       </c>
-      <c r="BM8" s="101" t="str">
+      <c r="BM8" s="98" t="str">
         <f>IF(BL8&lt;7,"NO PARRILLA","PARRILLA")</f>
         <v>NO PARRILLA</v>
       </c>
     </row>
     <row r="9" spans="2:65" x14ac:dyDescent="0.25">
-      <c r="B9" s="99" t="s">
+      <c r="B9" s="96" t="s">
         <v>194</v>
       </c>
       <c r="C9" s="30" t="str">
@@ -75872,13 +75888,13 @@
         <f t="shared" ref="BL9:BL45" si="43">BJ9/BK9/10</f>
         <v>1.8057457172921936</v>
       </c>
-      <c r="BM9" s="101" t="str">
+      <c r="BM9" s="98" t="str">
         <f t="shared" ref="BM9:BM45" si="44">IF(BL9&lt;7,"NO PARRILLA","PARRILLA")</f>
         <v>NO PARRILLA</v>
       </c>
     </row>
     <row r="10" spans="2:65" x14ac:dyDescent="0.25">
-      <c r="B10" s="99" t="s">
+      <c r="B10" s="96" t="s">
         <v>194</v>
       </c>
       <c r="C10" s="30" t="str">
@@ -76120,13 +76136,13 @@
         <f t="shared" si="43"/>
         <v>2.6448202602726485</v>
       </c>
-      <c r="BM10" s="101" t="str">
+      <c r="BM10" s="98" t="str">
         <f t="shared" si="44"/>
         <v>NO PARRILLA</v>
       </c>
     </row>
     <row r="11" spans="2:65" x14ac:dyDescent="0.25">
-      <c r="B11" s="100" t="s">
+      <c r="B11" s="97" t="s">
         <v>194</v>
       </c>
       <c r="C11" s="30" t="str">
@@ -76368,13 +76384,13 @@
         <f t="shared" si="43"/>
         <v>1.4929134542150453</v>
       </c>
-      <c r="BM11" s="101" t="str">
+      <c r="BM11" s="98" t="str">
         <f t="shared" si="44"/>
         <v>NO PARRILLA</v>
       </c>
     </row>
     <row r="12" spans="2:65" x14ac:dyDescent="0.25">
-      <c r="B12" s="99" t="s">
+      <c r="B12" s="96" t="s">
         <v>194</v>
       </c>
       <c r="C12" s="30" t="str">
@@ -76616,13 +76632,13 @@
         <f t="shared" ref="BL12" si="86">BJ12/BK12/10</f>
         <v>1.7316246196905087</v>
       </c>
-      <c r="BM12" s="101" t="str">
+      <c r="BM12" s="98" t="str">
         <f t="shared" ref="BM12" si="87">IF(BL12&lt;7,"NO PARRILLA","PARRILLA")</f>
         <v>NO PARRILLA</v>
       </c>
     </row>
     <row r="13" spans="2:65" x14ac:dyDescent="0.25">
-      <c r="B13" s="99" t="s">
+      <c r="B13" s="96" t="s">
         <v>194</v>
       </c>
       <c r="C13" s="30" t="str">
@@ -76864,13 +76880,13 @@
         <f t="shared" si="43"/>
         <v>5.5464825444066461</v>
       </c>
-      <c r="BM13" s="101" t="str">
+      <c r="BM13" s="98" t="str">
         <f t="shared" si="44"/>
         <v>NO PARRILLA</v>
       </c>
     </row>
     <row r="14" spans="2:65" x14ac:dyDescent="0.25">
-      <c r="B14" s="99" t="s">
+      <c r="B14" s="96" t="s">
         <v>194</v>
       </c>
       <c r="C14" s="30" t="str">
@@ -77112,13 +77128,13 @@
         <f t="shared" si="43"/>
         <v>1.7304111079617037</v>
       </c>
-      <c r="BM14" s="101" t="str">
+      <c r="BM14" s="98" t="str">
         <f t="shared" si="44"/>
         <v>NO PARRILLA</v>
       </c>
     </row>
     <row r="15" spans="2:65" x14ac:dyDescent="0.25">
-      <c r="B15" s="99" t="s">
+      <c r="B15" s="96" t="s">
         <v>194</v>
       </c>
       <c r="C15" s="30" t="str">
@@ -77344,7 +77360,7 @@
         <f t="shared" si="39"/>
         <v>3.1631819687825184</v>
       </c>
-      <c r="BI15" s="101" t="str">
+      <c r="BI15" s="98" t="str">
         <f t="shared" si="40"/>
         <v>NO PARRILLA</v>
       </c>
@@ -77360,13 +77376,13 @@
         <f t="shared" si="43"/>
         <v>1.8717053069719043</v>
       </c>
-      <c r="BM15" s="101" t="str">
+      <c r="BM15" s="98" t="str">
         <f t="shared" si="44"/>
         <v>NO PARRILLA</v>
       </c>
     </row>
     <row r="16" spans="2:65" x14ac:dyDescent="0.25">
-      <c r="B16" s="99" t="s">
+      <c r="B16" s="96" t="s">
         <v>194</v>
       </c>
       <c r="C16" s="30" t="str">
@@ -77592,7 +77608,7 @@
         <f t="shared" si="39"/>
         <v>4.9249361306805515</v>
       </c>
-      <c r="BI16" s="101" t="str">
+      <c r="BI16" s="98" t="str">
         <f t="shared" si="40"/>
         <v>NO PARRILLA</v>
       </c>
@@ -77608,13 +77624,13 @@
         <f t="shared" si="43"/>
         <v>1.0906432953756242</v>
       </c>
-      <c r="BM16" s="101" t="str">
+      <c r="BM16" s="98" t="str">
         <f t="shared" si="44"/>
         <v>NO PARRILLA</v>
       </c>
     </row>
     <row r="17" spans="2:65" x14ac:dyDescent="0.25">
-      <c r="B17" s="99" t="s">
+      <c r="B17" s="96" t="s">
         <v>194</v>
       </c>
       <c r="C17" s="30" t="str">
@@ -77840,7 +77856,7 @@
         <f t="shared" si="39"/>
         <v>3.9106003570664449</v>
       </c>
-      <c r="BI17" s="101" t="str">
+      <c r="BI17" s="98" t="str">
         <f t="shared" si="40"/>
         <v>NO PARRILLA</v>
       </c>
@@ -77856,13 +77872,13 @@
         <f t="shared" si="43"/>
         <v>0.86601530398703253</v>
       </c>
-      <c r="BM17" s="101" t="str">
+      <c r="BM17" s="98" t="str">
         <f t="shared" si="44"/>
         <v>NO PARRILLA</v>
       </c>
     </row>
     <row r="18" spans="2:65" x14ac:dyDescent="0.25">
-      <c r="B18" s="99" t="s">
+      <c r="B18" s="96" t="s">
         <v>194</v>
       </c>
       <c r="C18" s="30" t="str">
@@ -78088,7 +78104,7 @@
         <f t="shared" si="39"/>
         <v>5.4479005571696124</v>
       </c>
-      <c r="BI18" s="101" t="str">
+      <c r="BI18" s="98" t="str">
         <f t="shared" si="40"/>
         <v>NO PARRILLA</v>
       </c>
@@ -78104,7 +78120,7 @@
         <f t="shared" si="43"/>
         <v>3.0644440634079029</v>
       </c>
-      <c r="BM18" s="101" t="str">
+      <c r="BM18" s="98" t="str">
         <f t="shared" si="44"/>
         <v>NO PARRILLA</v>
       </c>
@@ -78336,7 +78352,7 @@
         <f t="shared" si="39"/>
         <v>4.1014270592915354</v>
       </c>
-      <c r="BI19" s="101" t="str">
+      <c r="BI19" s="98" t="str">
         <f t="shared" si="40"/>
         <v>NO PARRILLA</v>
       </c>
@@ -78352,7 +78368,7 @@
         <f t="shared" si="43"/>
         <v>2.2056563296634466</v>
       </c>
-      <c r="BM19" s="101" t="str">
+      <c r="BM19" s="98" t="str">
         <f t="shared" si="44"/>
         <v>NO PARRILLA</v>
       </c>
@@ -78584,7 +78600,7 @@
         <f t="shared" si="39"/>
         <v>5.8879073077688071</v>
       </c>
-      <c r="BI20" s="101" t="str">
+      <c r="BI20" s="98" t="str">
         <f t="shared" si="40"/>
         <v>NO PARRILLA</v>
       </c>
@@ -78600,7 +78616,7 @@
         <f t="shared" si="43"/>
         <v>2.6168476923416888</v>
       </c>
-      <c r="BM20" s="101" t="str">
+      <c r="BM20" s="98" t="str">
         <f t="shared" si="44"/>
         <v>NO PARRILLA</v>
       </c>
@@ -78833,7 +78849,7 @@
         <f t="shared" si="39"/>
         <v>0.79392482106465467</v>
       </c>
-      <c r="BI21" s="101" t="str">
+      <c r="BI21" s="98" t="str">
         <f t="shared" si="40"/>
         <v>NO PARRILLA</v>
       </c>
@@ -78849,7 +78865,7 @@
         <f t="shared" si="43"/>
         <v>0.25924075789866324</v>
       </c>
-      <c r="BM21" s="101" t="str">
+      <c r="BM21" s="98" t="str">
         <f t="shared" si="44"/>
         <v>NO PARRILLA</v>
       </c>
@@ -79082,7 +79098,7 @@
         <f t="shared" si="39"/>
         <v>4.5107659182868964</v>
       </c>
-      <c r="BI22" s="101" t="str">
+      <c r="BI22" s="98" t="str">
         <f t="shared" si="40"/>
         <v>NO PARRILLA</v>
       </c>
@@ -79098,7 +79114,7 @@
         <f t="shared" si="43"/>
         <v>1.5608186568466769</v>
       </c>
-      <c r="BM22" s="101" t="str">
+      <c r="BM22" s="98" t="str">
         <f t="shared" si="44"/>
         <v>NO PARRILLA</v>
       </c>
@@ -79331,7 +79347,7 @@
         <f t="shared" si="39"/>
         <v>0.59341562503109802</v>
       </c>
-      <c r="BI23" s="101" t="str">
+      <c r="BI23" s="98" t="str">
         <f t="shared" si="40"/>
         <v>NO PARRILLA</v>
       </c>
@@ -79347,7 +79363,7 @@
         <f t="shared" si="43"/>
         <v>0.14835390625777523</v>
       </c>
-      <c r="BM23" s="101" t="str">
+      <c r="BM23" s="98" t="str">
         <f t="shared" si="44"/>
         <v>NO PARRILLA</v>
       </c>
@@ -79580,7 +79596,7 @@
         <f t="shared" si="39"/>
         <v>6.6365821928568893</v>
       </c>
-      <c r="BI24" s="101" t="str">
+      <c r="BI24" s="98" t="str">
         <f t="shared" si="40"/>
         <v>NO PARRILLA</v>
       </c>
@@ -79596,13 +79612,13 @@
         <f t="shared" si="43"/>
         <v>2.3891695894284806</v>
       </c>
-      <c r="BM24" s="101" t="str">
+      <c r="BM24" s="98" t="str">
         <f t="shared" si="44"/>
         <v>NO PARRILLA</v>
       </c>
     </row>
-    <row r="25" spans="2:65" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="96" t="s">
+    <row r="25" spans="2:65" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="70" t="s">
         <v>194</v>
       </c>
       <c r="C25" s="30" t="str">
@@ -79654,27 +79670,27 @@
         <v>335.75560000000002</v>
       </c>
       <c r="O25" s="45">
-        <f t="shared" si="88"/>
-        <v>14.600000000000001</v>
+        <f>0.4+E25+0.15</f>
+        <v>14.55</v>
       </c>
       <c r="P25" s="46">
-        <v>1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="Q25" s="46">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R25" s="57">
         <f t="shared" si="18"/>
-        <v>36.5</v>
+        <v>80.025000000000006</v>
       </c>
       <c r="S25" s="52">
         <f t="shared" si="19"/>
-        <v>2.4333333333333336</v>
+        <v>2.4250000000000003</v>
       </c>
       <c r="T25" s="9"/>
       <c r="U25" s="33">
         <f t="shared" si="0"/>
-        <v>488.78829999999999</v>
+        <v>532.31330000000003</v>
       </c>
       <c r="V25" s="34">
         <f t="shared" si="20"/>
@@ -79682,15 +79698,15 @@
       </c>
       <c r="W25" s="35">
         <f t="shared" si="21"/>
-        <v>2.9153312384932293</v>
+        <v>2.6769569725197546</v>
       </c>
       <c r="X25" s="32">
         <f t="shared" si="45"/>
-        <v>7.4317784168190331</v>
+        <v>7.016335412348579</v>
       </c>
       <c r="Y25" s="33">
         <f t="shared" si="1"/>
-        <v>571.81320000000005</v>
+        <v>615.33820000000003</v>
       </c>
       <c r="Z25" s="34">
         <f t="shared" si="2"/>
@@ -79698,24 +79714,24 @@
       </c>
       <c r="AA25" s="35">
         <f t="shared" si="22"/>
-        <v>2.6113554216656767</v>
+        <v>2.4266452172155084</v>
       </c>
       <c r="AB25" s="32">
         <f t="shared" si="23"/>
-        <v>8.1304691287866238</v>
+        <v>7.6919338442072744</v>
       </c>
       <c r="AC25" s="53">
         <f t="shared" si="89"/>
-        <v>0.92897230210237913</v>
+        <v>0.87704192654357238</v>
       </c>
       <c r="AD25" s="53">
         <f t="shared" si="90"/>
-        <v>1.016308641098328</v>
+        <v>0.9614917305259093</v>
       </c>
       <c r="AE25" s="36"/>
       <c r="AF25" s="38">
         <f t="shared" si="5"/>
-        <v>552.79679999999996</v>
+        <v>596.32180000000005</v>
       </c>
       <c r="AG25" s="34">
         <f t="shared" si="6"/>
@@ -79723,15 +79739,15 @@
       </c>
       <c r="AH25" s="34">
         <f t="shared" si="24"/>
-        <v>1.7580680640698356</v>
+        <v>1.6297482332525828</v>
       </c>
       <c r="AI25" s="32">
         <f t="shared" si="25"/>
-        <v>6.521842597110151</v>
+        <v>6.2298438052541565</v>
       </c>
       <c r="AJ25" s="38">
         <f t="shared" si="7"/>
-        <v>424.77980000000002</v>
+        <v>468.3048</v>
       </c>
       <c r="AK25" s="34">
         <f t="shared" si="8"/>
@@ -79739,15 +79755,15 @@
       </c>
       <c r="AL25" s="34">
         <f t="shared" si="26"/>
-        <v>4.4213618444191551</v>
+        <v>4.0104333758697326</v>
       </c>
       <c r="AM25" s="32">
         <f t="shared" si="27"/>
-        <v>9.8375175353080291</v>
+        <v>8.6939898487967078</v>
       </c>
       <c r="AN25" s="38">
         <f t="shared" si="9"/>
-        <v>599.06335000000001</v>
+        <v>642.5883500000001</v>
       </c>
       <c r="AO25" s="34">
         <f t="shared" si="10"/>
@@ -79755,15 +79771,15 @@
       </c>
       <c r="AP25" s="34">
         <f t="shared" si="28"/>
-        <v>1.8968052794416483</v>
+        <v>1.7683273047200432</v>
       </c>
       <c r="AQ25" s="32">
         <f t="shared" si="29"/>
-        <v>7.3016344811409253</v>
+        <v>6.9426326792207336</v>
       </c>
       <c r="AR25" s="38">
         <f t="shared" si="11"/>
-        <v>503.05059999999997</v>
+        <v>546.57560000000001</v>
       </c>
       <c r="AS25" s="34">
         <f t="shared" si="12"/>
@@ -79771,15 +79787,15 @@
       </c>
       <c r="AT25" s="34">
         <f t="shared" si="30"/>
-        <v>3.6099641368085047</v>
+        <v>3.3224948662179581</v>
       </c>
       <c r="AU25" s="32">
         <f t="shared" si="31"/>
-        <v>9.0884500612037193</v>
+        <v>8.3809616479098104</v>
       </c>
       <c r="AV25" s="38">
         <f t="shared" si="13"/>
-        <v>357.28147999999999</v>
+        <v>383.39648</v>
       </c>
       <c r="AW25" s="34">
         <f t="shared" si="14"/>
@@ -79787,15 +79803,15 @@
       </c>
       <c r="AX25" s="34">
         <f t="shared" si="32"/>
-        <v>1.1247783680251213</v>
+        <v>1.0481642397968809</v>
       </c>
       <c r="AY25" s="32">
         <f t="shared" si="33"/>
-        <v>3.5782907149559007</v>
+        <v>3.4308838900214811</v>
       </c>
       <c r="AZ25" s="38">
         <f t="shared" si="15"/>
-        <v>229.26447999999996</v>
+        <v>255.37947999999997</v>
       </c>
       <c r="BA25" s="34">
         <f t="shared" si="16"/>
@@ -79803,55 +79819,55 @@
       </c>
       <c r="BB25" s="34">
         <f t="shared" si="34"/>
-        <v>5.7056953610956231</v>
+        <v>5.1222333133421687</v>
       </c>
       <c r="BC25" s="32">
         <f t="shared" si="35"/>
-        <v>9.5868118888308516</v>
+        <v>7.1896059792959317</v>
       </c>
       <c r="BD25" s="37">
         <f t="shared" si="36"/>
-        <v>9.8375175353080291</v>
+        <v>8.6939898487967078</v>
       </c>
       <c r="BE25" s="53">
         <f t="shared" si="17"/>
-        <v>0.98375175353080291</v>
+        <v>0.86939898487967082</v>
       </c>
       <c r="BF25" s="38">
         <f t="shared" si="37"/>
-        <v>12.296896919135037</v>
+        <v>13.149659646305022</v>
       </c>
       <c r="BG25" s="34">
         <f t="shared" si="38"/>
-        <v>0.16666666666666666</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="BH25" s="34">
         <f t="shared" si="39"/>
-        <v>7.3781381514810223</v>
-      </c>
-      <c r="BI25" s="101" t="str">
+        <v>1.9724489469457533</v>
+      </c>
+      <c r="BI25" s="98" t="str">
         <f t="shared" si="40"/>
-        <v>PARRILLA</v>
+        <v>NO PARRILLA</v>
       </c>
       <c r="BJ25" s="38">
         <f t="shared" si="41"/>
-        <v>4.426882890888634</v>
+        <v>3.2874149115762634</v>
       </c>
       <c r="BK25" s="34">
         <f t="shared" si="42"/>
-        <v>0.16666666666666666</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="BL25" s="34">
         <f t="shared" si="43"/>
-        <v>2.6561297345331805</v>
-      </c>
-      <c r="BM25" s="101" t="str">
+        <v>0.4931122367364395</v>
+      </c>
+      <c r="BM25" s="98" t="str">
         <f t="shared" si="44"/>
         <v>NO PARRILLA</v>
       </c>
     </row>
-    <row r="26" spans="2:65" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="97" t="s">
+    <row r="26" spans="2:65" x14ac:dyDescent="0.25">
+      <c r="B26" s="102" t="s">
         <v>193</v>
       </c>
       <c r="C26" s="42" t="str">
@@ -79903,26 +79919,26 @@
         <v>984.27760000000001</v>
       </c>
       <c r="O26" s="65">
-        <f t="shared" si="88"/>
-        <v>36.380999999999993</v>
+        <f>0+E26+0.1</f>
+        <v>35.881</v>
       </c>
       <c r="P26" s="42">
         <v>1</v>
       </c>
       <c r="Q26" s="42">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R26" s="54">
         <f>2.5*O26*P26*Q26</f>
-        <v>90.952499999999986</v>
+        <v>179.405</v>
       </c>
       <c r="S26" s="55">
         <f t="shared" si="19"/>
-        <v>6.0634999999999986</v>
+        <v>5.9801666666666664</v>
       </c>
       <c r="U26" s="61">
         <f t="shared" si="0"/>
-        <v>290.19569999999999</v>
+        <v>378.64819999999997</v>
       </c>
       <c r="V26" s="54">
         <f t="shared" si="20"/>
@@ -79930,15 +79946,15 @@
       </c>
       <c r="W26" s="62">
         <f t="shared" si="21"/>
-        <v>7.8609459065037841</v>
+        <v>6.0246231198246818</v>
       </c>
       <c r="X26" s="55">
         <f t="shared" si="45"/>
-        <v>1.8729153093046911</v>
+        <v>2.1184520104710858</v>
       </c>
       <c r="Y26" s="61">
         <f t="shared" si="1"/>
-        <v>361.18290000000002</v>
+        <v>449.6354</v>
       </c>
       <c r="Z26" s="54">
         <f t="shared" si="2"/>
@@ -79946,24 +79962,24 @@
       </c>
       <c r="AA26" s="62">
         <f t="shared" si="22"/>
-        <v>6.4066488197530953</v>
+        <v>5.1463296706620527</v>
       </c>
       <c r="AB26" s="55">
         <f t="shared" si="23"/>
-        <v>2.0433778084674934</v>
+        <v>2.3315304901048988</v>
       </c>
       <c r="AC26" s="53">
         <f t="shared" si="89"/>
-        <v>0.23411441366308638</v>
+        <v>0.26480650130888572</v>
       </c>
       <c r="AD26" s="53">
         <f t="shared" si="90"/>
-        <v>0.25542222605843667</v>
+        <v>0.29144131126311235</v>
       </c>
       <c r="AE26" s="36"/>
       <c r="AF26" s="56">
         <f>ABS(IF(B26="x",$R26+ABS($G26)+$I26,$R26+ABS($G26)+$J26))</f>
-        <v>324.79629999999997</v>
+        <v>413.24879999999996</v>
       </c>
       <c r="AG26" s="54">
         <f t="shared" si="6"/>
@@ -79971,15 +79987,15 @@
       </c>
       <c r="AH26" s="54">
         <f t="shared" si="24"/>
-        <v>3.9930722732986808</v>
+        <v>3.1383880606549863</v>
       </c>
       <c r="AI26" s="55">
         <f t="shared" si="25"/>
-        <v>1.4806862318093448</v>
+        <v>1.7561426238778459</v>
       </c>
       <c r="AJ26" s="56">
         <f t="shared" si="7"/>
-        <v>255.5951</v>
+        <v>344.04759999999999</v>
       </c>
       <c r="AK26" s="54">
         <f t="shared" si="8"/>
@@ -79987,15 +80003,15 @@
       </c>
       <c r="AL26" s="54">
         <f t="shared" si="26"/>
-        <v>12.776028570187769</v>
+        <v>9.4913910168244158</v>
       </c>
       <c r="AM26" s="55">
         <f t="shared" si="27"/>
-        <v>3.1470612698244982</v>
+        <v>2.7146657372202596</v>
       </c>
       <c r="AN26" s="56">
         <f t="shared" si="9"/>
-        <v>369.38655</v>
+        <v>457.83904999999999</v>
       </c>
       <c r="AO26" s="54">
         <f t="shared" si="10"/>
@@ -80003,15 +80019,15 @@
       </c>
       <c r="AP26" s="54">
         <f t="shared" si="28"/>
-        <v>4.2437223959562136</v>
+        <v>3.4238538084508079</v>
       </c>
       <c r="AQ26" s="55">
         <f t="shared" si="29"/>
-        <v>1.72593609187776</v>
+        <v>2.0065434645425921</v>
       </c>
       <c r="AR26" s="56">
         <f t="shared" si="11"/>
-        <v>317.48565000000002</v>
+        <v>405.93815000000001</v>
       </c>
       <c r="AS26" s="54">
         <f t="shared" si="12"/>
@@ -80019,15 +80035,15 @@
       </c>
       <c r="AT26" s="54">
         <f t="shared" si="30"/>
-        <v>9.5878045984125571</v>
+        <v>7.4986555833690423</v>
       </c>
       <c r="AU26" s="55">
         <f t="shared" si="31"/>
-        <v>2.4603579473584909</v>
+        <v>2.5917397591396996</v>
       </c>
       <c r="AV26" s="56">
         <f t="shared" si="13"/>
-        <v>208.71801999999997</v>
+        <v>261.78951999999998</v>
       </c>
       <c r="AW26" s="54">
         <f t="shared" si="14"/>
@@ -80035,15 +80051,15 @@
       </c>
       <c r="AX26" s="54">
         <f t="shared" si="32"/>
-        <v>1.8419589262105875</v>
+        <v>1.4685462580778632</v>
       </c>
       <c r="AY26" s="55">
         <f t="shared" si="33"/>
-        <v>0.74797833457176144</v>
+        <v>0.90877352712227299</v>
       </c>
       <c r="AZ26" s="56">
         <f t="shared" si="15"/>
-        <v>139.51682</v>
+        <v>192.58832000000001</v>
       </c>
       <c r="BA26" s="54">
         <f t="shared" si="16"/>
@@ -80051,55 +80067,55 @@
       </c>
       <c r="BB26" s="54">
         <f t="shared" si="34"/>
-        <v>16.86538741350326</v>
+        <v>12.217798150998981</v>
       </c>
       <c r="BC26" s="55">
         <f t="shared" si="35"/>
-        <v>7.0191177927931037</v>
+        <v>2.2435593662064721</v>
       </c>
       <c r="BD26" s="59">
         <f t="shared" si="36"/>
-        <v>7.0191177927931037</v>
+        <v>2.7146657372202596</v>
       </c>
       <c r="BE26" s="53">
         <f t="shared" si="17"/>
-        <v>0.70191177927931037</v>
+        <v>0.27146657372202598</v>
       </c>
       <c r="BF26" s="56">
         <f t="shared" si="37"/>
-        <v>8.7738972409913796</v>
+        <v>3.3933321715253246</v>
       </c>
       <c r="BG26" s="54">
         <f t="shared" si="38"/>
-        <v>0.16666666666666666</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="BH26" s="54">
         <f t="shared" si="39"/>
-        <v>5.2643383445948277</v>
-      </c>
-      <c r="BI26" s="102" t="str">
+        <v>0.50899982572879865</v>
+      </c>
+      <c r="BI26" s="99" t="str">
         <f t="shared" si="40"/>
         <v>NO PARRILLA</v>
       </c>
       <c r="BJ26" s="56">
         <f t="shared" si="41"/>
-        <v>3.1586030067568367</v>
+        <v>3.3933321715254212E-2</v>
       </c>
       <c r="BK26" s="54">
         <f t="shared" si="42"/>
-        <v>0.16666666666666666</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="BL26" s="54">
         <f t="shared" si="43"/>
-        <v>1.8951618040541021</v>
-      </c>
-      <c r="BM26" s="102" t="str">
+        <v>5.0899982572881319E-3</v>
+      </c>
+      <c r="BM26" s="99" t="str">
         <f t="shared" si="44"/>
         <v>NO PARRILLA</v>
       </c>
     </row>
     <row r="27" spans="2:65" x14ac:dyDescent="0.25">
-      <c r="B27" s="103" t="s">
+      <c r="B27" s="100" t="s">
         <v>193</v>
       </c>
       <c r="C27" s="30" t="str">
@@ -80325,7 +80341,7 @@
         <f t="shared" si="39"/>
         <v>6.5250729896748307</v>
       </c>
-      <c r="BI27" s="101" t="str">
+      <c r="BI27" s="98" t="str">
         <f t="shared" si="40"/>
         <v>NO PARRILLA</v>
       </c>
@@ -80341,7 +80357,7 @@
         <f t="shared" si="43"/>
         <v>0.58725656907073409</v>
       </c>
-      <c r="BM27" s="101" t="str">
+      <c r="BM27" s="98" t="str">
         <f t="shared" si="44"/>
         <v>NO PARRILLA</v>
       </c>
@@ -80573,7 +80589,7 @@
         <f t="shared" si="39"/>
         <v>2.6563975208333335</v>
       </c>
-      <c r="BI28" s="101" t="str">
+      <c r="BI28" s="98" t="str">
         <f t="shared" si="40"/>
         <v>NO PARRILLA</v>
       </c>
@@ -80589,7 +80605,7 @@
         <f t="shared" si="43"/>
         <v>3.080792391025641</v>
       </c>
-      <c r="BM28" s="101" t="str">
+      <c r="BM28" s="98" t="str">
         <f t="shared" si="44"/>
         <v>NO PARRILLA</v>
       </c>
@@ -80821,7 +80837,7 @@
         <f t="shared" si="39"/>
         <v>2.7818406916544922</v>
       </c>
-      <c r="BI29" s="101" t="str">
+      <c r="BI29" s="98" t="str">
         <f t="shared" si="40"/>
         <v>NO PARRILLA</v>
       </c>
@@ -80837,7 +80853,7 @@
         <f t="shared" si="43"/>
         <v>1.4193064753339248</v>
       </c>
-      <c r="BM29" s="101" t="str">
+      <c r="BM29" s="98" t="str">
         <f t="shared" si="44"/>
         <v>NO PARRILLA</v>
       </c>
@@ -81069,7 +81085,7 @@
         <f t="shared" si="39"/>
         <v>4.3128806190421756</v>
       </c>
-      <c r="BI30" s="101" t="str">
+      <c r="BI30" s="98" t="str">
         <f t="shared" si="40"/>
         <v>NO PARRILLA</v>
       </c>
@@ -81085,7 +81101,7 @@
         <f t="shared" si="43"/>
         <v>2.1489785783462723</v>
       </c>
-      <c r="BM30" s="101" t="str">
+      <c r="BM30" s="98" t="str">
         <f t="shared" si="44"/>
         <v>NO PARRILLA</v>
       </c>
@@ -81317,7 +81333,7 @@
         <f t="shared" si="39"/>
         <v>4.2443556836748826</v>
       </c>
-      <c r="BI31" s="101" t="str">
+      <c r="BI31" s="98" t="str">
         <f t="shared" si="40"/>
         <v>NO PARRILLA</v>
       </c>
@@ -81333,7 +81349,7 @@
         <f t="shared" si="43"/>
         <v>0.26527223022968055</v>
       </c>
-      <c r="BM31" s="101" t="str">
+      <c r="BM31" s="98" t="str">
         <f t="shared" si="44"/>
         <v>NO PARRILLA</v>
       </c>
@@ -81565,7 +81581,7 @@
         <f t="shared" si="39"/>
         <v>4.273734642235345</v>
       </c>
-      <c r="BI32" s="101" t="str">
+      <c r="BI32" s="98" t="str">
         <f t="shared" si="40"/>
         <v>NO PARRILLA</v>
       </c>
@@ -81581,7 +81597,7 @@
         <f t="shared" si="43"/>
         <v>2.8213326349131758</v>
       </c>
-      <c r="BM32" s="101" t="str">
+      <c r="BM32" s="98" t="str">
         <f t="shared" si="44"/>
         <v>NO PARRILLA</v>
       </c>
@@ -81813,7 +81829,7 @@
         <f t="shared" si="39"/>
         <v>4.863086406474558</v>
       </c>
-      <c r="BI33" s="101" t="str">
+      <c r="BI33" s="98" t="str">
         <f t="shared" si="40"/>
         <v>NO PARRILLA</v>
       </c>
@@ -81829,7 +81845,7 @@
         <f t="shared" si="43"/>
         <v>1.5009525945909128</v>
       </c>
-      <c r="BM33" s="101" t="str">
+      <c r="BM33" s="98" t="str">
         <f t="shared" si="44"/>
         <v>NO PARRILLA</v>
       </c>
@@ -82061,7 +82077,7 @@
         <f t="shared" si="39"/>
         <v>6.7699824099534975</v>
       </c>
-      <c r="BI34" s="101" t="str">
+      <c r="BI34" s="98" t="str">
         <f t="shared" si="40"/>
         <v>NO PARRILLA</v>
       </c>
@@ -82077,7 +82093,7 @@
         <f t="shared" si="43"/>
         <v>2.5943923521137013</v>
       </c>
-      <c r="BM34" s="101" t="str">
+      <c r="BM34" s="98" t="str">
         <f t="shared" si="44"/>
         <v>NO PARRILLA</v>
       </c>
@@ -82309,7 +82325,7 @@
         <f t="shared" si="39"/>
         <v>5.9105732732272234</v>
       </c>
-      <c r="BI35" s="101" t="str">
+      <c r="BI35" s="98" t="str">
         <f t="shared" si="40"/>
         <v>NO PARRILLA</v>
       </c>
@@ -82325,7 +82341,7 @@
         <f t="shared" si="43"/>
         <v>0.58942004940770099</v>
       </c>
-      <c r="BM35" s="101" t="str">
+      <c r="BM35" s="98" t="str">
         <f t="shared" si="44"/>
         <v>NO PARRILLA</v>
       </c>
@@ -82557,7 +82573,7 @@
         <f t="shared" si="39"/>
         <v>2.8164457228328938</v>
       </c>
-      <c r="BI36" s="101" t="str">
+      <c r="BI36" s="98" t="str">
         <f t="shared" si="40"/>
         <v>NO PARRILLA</v>
       </c>
@@ -82573,7 +82589,7 @@
         <f t="shared" si="43"/>
         <v>2.4284659548916285</v>
       </c>
-      <c r="BM36" s="101" t="str">
+      <c r="BM36" s="98" t="str">
         <f t="shared" si="44"/>
         <v>NO PARRILLA</v>
       </c>
@@ -82805,7 +82821,7 @@
         <f t="shared" si="39"/>
         <v>4.1782602125000006</v>
       </c>
-      <c r="BI37" s="101" t="str">
+      <c r="BI37" s="98" t="str">
         <f t="shared" si="40"/>
         <v>NO PARRILLA</v>
       </c>
@@ -82821,13 +82837,13 @@
         <f t="shared" si="43"/>
         <v>2.8336989676470585</v>
       </c>
-      <c r="BM37" s="101" t="str">
+      <c r="BM37" s="98" t="str">
         <f t="shared" si="44"/>
         <v>NO PARRILLA</v>
       </c>
     </row>
     <row r="38" spans="1:65" x14ac:dyDescent="0.25">
-      <c r="B38" s="103" t="s">
+      <c r="B38" s="100" t="s">
         <v>193</v>
       </c>
       <c r="C38" s="30" t="str">
@@ -83053,7 +83069,7 @@
         <f t="shared" si="39"/>
         <v>4.9129950058886696</v>
       </c>
-      <c r="BI38" s="101" t="str">
+      <c r="BI38" s="98" t="str">
         <f t="shared" si="40"/>
         <v>NO PARRILLA</v>
       </c>
@@ -83069,13 +83085,13 @@
         <f t="shared" si="43"/>
         <v>2.1835533359505197</v>
       </c>
-      <c r="BM38" s="101" t="str">
+      <c r="BM38" s="98" t="str">
         <f t="shared" si="44"/>
         <v>NO PARRILLA</v>
       </c>
     </row>
     <row r="39" spans="1:65" x14ac:dyDescent="0.25">
-      <c r="B39" s="104" t="s">
+      <c r="B39" s="101" t="s">
         <v>193</v>
       </c>
       <c r="C39" s="30" t="str">
@@ -83127,26 +83143,26 @@
         <v>31.666899999999998</v>
       </c>
       <c r="O39" s="29">
-        <f>1.3+E39+1.3</f>
-        <v>5.22</v>
+        <f>0.3+E39+0.3</f>
+        <v>3.2199999999999998</v>
       </c>
       <c r="P39" s="30">
-        <v>2.4</v>
+        <v>1.7</v>
       </c>
       <c r="Q39" s="30">
         <v>2</v>
       </c>
       <c r="R39" s="34">
         <f t="shared" si="18"/>
-        <v>62.639999999999993</v>
+        <v>27.369999999999994</v>
       </c>
       <c r="S39" s="32">
         <f t="shared" si="19"/>
-        <v>0.87</v>
+        <v>0.53666666666666663</v>
       </c>
       <c r="U39" s="33">
         <f t="shared" si="0"/>
-        <v>87.642599999999987</v>
+        <v>52.372599999999991</v>
       </c>
       <c r="V39" s="34">
         <f t="shared" si="20"/>
@@ -83154,15 +83170,15 @@
       </c>
       <c r="W39" s="35">
         <f t="shared" si="21"/>
-        <v>2.2366474750863166</v>
+        <v>3.7429037321041925</v>
       </c>
       <c r="X39" s="32">
         <f t="shared" si="45"/>
-        <v>6.520691582920219</v>
+        <v>-0.96292552732992376</v>
       </c>
       <c r="Y39" s="33">
         <f t="shared" si="1"/>
-        <v>96.231199999999987</v>
+        <v>60.961199999999991</v>
       </c>
       <c r="Z39" s="34">
         <f t="shared" si="2"/>
@@ -83170,24 +83186,24 @@
       </c>
       <c r="AA39" s="35">
         <f t="shared" si="22"/>
-        <v>2.0423500901994367</v>
+        <v>3.2239818113816661</v>
       </c>
       <c r="AB39" s="32">
         <f t="shared" si="23"/>
-        <v>4.7090448579971511</v>
+        <v>-1.4812033675095249</v>
       </c>
       <c r="AC39" s="53">
         <f t="shared" si="89"/>
-        <v>0.81508644786502737</v>
+        <v>-0.12036569091624047</v>
       </c>
       <c r="AD39" s="53">
         <f t="shared" si="90"/>
-        <v>0.58863060724964389</v>
+        <v>-0.18515042093869061</v>
       </c>
       <c r="AE39" s="36"/>
       <c r="AF39" s="38">
         <f t="shared" si="5"/>
-        <v>101.75129999999999</v>
+        <v>66.48129999999999</v>
       </c>
       <c r="AG39" s="34">
         <f t="shared" si="6"/>
@@ -83195,15 +83211,15 @@
       </c>
       <c r="AH39" s="34">
         <f t="shared" si="24"/>
-        <v>1.6152982812013215</v>
+        <v>2.472254603926217</v>
       </c>
       <c r="AI39" s="32">
         <f t="shared" si="25"/>
-        <v>2.8414799598552323</v>
+        <v>-3.0235962696519945</v>
       </c>
       <c r="AJ39" s="38">
         <f t="shared" si="7"/>
-        <v>73.533899999999988</v>
+        <v>38.263899999999992</v>
       </c>
       <c r="AK39" s="34">
         <f t="shared" si="8"/>
@@ -83211,15 +83227,15 @@
       </c>
       <c r="AL39" s="34">
         <f t="shared" si="26"/>
-        <v>3.0964289939742082</v>
+        <v>5.95058266407763</v>
       </c>
       <c r="AM39" s="32">
         <f t="shared" si="27"/>
-        <v>-4.199191163842583</v>
+        <v>-0.34570130652219244</v>
       </c>
       <c r="AN39" s="38">
         <f t="shared" si="9"/>
-        <v>104.66557499999999</v>
+        <v>69.395574999999994</v>
       </c>
       <c r="AO39" s="34">
         <f t="shared" si="10"/>
@@ -83227,15 +83243,15 @@
       </c>
       <c r="AP39" s="34">
         <f t="shared" si="28"/>
-        <v>1.6496309794313941</v>
+        <v>2.4880487696801996</v>
       </c>
       <c r="AQ39" s="32">
         <f t="shared" si="29"/>
-        <v>3.0273540910471706</v>
+        <v>-3.0993666775826059</v>
       </c>
       <c r="AR39" s="38">
         <f t="shared" si="11"/>
-        <v>83.502524999999991</v>
+        <v>48.232524999999995</v>
       </c>
       <c r="AS39" s="34">
         <f t="shared" si="12"/>
@@ -83243,15 +83259,15 @@
       </c>
       <c r="AT39" s="34">
         <f t="shared" si="30"/>
-        <v>2.6365660798880035</v>
+        <v>4.5645531723665727</v>
       </c>
       <c r="AU39" s="32">
         <f t="shared" si="31"/>
-        <v>-87.311134842320087</v>
+        <v>-0.64018870478218459</v>
       </c>
       <c r="AV39" s="38">
         <f t="shared" si="13"/>
-        <v>66.69426</v>
+        <v>45.532259999999994</v>
       </c>
       <c r="AW39" s="34">
         <f t="shared" si="14"/>
@@ -83259,15 +83275,15 @@
       </c>
       <c r="AX39" s="34">
         <f t="shared" si="32"/>
-        <v>1.2886935097563119</v>
+        <v>1.8876387862144337</v>
       </c>
       <c r="AY39" s="32">
         <f t="shared" si="33"/>
-        <v>1.402110976531763</v>
+        <v>-6.4313017927917429</v>
       </c>
       <c r="AZ39" s="38">
         <f t="shared" si="15"/>
-        <v>38.476859999999995</v>
+        <v>17.314859999999996</v>
       </c>
       <c r="BA39" s="34">
         <f t="shared" si="16"/>
@@ -83275,23 +83291,23 @@
       </c>
       <c r="BB39" s="34">
         <f t="shared" si="34"/>
-        <v>3.8797932055786264</v>
+        <v>8.621626741423265</v>
       </c>
       <c r="BC39" s="32">
         <f t="shared" si="35"/>
-        <v>-0.8417131718543327</v>
+        <v>-9.6841167205262257E-2</v>
       </c>
       <c r="BD39" s="37">
         <f t="shared" si="36"/>
-        <v>3.0273540910471706</v>
+        <v>-9.6841167205262257E-2</v>
       </c>
       <c r="BE39" s="53">
         <f t="shared" si="17"/>
-        <v>0.30273540910471708</v>
+        <v>-9.684116720526225E-3</v>
       </c>
       <c r="BF39" s="38">
         <f t="shared" si="37"/>
-        <v>21.796949455539629</v>
+        <v>-0.34983871652900989</v>
       </c>
       <c r="BG39" s="34">
         <f t="shared" si="38"/>
@@ -83299,15 +83315,15 @@
       </c>
       <c r="BH39" s="34">
         <f t="shared" si="39"/>
-        <v>3.2695424183309449</v>
-      </c>
-      <c r="BI39" s="101" t="str">
+        <v>-5.2475807479351488E-2</v>
+      </c>
+      <c r="BI39" s="98" t="str">
         <f t="shared" si="40"/>
         <v>NO PARRILLA</v>
       </c>
       <c r="BJ39" s="38">
         <f t="shared" si="41"/>
-        <v>25.581142069348584</v>
+        <v>-4.3578525242367966E-2</v>
       </c>
       <c r="BK39" s="34">
         <f t="shared" si="42"/>
@@ -83315,9 +83331,9 @@
       </c>
       <c r="BL39" s="34">
         <f t="shared" si="43"/>
-        <v>3.837171310402288</v>
-      </c>
-      <c r="BM39" s="101" t="str">
+        <v>-6.5367787863551945E-3</v>
+      </c>
+      <c r="BM39" s="98" t="str">
         <f t="shared" si="44"/>
         <v>NO PARRILLA</v>
       </c>
@@ -83549,7 +83565,7 @@
         <f t="shared" si="39"/>
         <v>3.2824237842279564</v>
       </c>
-      <c r="BI40" s="101" t="str">
+      <c r="BI40" s="98" t="str">
         <f t="shared" si="40"/>
         <v>NO PARRILLA</v>
       </c>
@@ -83565,7 +83581,7 @@
         <f t="shared" si="43"/>
         <v>3.2824237842279542</v>
       </c>
-      <c r="BM40" s="101" t="str">
+      <c r="BM40" s="98" t="str">
         <f t="shared" si="44"/>
         <v>NO PARRILLA</v>
       </c>
@@ -83797,7 +83813,7 @@
         <f t="shared" si="39"/>
         <v>2.8488332292443266</v>
       </c>
-      <c r="BI41" s="101" t="str">
+      <c r="BI41" s="98" t="str">
         <f t="shared" si="40"/>
         <v>NO PARRILLA</v>
       </c>
@@ -83813,7 +83829,7 @@
         <f t="shared" si="43"/>
         <v>0.93023125852875965</v>
       </c>
-      <c r="BM41" s="101" t="str">
+      <c r="BM41" s="98" t="str">
         <f t="shared" si="44"/>
         <v>NO PARRILLA</v>
       </c>
@@ -84045,7 +84061,7 @@
         <f t="shared" si="39"/>
         <v>5.2396624863625521</v>
       </c>
-      <c r="BI42" s="101" t="str">
+      <c r="BI42" s="98" t="str">
         <f t="shared" si="40"/>
         <v>NO PARRILLA</v>
       </c>
@@ -84061,13 +84077,13 @@
         <f t="shared" si="43"/>
         <v>5.8742236871331084</v>
       </c>
-      <c r="BM42" s="101" t="str">
+      <c r="BM42" s="98" t="str">
         <f t="shared" si="44"/>
         <v>NO PARRILLA</v>
       </c>
     </row>
     <row r="43" spans="1:65" x14ac:dyDescent="0.25">
-      <c r="B43" s="29" t="s">
+      <c r="B43" s="101" t="s">
         <v>193</v>
       </c>
       <c r="C43" s="30" t="str">
@@ -84119,26 +84135,26 @@
         <v>36.224299999999999</v>
       </c>
       <c r="O43" s="29">
-        <f>1+E43+1</f>
-        <v>6</v>
+        <f>0+E43+0</f>
+        <v>4</v>
       </c>
       <c r="P43" s="30">
-        <v>5.3</v>
+        <v>1</v>
       </c>
       <c r="Q43" s="30">
         <v>2</v>
       </c>
       <c r="R43" s="34">
         <f t="shared" si="18"/>
-        <v>159</v>
+        <v>20</v>
       </c>
       <c r="S43" s="32">
         <f t="shared" si="19"/>
-        <v>1</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="U43" s="33">
         <f t="shared" si="0"/>
-        <v>159.0393</v>
+        <v>20.039300000000001</v>
       </c>
       <c r="V43" s="34">
         <f t="shared" si="20"/>
@@ -84146,15 +84162,15 @@
       </c>
       <c r="W43" s="35">
         <f t="shared" si="21"/>
-        <v>3.075651741424918</v>
+        <v>24.409510312236453</v>
       </c>
       <c r="X43" s="32">
         <f t="shared" si="45"/>
-        <v>-26.443467155452975</v>
+        <v>-5.9615463020798433E-2</v>
       </c>
       <c r="Y43" s="33">
         <f t="shared" si="1"/>
-        <v>161.6926</v>
+        <v>22.692600000000002</v>
       </c>
       <c r="Z43" s="34">
         <f t="shared" si="2"/>
@@ -84162,24 +84178,24 @@
       </c>
       <c r="AA43" s="35">
         <f t="shared" si="22"/>
-        <v>3.0167546319373924</v>
+        <v>21.49541700818769</v>
       </c>
       <c r="AB43" s="32">
         <f t="shared" si="23"/>
-        <v>-121.39145700066531</v>
+        <v>-7.7599776366139656E-2</v>
       </c>
       <c r="AC43" s="53">
         <f t="shared" si="89"/>
-        <v>-3.3054333944316219</v>
+        <v>-7.4519328775998041E-3</v>
       </c>
       <c r="AD43" s="53">
         <f t="shared" si="90"/>
-        <v>-15.173932125083164</v>
+        <v>-9.6999720457674569E-3</v>
       </c>
       <c r="AE43" s="36"/>
       <c r="AF43" s="38">
         <f t="shared" si="5"/>
-        <v>169.3878</v>
+        <v>30.387799999999999</v>
       </c>
       <c r="AG43" s="34">
         <f t="shared" si="6"/>
@@ -84187,15 +84203,15 @@
       </c>
       <c r="AH43" s="34">
         <f t="shared" si="24"/>
-        <v>3.1016035393340013</v>
+        <v>17.288971231875951</v>
       </c>
       <c r="AI43" s="32">
         <f t="shared" si="25"/>
-        <v>-20.970373324685703</v>
+        <v>-0.13250422821841895</v>
       </c>
       <c r="AJ43" s="38">
         <f t="shared" si="7"/>
-        <v>148.6908</v>
+        <v>9.6908000000000012</v>
       </c>
       <c r="AK43" s="34">
         <f t="shared" si="8"/>
@@ -84203,15 +84219,15 @@
       </c>
       <c r="AL43" s="34">
         <f t="shared" si="26"/>
-        <v>3.0460875857820393</v>
+        <v>46.737648078589999</v>
       </c>
       <c r="AM43" s="32">
         <f t="shared" si="27"/>
-        <v>-40.581959253564698</v>
+        <v>-1.4440931990846289E-2</v>
       </c>
       <c r="AN43" s="38">
         <f t="shared" si="9"/>
-        <v>168.79064999999997</v>
+        <v>29.790649999999999</v>
       </c>
       <c r="AO43" s="34">
         <f t="shared" si="10"/>
@@ -84219,15 +84235,15 @@
       </c>
       <c r="AP43" s="34">
         <f t="shared" si="28"/>
-        <v>3.0528691903254122</v>
+        <v>17.297231681752493</v>
       </c>
       <c r="AQ43" s="32">
         <f t="shared" si="29"/>
-        <v>-40.158603094176051</v>
+        <v>-0.12983024475614185</v>
       </c>
       <c r="AR43" s="38">
         <f t="shared" si="11"/>
-        <v>153.2679</v>
+        <v>14.267900000000003</v>
       </c>
       <c r="AS43" s="34">
         <f t="shared" si="12"/>
@@ -84235,15 +84251,15 @@
       </c>
       <c r="AT43" s="34">
         <f t="shared" si="30"/>
-        <v>3.0075399023539826</v>
+        <v>32.307440127839406</v>
       </c>
       <c r="AU43" s="32">
         <f t="shared" si="31"/>
-        <v>-255.69271625768778</v>
+        <v>-3.1384812749645559E-2</v>
       </c>
       <c r="AV43" s="38">
         <f t="shared" si="13"/>
-        <v>105.77207999999999</v>
+        <v>22.37208</v>
       </c>
       <c r="AW43" s="34">
         <f t="shared" si="14"/>
@@ -84251,15 +84267,15 @@
       </c>
       <c r="AX43" s="34">
         <f t="shared" si="32"/>
-        <v>3.1172120279756244</v>
+        <v>14.737744545880398</v>
       </c>
       <c r="AY43" s="32">
         <f t="shared" si="33"/>
-        <v>-11.350937596361918</v>
+        <v>-0.1170907451180097</v>
       </c>
       <c r="AZ43" s="38">
         <f t="shared" si="15"/>
-        <v>85.075079999999986</v>
+        <v>1.6750800000000012</v>
       </c>
       <c r="BA43" s="34">
         <f t="shared" si="16"/>
@@ -84267,23 +84283,23 @@
       </c>
       <c r="BB43" s="34">
         <f t="shared" si="34"/>
-        <v>3.0239807003413932</v>
+        <v>153.58394822933818</v>
       </c>
       <c r="BC43" s="32">
         <f t="shared" si="35"/>
-        <v>-44.624501253855314</v>
+        <v>-7.3670069492481145E-4</v>
       </c>
       <c r="BD43" s="37">
         <f t="shared" si="36"/>
-        <v>-11.350937596361918</v>
+        <v>-7.3670069492481145E-4</v>
       </c>
       <c r="BE43" s="53">
         <f t="shared" si="17"/>
-        <v>-1.1350937596361919</v>
+        <v>-7.3670069492481151E-5</v>
       </c>
       <c r="BF43" s="38">
         <f t="shared" si="37"/>
-        <v>-398.55979635225782</v>
+        <v>-9.2087586865601434E-4</v>
       </c>
       <c r="BG43" s="34">
         <f t="shared" si="38"/>
@@ -84291,15 +84307,15 @@
       </c>
       <c r="BH43" s="34">
         <f t="shared" si="39"/>
-        <v>-59.783969452838676</v>
-      </c>
-      <c r="BI43" s="101" t="str">
+        <v>-1.3813138029840217E-4</v>
+      </c>
+      <c r="BI43" s="98" t="str">
         <f t="shared" si="40"/>
         <v>NO PARRILLA</v>
       </c>
       <c r="BJ43" s="38">
         <f t="shared" si="41"/>
-        <v>-56.754687981809589</v>
+        <v>0</v>
       </c>
       <c r="BK43" s="34">
         <f t="shared" si="42"/>
@@ -84307,15 +84323,15 @@
       </c>
       <c r="BL43" s="34">
         <f t="shared" si="43"/>
-        <v>-8.513203197271439</v>
-      </c>
-      <c r="BM43" s="101" t="str">
+        <v>0</v>
+      </c>
+      <c r="BM43" s="98" t="str">
         <f t="shared" si="44"/>
         <v>NO PARRILLA</v>
       </c>
     </row>
     <row r="44" spans="1:65" x14ac:dyDescent="0.25">
-      <c r="B44" s="29" t="s">
+      <c r="B44" s="101" t="s">
         <v>193</v>
       </c>
       <c r="C44" s="30" t="str">
@@ -84328,7 +84344,7 @@
       </c>
       <c r="E44" s="30">
         <f>'MUROS EJE Y'!E22</f>
-        <v>8.6199999999999992</v>
+        <v>8.64</v>
       </c>
       <c r="F44" s="14">
         <f>'MUROS EJE Y'!F22</f>
@@ -84367,26 +84383,26 @@
         <v>43.931199999999997</v>
       </c>
       <c r="O44" s="29">
-        <f t="shared" si="88"/>
-        <v>9.2200000000000006</v>
+        <f>0+E44+0</f>
+        <v>8.64</v>
       </c>
       <c r="P44" s="30">
         <v>1</v>
       </c>
       <c r="Q44" s="30">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R44" s="34">
         <f t="shared" si="18"/>
-        <v>23.05</v>
+        <v>43.2</v>
       </c>
       <c r="S44" s="32">
         <f t="shared" si="19"/>
-        <v>1.5366666666666668</v>
+        <v>1.4400000000000002</v>
       </c>
       <c r="U44" s="33">
         <f t="shared" si="0"/>
-        <v>122.49159999999999</v>
+        <v>142.64159999999998</v>
       </c>
       <c r="V44" s="34">
         <f t="shared" si="20"/>
@@ -84394,15 +84410,15 @@
       </c>
       <c r="W44" s="35">
         <f t="shared" si="21"/>
-        <v>11.58452089775952</v>
+        <v>9.9480551255734664</v>
       </c>
       <c r="X44" s="32">
         <f t="shared" si="45"/>
-        <v>-1.170848404696863</v>
+        <v>-1.6896494060247931</v>
       </c>
       <c r="Y44" s="33">
         <f t="shared" si="1"/>
-        <v>142.5378</v>
+        <v>162.68779999999998</v>
       </c>
       <c r="Z44" s="34">
         <f t="shared" si="2"/>
@@ -84410,24 +84426,24 @@
       </c>
       <c r="AA44" s="35">
         <f t="shared" si="22"/>
-        <v>10.153389486858924</v>
+        <v>8.8958225509226878</v>
       </c>
       <c r="AB44" s="32">
         <f t="shared" si="23"/>
-        <v>-1.7142075299826096</v>
+        <v>-2.370252170540645</v>
       </c>
       <c r="AC44" s="53">
         <f t="shared" si="89"/>
-        <v>-0.14635605058710788</v>
+        <v>-0.21120617575309913</v>
       </c>
       <c r="AD44" s="53">
         <f t="shared" si="90"/>
-        <v>-0.2142759412478262</v>
+        <v>-0.29628152131758062</v>
       </c>
       <c r="AE44" s="36"/>
       <c r="AF44" s="38">
         <f t="shared" si="5"/>
-        <v>123.53699999999999</v>
+        <v>143.68699999999998</v>
       </c>
       <c r="AG44" s="34">
         <f t="shared" si="6"/>
@@ -84435,15 +84451,15 @@
       </c>
       <c r="AH44" s="34">
         <f t="shared" si="24"/>
-        <v>11.842101556618665</v>
+        <v>10.181420031039691</v>
       </c>
       <c r="AI44" s="32">
         <f t="shared" si="25"/>
-        <v>-1.1387837871915352</v>
+        <v>-1.6342683654483299</v>
       </c>
       <c r="AJ44" s="38">
         <f t="shared" si="7"/>
-        <v>121.44619999999999</v>
+        <v>141.59619999999998</v>
       </c>
       <c r="AK44" s="34">
         <f t="shared" si="8"/>
@@ -84451,15 +84467,15 @@
       </c>
       <c r="AL44" s="34">
         <f t="shared" si="26"/>
-        <v>11.322505767986154</v>
+        <v>9.7112443695522916</v>
       </c>
       <c r="AM44" s="32">
         <f t="shared" si="27"/>
-        <v>-1.206168547660313</v>
+        <v>-1.7509402319024496</v>
       </c>
       <c r="AN44" s="38">
         <f t="shared" si="9"/>
-        <v>138.31030000000001</v>
+        <v>158.46029999999999</v>
       </c>
       <c r="AO44" s="34">
         <f t="shared" si="10"/>
@@ -84467,15 +84483,15 @@
       </c>
       <c r="AP44" s="34">
         <f t="shared" si="28"/>
-        <v>10.650915911540933</v>
+        <v>9.2965327908630737</v>
       </c>
       <c r="AQ44" s="32">
         <f t="shared" si="29"/>
-        <v>-1.5263722921636613</v>
+        <v>-2.1227670838210022</v>
       </c>
       <c r="AR44" s="38">
         <f t="shared" si="11"/>
-        <v>136.7422</v>
+        <v>156.89219999999997</v>
       </c>
       <c r="AS44" s="34">
         <f t="shared" si="12"/>
@@ -84483,15 +84499,15 @@
       </c>
       <c r="AT44" s="34">
         <f t="shared" si="30"/>
-        <v>10.291150610418729</v>
+        <v>8.9694361797463493</v>
       </c>
       <c r="AU44" s="32">
         <f t="shared" si="31"/>
-        <v>-1.6046303454705917</v>
+        <v>-2.2496233082116674</v>
       </c>
       <c r="AV44" s="38">
         <f t="shared" si="13"/>
-        <v>74.540359999999993</v>
+        <v>86.630359999999996</v>
       </c>
       <c r="AW44" s="34">
         <f t="shared" si="14"/>
@@ -84499,15 +84515,15 @@
       </c>
       <c r="AX44" s="34">
         <f t="shared" si="32"/>
-        <v>12.011413682466786</v>
+        <v>10.335119235335048</v>
       </c>
       <c r="AY44" s="32">
         <f t="shared" si="33"/>
-        <v>-0.67140651050288491</v>
+        <v>-0.96014012480529676</v>
       </c>
       <c r="AZ44" s="38">
         <f t="shared" si="15"/>
-        <v>72.449559999999991</v>
+        <v>84.539559999999994</v>
       </c>
       <c r="BA44" s="34">
         <f t="shared" si="16"/>
@@ -84515,55 +84531,55 @@
       </c>
       <c r="BB44" s="34">
         <f t="shared" si="34"/>
-        <v>11.145308542936631</v>
+        <v>9.5514182945830335</v>
       </c>
       <c r="BC44" s="32">
         <f t="shared" si="35"/>
-        <v>-0.73905778662690746</v>
+        <v>-1.077331298952434</v>
       </c>
       <c r="BD44" s="37">
         <f t="shared" si="36"/>
-        <v>-0.67140651050288491</v>
+        <v>-0.96014012480529676</v>
       </c>
       <c r="BE44" s="53">
         <f t="shared" si="17"/>
-        <v>-6.7140651050288491E-2</v>
+        <v>-9.6014012480529681E-2</v>
       </c>
       <c r="BF44" s="38">
         <f t="shared" si="37"/>
-        <v>-0.83925813812860617</v>
+        <v>-1.2001751560066209</v>
       </c>
       <c r="BG44" s="34">
         <f t="shared" si="38"/>
-        <v>0.16666666666666666</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="BH44" s="34">
         <f t="shared" si="39"/>
-        <v>-0.50355488287716377</v>
-      </c>
-      <c r="BI44" s="101" t="str">
+        <v>-0.18002627340099314</v>
+      </c>
+      <c r="BI44" s="98" t="str">
         <f t="shared" si="40"/>
         <v>NO PARRILLA</v>
       </c>
       <c r="BJ44" s="38">
         <f t="shared" si="41"/>
-        <v>-0.30213292972629963</v>
+        <v>0</v>
       </c>
       <c r="BK44" s="34">
         <f t="shared" si="42"/>
-        <v>0.16666666666666666</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="BL44" s="34">
         <f t="shared" si="43"/>
-        <v>-0.18127975783577979</v>
-      </c>
-      <c r="BM44" s="101" t="str">
+        <v>0</v>
+      </c>
+      <c r="BM44" s="98" t="str">
         <f t="shared" si="44"/>
         <v>NO PARRILLA</v>
       </c>
     </row>
-    <row r="45" spans="1:65" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="98" t="s">
+    <row r="45" spans="1:65" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B45" s="103" t="s">
         <v>193</v>
       </c>
       <c r="C45" s="46" t="str">
@@ -84615,26 +84631,26 @@
         <v>468.2029</v>
       </c>
       <c r="O45" s="66">
-        <f t="shared" si="88"/>
-        <v>38.881999999999991</v>
+        <f>0+E45+0</f>
+        <v>38.281999999999996</v>
       </c>
       <c r="P45" s="46">
-        <v>1</v>
+        <v>1.2</v>
       </c>
       <c r="Q45" s="46">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R45" s="57">
         <f t="shared" si="18"/>
-        <v>97.204999999999984</v>
+        <v>229.69199999999995</v>
       </c>
       <c r="S45" s="52">
         <f t="shared" si="19"/>
-        <v>6.4803333333333315</v>
+        <v>6.3803333333333327</v>
       </c>
       <c r="U45" s="63">
         <f t="shared" si="0"/>
-        <v>145.32749999999999</v>
+        <v>277.81449999999995</v>
       </c>
       <c r="V45" s="57">
         <f t="shared" si="20"/>
@@ -84642,15 +84658,15 @@
       </c>
       <c r="W45" s="64">
         <f t="shared" si="21"/>
-        <v>26.104805353425885</v>
+        <v>13.655680679014235</v>
       </c>
       <c r="X45" s="52">
         <f t="shared" si="45"/>
-        <v>-1.4538990090728119</v>
+        <v>2.8137174858427803</v>
       </c>
       <c r="Y45" s="63">
         <f t="shared" si="1"/>
-        <v>172.06659999999999</v>
+        <v>304.55359999999996</v>
       </c>
       <c r="Z45" s="57">
         <f t="shared" si="2"/>
@@ -84658,24 +84674,24 @@
       </c>
       <c r="AA45" s="64">
         <f t="shared" si="22"/>
-        <v>22.448002110810581</v>
+        <v>12.682665383039309</v>
       </c>
       <c r="AB45" s="52">
         <f t="shared" si="23"/>
-        <v>-3.8147983419853491</v>
+        <v>2.6198153932765527</v>
       </c>
       <c r="AC45" s="53">
         <f t="shared" si="89"/>
-        <v>-0.18173737613410149</v>
+        <v>0.35171468573034753</v>
       </c>
       <c r="AD45" s="53">
         <f t="shared" si="90"/>
-        <v>-0.47684979274816863</v>
+        <v>0.32747692415956908</v>
       </c>
       <c r="AE45" s="36"/>
       <c r="AF45" s="58">
         <f t="shared" si="5"/>
-        <v>156.30799999999999</v>
+        <v>288.79499999999996</v>
       </c>
       <c r="AG45" s="57">
         <f t="shared" si="6"/>
@@ -84683,15 +84699,15 @@
       </c>
       <c r="AH45" s="57">
         <f t="shared" si="24"/>
-        <v>21.275578985080738</v>
+        <v>11.515238144704723</v>
       </c>
       <c r="AI45" s="52">
         <f t="shared" si="25"/>
-        <v>-5.6800679709490449</v>
+        <v>2.1039427890769637</v>
       </c>
       <c r="AJ45" s="58">
         <f t="shared" si="7"/>
-        <v>134.34699999999998</v>
+        <v>266.83399999999995</v>
       </c>
       <c r="AK45" s="57">
         <f t="shared" si="8"/>
@@ -84699,15 +84715,15 @@
       </c>
       <c r="AL45" s="57">
         <f t="shared" si="26"/>
-        <v>31.723440047042363</v>
+        <v>15.972286140446871</v>
       </c>
       <c r="AM45" s="52">
         <f t="shared" si="27"/>
-        <v>-0.72920906858596057</v>
+        <v>4.6782738259622159</v>
       </c>
       <c r="AN45" s="58">
         <f t="shared" si="9"/>
-        <v>173.6172</v>
+        <v>306.10419999999993</v>
       </c>
       <c r="AO45" s="57">
         <f t="shared" si="10"/>
@@ -84715,15 +84731,15 @@
       </c>
       <c r="AP45" s="57">
         <f t="shared" si="28"/>
-        <v>20.125874049345338</v>
+        <v>11.415060296461141</v>
       </c>
       <c r="AQ45" s="52">
         <f t="shared" si="29"/>
-        <v>-16.90015851975091</v>
+        <v>2.2011288647644252</v>
       </c>
       <c r="AR45" s="58">
         <f t="shared" si="11"/>
-        <v>157.14644999999999</v>
+        <v>289.63344999999998</v>
       </c>
       <c r="AS45" s="57">
         <f t="shared" si="12"/>
@@ -84731,15 +84747,15 @@
       </c>
       <c r="AT45" s="57">
         <f t="shared" si="30"/>
-        <v>26.704403758404979</v>
+        <v>14.489011024106503</v>
       </c>
       <c r="AU45" s="52">
         <f t="shared" si="31"/>
-        <v>-1.4423582040137866</v>
+        <v>3.4588962496695759</v>
       </c>
       <c r="AV45" s="58">
         <f t="shared" si="13"/>
-        <v>98.176999999999992</v>
+        <v>177.66919999999999</v>
       </c>
       <c r="AW45" s="57">
         <f t="shared" si="14"/>
@@ -84747,15 +84763,15 @@
       </c>
       <c r="AX45" s="57">
         <f t="shared" si="32"/>
-        <v>18.416174460413337</v>
+        <v>10.176467052252164</v>
       </c>
       <c r="AY45" s="52">
         <f t="shared" si="33"/>
-        <v>6.3865829651095307</v>
+        <v>1.1010625058376171</v>
       </c>
       <c r="AZ45" s="58">
         <f t="shared" si="15"/>
-        <v>76.21599999999998</v>
+        <v>155.70819999999998</v>
       </c>
       <c r="BA45" s="57">
         <f t="shared" si="16"/>
@@ -84763,31 +84779,31 @@
       </c>
       <c r="BB45" s="57">
         <f t="shared" si="34"/>
-        <v>36.008850635037277</v>
+        <v>17.625600706963414</v>
       </c>
       <c r="BC45" s="52">
         <f t="shared" si="35"/>
-        <v>-0.30668230771717309</v>
+        <v>5.708367157953214</v>
       </c>
       <c r="BD45" s="60">
         <f t="shared" si="36"/>
-        <v>6.3865829651095307</v>
+        <v>5.708367157953214</v>
       </c>
       <c r="BE45" s="53">
         <f t="shared" si="17"/>
-        <v>0.63865829651095307</v>
+        <v>0.57083671579532136</v>
       </c>
       <c r="BF45" s="58">
         <f t="shared" si="37"/>
-        <v>7.9832287063869138</v>
+        <v>10.275060884315785</v>
       </c>
       <c r="BG45" s="57">
         <f t="shared" si="38"/>
-        <v>0.16666666666666666</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="BH45" s="57">
         <f t="shared" si="39"/>
-        <v>4.7899372238321485</v>
+        <v>1.5412591326473677</v>
       </c>
       <c r="BI45" s="52" t="str">
         <f t="shared" si="40"/>
@@ -84795,15 +84811,15 @@
       </c>
       <c r="BJ45" s="58">
         <f t="shared" si="41"/>
-        <v>2.8739623342992342</v>
+        <v>0</v>
       </c>
       <c r="BK45" s="57">
         <f t="shared" si="42"/>
-        <v>0.16666666666666666</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="BL45" s="57">
         <f t="shared" si="43"/>
-        <v>1.7243774005795405</v>
+        <v>0</v>
       </c>
       <c r="BM45" s="52" t="str">
         <f t="shared" si="44"/>

</xml_diff>